<commit_message>
Latest measures. Adding PNW results.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -29,7 +29,7 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1410,10 +1410,10 @@
     <t>../weather/national/*.*</t>
   </si>
   <si>
-    <t>1.19.1-rc3</t>
-  </si>
-  <si>
     <t>integer_sequence</t>
+  </si>
+  <si>
+    <t>1.19.1-rc4</t>
   </si>
 </sst>
 </file>
@@ -5489,7 +5489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5548,7 +5550,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -6245,7 +6247,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>

</xml_diff>

<commit_message>
Added integrity checks back in as a rake task. Cleaned out all the other rake tasks that we don't use.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -29,7 +29,7 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1173,9 +1173,6 @@
     <t>BuildingCharacteristicsReport</t>
   </si>
   <si>
-    <t>run_baseline</t>
-  </si>
-  <si>
     <t>building_characteristics_report.Location Region</t>
   </si>
   <si>
@@ -1404,9 +1401,6 @@
     <t>ResStock_National</t>
   </si>
   <si>
-    <t>../results/national</t>
-  </si>
-  <si>
     <t>../weather/national/*.*</t>
   </si>
   <si>
@@ -1414,6 +1408,12 @@
   </si>
   <si>
     <t>1.19.1-rc4</t>
+  </si>
+  <si>
+    <t>../analysis_results/national</t>
+  </si>
+  <si>
+    <t>Run Baseline</t>
   </si>
 </sst>
 </file>
@@ -5489,9 +5489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5550,7 +5548,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5661,7 +5659,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5683,7 +5681,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5777,19 +5775,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>379</v>
+        <v>459</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5853,7 +5851,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6247,7 +6245,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6420,10 +6418,10 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
@@ -6458,10 +6456,10 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
@@ -6606,10 +6604,10 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
@@ -6644,10 +6642,10 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
@@ -6792,10 +6790,10 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
@@ -6830,10 +6828,10 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10" t="s">
@@ -6978,10 +6976,10 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
@@ -6989,7 +6987,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7016,10 +7014,10 @@
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10" t="s">
@@ -7027,7 +7025,7 @@
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -7336,7 +7334,7 @@
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7363,7 +7361,7 @@
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7390,7 +7388,7 @@
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7417,7 +7415,7 @@
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7444,7 +7442,7 @@
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7471,7 +7469,7 @@
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7498,7 +7496,7 @@
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
       <c r="D10" s="48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7525,7 +7523,7 @@
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7552,7 +7550,7 @@
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7579,7 +7577,7 @@
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7606,7 +7604,7 @@
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7633,7 +7631,7 @@
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7660,7 +7658,7 @@
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7685,7 +7683,7 @@
         <v>301</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>243</v>
@@ -7705,7 +7703,7 @@
         <v>302</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7727,7 +7725,7 @@
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48" t="s">
@@ -7754,7 +7752,7 @@
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7781,7 +7779,7 @@
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -7808,7 +7806,7 @@
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -7835,7 +7833,7 @@
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -7860,7 +7858,7 @@
         <v>307</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>243</v>
@@ -7880,7 +7878,7 @@
         <v>308</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -7900,7 +7898,7 @@
         <v>309</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -7920,7 +7918,7 @@
         <v>310</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -7940,7 +7938,7 @@
         <v>311</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -7960,7 +7958,7 @@
         <v>312</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -7980,7 +7978,7 @@
         <v>313</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -8000,7 +7998,7 @@
         <v>314</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -8020,7 +8018,7 @@
         <v>315</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -8040,7 +8038,7 @@
         <v>316</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -8060,7 +8058,7 @@
         <v>317</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -8080,7 +8078,7 @@
         <v>318</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8100,7 +8098,7 @@
         <v>319</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8120,7 +8118,7 @@
         <v>320</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8140,7 +8138,7 @@
         <v>321</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8160,7 +8158,7 @@
         <v>322</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8180,7 +8178,7 @@
         <v>323</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8200,7 +8198,7 @@
         <v>276</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8220,7 +8218,7 @@
         <v>324</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8240,7 +8238,7 @@
         <v>325</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8260,7 +8258,7 @@
         <v>326</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8280,7 +8278,7 @@
         <v>327</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8300,7 +8298,7 @@
         <v>328</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8320,7 +8318,7 @@
         <v>329</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8340,7 +8338,7 @@
         <v>330</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8360,7 +8358,7 @@
         <v>331</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8380,7 +8378,7 @@
         <v>332</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8400,7 +8398,7 @@
         <v>333</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8420,7 +8418,7 @@
         <v>334</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8440,7 +8438,7 @@
         <v>335</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8460,7 +8458,7 @@
         <v>336</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8480,7 +8478,7 @@
         <v>278</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8500,7 +8498,7 @@
         <v>337</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8520,7 +8518,7 @@
         <v>338</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8540,7 +8538,7 @@
         <v>339</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8560,7 +8558,7 @@
         <v>340</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8580,7 +8578,7 @@
         <v>341</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8600,7 +8598,7 @@
         <v>342</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8620,7 +8618,7 @@
         <v>343</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8640,7 +8638,7 @@
         <v>344</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8660,7 +8658,7 @@
         <v>345</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8680,7 +8678,7 @@
         <v>346</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8700,7 +8698,7 @@
         <v>347</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8720,7 +8718,7 @@
         <v>348</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8740,7 +8738,7 @@
         <v>349</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8760,7 +8758,7 @@
         <v>350</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8783,7 +8781,7 @@
         <v>354</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G70" s="14" t="b">
         <v>0</v>
@@ -8803,7 +8801,7 @@
         <v>355</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G71" s="14" t="b">
         <v>0</v>
@@ -8823,7 +8821,7 @@
         <v>356</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G72" s="14" t="b">
         <v>0</v>
@@ -8843,7 +8841,7 @@
         <v>357</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G73" s="14" t="b">
         <v>0</v>
@@ -8863,7 +8861,7 @@
         <v>358</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -8883,7 +8881,7 @@
         <v>359</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -8903,7 +8901,7 @@
         <v>360</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -8923,7 +8921,7 @@
         <v>361</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -8943,7 +8941,7 @@
         <v>362</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -8963,7 +8961,7 @@
         <v>363</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -8983,7 +8981,7 @@
         <v>364</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -9003,7 +9001,7 @@
         <v>365</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -9023,7 +9021,7 @@
         <v>366</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -9043,7 +9041,7 @@
         <v>367</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -9063,7 +9061,7 @@
         <v>368</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G84" s="14" t="b">
         <v>0</v>
@@ -9083,7 +9081,7 @@
         <v>369</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9103,7 +9101,7 @@
         <v>370</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9123,7 +9121,7 @@
         <v>371</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added hot water distribution measure. Latest measures.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="462">
   <si>
     <t>type</t>
   </si>
@@ -1414,6 +1414,12 @@
   </si>
   <si>
     <t>Run Baseline</t>
+  </si>
+  <si>
+    <t>Hot Water Distribution</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.Hot Water Distribution</t>
   </si>
 </sst>
 </file>
@@ -7209,7 +7215,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M126"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8255,10 +8261,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>326</v>
+        <v>460</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>419</v>
+        <v>461</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8275,10 +8281,10 @@
     </row>
     <row r="45" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8295,10 +8301,10 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8315,10 +8321,10 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8335,10 +8341,10 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8355,10 +8361,10 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8375,10 +8381,10 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8395,10 +8401,10 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8415,10 +8421,10 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8435,10 +8441,10 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8455,10 +8461,10 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8475,10 +8481,10 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>278</v>
+        <v>336</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8495,10 +8501,10 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>337</v>
+        <v>278</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8515,10 +8521,10 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8535,10 +8541,10 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8555,10 +8561,10 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8575,10 +8581,10 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8595,10 +8601,10 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8615,10 +8621,10 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8635,10 +8641,10 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8655,10 +8661,10 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8675,10 +8681,10 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8695,10 +8701,10 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8715,10 +8721,10 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8735,10 +8741,10 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8755,10 +8761,10 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8773,32 +8779,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
-        <v>244</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="F70" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="G70" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I70" s="14" t="b">
+    <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="D70" s="48" t="s">
+        <v>444</v>
+      </c>
+      <c r="F70" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G70" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>445</v>
@@ -8815,10 +8821,10 @@
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>445</v>
@@ -8835,10 +8841,10 @@
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>445</v>
@@ -8855,10 +8861,10 @@
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>445</v>
@@ -8875,10 +8881,10 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>445</v>
@@ -8895,10 +8901,10 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>445</v>
@@ -8915,10 +8921,10 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>445</v>
@@ -8935,10 +8941,10 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>445</v>
@@ -8955,10 +8961,10 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>445</v>
@@ -8975,10 +8981,10 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>445</v>
@@ -8995,10 +9001,10 @@
     </row>
     <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F81" s="14" t="s">
         <v>445</v>
@@ -9014,11 +9020,11 @@
       </c>
     </row>
     <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>256</v>
+      <c r="A82" s="49" t="s">
+        <v>255</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F82" s="14" t="s">
         <v>445</v>
@@ -9035,10 +9041,10 @@
     </row>
     <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F83" s="14" t="s">
         <v>445</v>
@@ -9055,10 +9061,10 @@
     </row>
     <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F84" s="14" t="s">
         <v>445</v>
@@ -9075,10 +9081,10 @@
     </row>
     <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F85" s="14" t="s">
         <v>445</v>
@@ -9095,10 +9101,10 @@
     </row>
     <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F86" s="14" t="s">
         <v>445</v>
@@ -9115,10 +9121,10 @@
     </row>
     <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F87" s="14" t="s">
         <v>445</v>
@@ -9133,20 +9139,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="B88" s="15"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="15"/>
-      <c r="H88" s="15"/>
-      <c r="I88" s="15"/>
-      <c r="J88" s="15"/>
-      <c r="K88" s="15"/>
-      <c r="L88" s="15"/>
-      <c r="M88" s="15"/>
+    <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G88" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15"/>
@@ -9165,12 +9176,18 @@
     </row>
     <row r="90" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15"/>
-      <c r="B90" s="21"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="15"/>
       <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
       <c r="H90" s="15"/>
       <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="15"/>
     </row>
     <row r="91" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15"/>
@@ -9442,12 +9459,10 @@
       <c r="H120" s="15"/>
       <c r="I120" s="15"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
       <c r="B121" s="21"/>
-      <c r="C121" s="22"/>
       <c r="D121" s="15"/>
-      <c r="E121" s="22"/>
       <c r="F121" s="15"/>
       <c r="G121" s="15"/>
       <c r="H121" s="15"/>
@@ -9507,6 +9522,17 @@
       <c r="G126" s="15"/>
       <c r="H126" s="15"/>
       <c r="I126" s="15"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="15"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="22"/>
+      <c r="D127" s="15"/>
+      <c r="E127" s="22"/>
+      <c r="F127" s="15"/>
+      <c r="G127" s="15"/>
+      <c r="H127" s="15"/>
+      <c r="I127" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Simplified simulation output reporting measure. Fixed reporting of oil/propane energy consumption. Added hours heating/cooling setpoints not met to output.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="466">
   <si>
     <t>type</t>
   </si>
@@ -1410,9 +1410,6 @@
     <t>1.19.1-rc4</t>
   </si>
   <si>
-    <t>../analysis_results/national</t>
-  </si>
-  <si>
     <t>Run Baseline</t>
   </si>
   <si>
@@ -1420,6 +1417,21 @@
   </si>
   <si>
     <t>building_characteristics_report.Hot Water Distribution</t>
+  </si>
+  <si>
+    <t>../analysis_results</t>
+  </si>
+  <si>
+    <t>Hours Heating Setpoint Not Met</t>
+  </si>
+  <si>
+    <t>simulation_output_report.Hours Heating Setpoint Not Met</t>
+  </si>
+  <si>
+    <t>Hours Cooling Setpoint Not Met</t>
+  </si>
+  <si>
+    <t>simulation_output_report.Hours Cooling Setpoint Not Met</t>
   </si>
 </sst>
 </file>
@@ -5687,7 +5699,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5787,7 +5799,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
@@ -7215,7 +7227,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8261,10 +8273,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
+        <v>459</v>
+      </c>
+      <c r="D44" s="48" t="s">
         <v>460</v>
-      </c>
-      <c r="D44" s="48" t="s">
-        <v>461</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -9159,31 +9171,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
-      <c r="B89" s="15"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
-      <c r="F89" s="15"/>
-      <c r="G89" s="15"/>
-      <c r="H89" s="15"/>
-      <c r="I89" s="15"/>
+    <row r="89" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G89" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I89" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="J89" s="15"/>
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15"/>
     </row>
-    <row r="90" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="15"/>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="15"/>
-      <c r="H90" s="15"/>
-      <c r="I90" s="15"/>
+    <row r="90" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="J90" s="15"/>
       <c r="K90" s="15"/>
       <c r="L90" s="15"/>
@@ -9191,21 +9227,33 @@
     </row>
     <row r="91" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15"/>
-      <c r="B91" s="21"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15"/>
       <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15"/>
       <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="15"/>
     </row>
     <row r="92" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
-      <c r="B92" s="21"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
       <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
       <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
     </row>
     <row r="93" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
@@ -9468,23 +9516,19 @@
       <c r="H121" s="15"/>
       <c r="I121" s="15"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122" s="21"/>
-      <c r="C122" s="22"/>
       <c r="D122" s="15"/>
-      <c r="E122" s="22"/>
       <c r="F122" s="15"/>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123" s="21"/>
-      <c r="C123" s="22"/>
       <c r="D123" s="15"/>
-      <c r="E123" s="22"/>
       <c r="F123" s="15"/>
       <c r="G123" s="15"/>
       <c r="H123" s="15"/>
@@ -9533,6 +9577,28 @@
       <c r="G127" s="15"/>
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="15"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="22"/>
+      <c r="D128" s="15"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="15"/>
+      <c r="H128" s="15"/>
+      <c r="I128" s="15"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="15"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="22"/>
+      <c r="D129" s="15"/>
+      <c r="E129" s="22"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
+      <c r="I129" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Latest measures. Improve handling/reporting of child measure errors in run_measure().
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="468">
   <si>
     <t>type</t>
   </si>
@@ -1407,9 +1407,6 @@
     <t>integer_sequence</t>
   </si>
   <si>
-    <t>1.19.1-rc4</t>
-  </si>
-  <si>
     <t>Run Baseline</t>
   </si>
   <si>
@@ -1432,6 +1429,15 @@
   </si>
   <si>
     <t>simulation_output_report.Hours Cooling Setpoint Not Met</t>
+  </si>
+  <si>
+    <t>1.19.1-rc5</t>
+  </si>
+  <si>
+    <t>Occupants</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.Occupants</t>
   </si>
 </sst>
 </file>
@@ -5566,7 +5572,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5699,7 +5705,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5799,7 +5805,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
@@ -6359,7 +6365,7 @@
     </row>
     <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="39" t="s">
         <v>271</v>
@@ -6545,7 +6551,7 @@
     </row>
     <row r="13" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" s="39" t="s">
         <v>281</v>
@@ -6731,7 +6737,7 @@
     </row>
     <row r="18" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>282</v>
@@ -6917,7 +6923,7 @@
     </row>
     <row r="23" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>280</v>
@@ -7227,7 +7233,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M129"/>
+  <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -7617,12 +7623,12 @@
     </row>
     <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>298</v>
+        <v>466</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>389</v>
+        <v>467</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7644,12 +7650,12 @@
     </row>
     <row r="15" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7671,12 +7677,12 @@
     </row>
     <row r="16" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7698,11 +7704,14 @@
     </row>
     <row r="17" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>301</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="48" t="s">
-        <v>392</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="E17" s="48"/>
       <c r="F17" s="48" t="s">
         <v>243</v>
       </c>
@@ -7715,13 +7724,17 @@
       <c r="I17" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
     </row>
     <row r="18" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7738,14 +7751,11 @@
     </row>
     <row r="19" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>303</v>
-      </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
+        <v>302</v>
+      </c>
       <c r="D19" s="48" t="s">
-        <v>394</v>
-      </c>
-      <c r="E19" s="48"/>
+        <v>393</v>
+      </c>
       <c r="F19" s="48" t="s">
         <v>243</v>
       </c>
@@ -7758,19 +7768,15 @@
       <c r="I19" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
     </row>
     <row r="20" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7792,12 +7798,12 @@
     </row>
     <row r="21" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -7819,12 +7825,12 @@
     </row>
     <row r="22" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -7846,12 +7852,12 @@
     </row>
     <row r="23" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -7873,11 +7879,14 @@
     </row>
     <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
-        <v>307</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="48" t="s">
-        <v>399</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="E24" s="48"/>
       <c r="F24" s="48" t="s">
         <v>243</v>
       </c>
@@ -7890,13 +7899,17 @@
       <c r="I24" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
     </row>
     <row r="25" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -7913,10 +7926,10 @@
     </row>
     <row r="26" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -7933,10 +7946,10 @@
     </row>
     <row r="27" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -7953,10 +7966,10 @@
     </row>
     <row r="28" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -7973,10 +7986,10 @@
     </row>
     <row r="29" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -7993,10 +8006,10 @@
     </row>
     <row r="30" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -8013,10 +8026,10 @@
     </row>
     <row r="31" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -8033,10 +8046,10 @@
     </row>
     <row r="32" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -8053,10 +8066,10 @@
     </row>
     <row r="33" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -8073,10 +8086,10 @@
     </row>
     <row r="34" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -8093,10 +8106,10 @@
     </row>
     <row r="35" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8113,10 +8126,10 @@
     </row>
     <row r="36" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8133,10 +8146,10 @@
     </row>
     <row r="37" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8153,10 +8166,10 @@
     </row>
     <row r="38" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8173,10 +8186,10 @@
     </row>
     <row r="39" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8193,10 +8206,10 @@
     </row>
     <row r="40" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8213,10 +8226,10 @@
     </row>
     <row r="41" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>276</v>
+        <v>323</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8233,10 +8246,10 @@
     </row>
     <row r="42" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8253,10 +8266,10 @@
     </row>
     <row r="43" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8273,10 +8286,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>459</v>
+        <v>325</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>460</v>
+        <v>418</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8293,10 +8306,10 @@
     </row>
     <row r="45" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>326</v>
+        <v>458</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>419</v>
+        <v>459</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8313,10 +8326,10 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8333,10 +8346,10 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8353,10 +8366,10 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8373,10 +8386,10 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8393,10 +8406,10 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8413,10 +8426,10 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8433,10 +8446,10 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8453,10 +8466,10 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8473,10 +8486,10 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8493,10 +8506,10 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8513,10 +8526,10 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>278</v>
+        <v>336</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8533,10 +8546,10 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>337</v>
+        <v>278</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8553,10 +8566,10 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8573,10 +8586,10 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8593,10 +8606,10 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8613,10 +8626,10 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8633,10 +8646,10 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8653,10 +8666,10 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8673,10 +8686,10 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8693,10 +8706,10 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8713,10 +8726,10 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8733,10 +8746,10 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8753,10 +8766,10 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8773,10 +8786,10 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8793,10 +8806,10 @@
     </row>
     <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D70" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>243</v>
@@ -8811,32 +8824,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
-        <v>244</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="G71" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I71" s="14" t="b">
+    <row r="71" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="D71" s="48" t="s">
+        <v>444</v>
+      </c>
+      <c r="F71" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>445</v>
@@ -8853,10 +8866,10 @@
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>445</v>
@@ -8873,10 +8886,10 @@
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>445</v>
@@ -8893,10 +8906,10 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>445</v>
@@ -8913,10 +8926,10 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>445</v>
@@ -8933,10 +8946,10 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>445</v>
@@ -8953,10 +8966,10 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>445</v>
@@ -8973,10 +8986,10 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>445</v>
@@ -8993,10 +9006,10 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>445</v>
@@ -9013,10 +9026,10 @@
     </row>
     <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F81" s="14" t="s">
         <v>445</v>
@@ -9033,10 +9046,10 @@
     </row>
     <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F82" s="14" t="s">
         <v>445</v>
@@ -9052,11 +9065,11 @@
       </c>
     </row>
     <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>256</v>
+      <c r="A83" s="49" t="s">
+        <v>255</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F83" s="14" t="s">
         <v>445</v>
@@ -9073,10 +9086,10 @@
     </row>
     <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F84" s="14" t="s">
         <v>445</v>
@@ -9093,10 +9106,10 @@
     </row>
     <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F85" s="14" t="s">
         <v>445</v>
@@ -9113,10 +9126,10 @@
     </row>
     <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F86" s="14" t="s">
         <v>445</v>
@@ -9133,10 +9146,10 @@
     </row>
     <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F87" s="14" t="s">
         <v>445</v>
@@ -9153,10 +9166,10 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>445</v>
@@ -9171,16 +9184,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
+        <v>261</v>
+      </c>
       <c r="D89" s="14" t="s">
-        <v>463</v>
-      </c>
-      <c r="E89" s="14"/>
+        <v>371</v>
+      </c>
       <c r="F89" s="14" t="s">
         <v>445</v>
       </c>
@@ -9193,19 +9203,15 @@
       <c r="I89" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J89" s="15"/>
-      <c r="K89" s="15"/>
-      <c r="L89" s="15"/>
-      <c r="M89" s="15"/>
     </row>
     <row r="90" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
       <c r="D90" s="14" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E90" s="14"/>
       <c r="F90" s="14" t="s">
@@ -9225,16 +9231,28 @@
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
     </row>
-    <row r="91" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-      <c r="B91" s="15"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="15"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="15"/>
-      <c r="H91" s="15"/>
-      <c r="I91" s="15"/>
+    <row r="91" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G91" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="J91" s="15"/>
       <c r="K91" s="15"/>
       <c r="L91" s="15"/>
@@ -9257,12 +9275,18 @@
     </row>
     <row r="93" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
-      <c r="B93" s="21"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="15"/>
       <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
       <c r="H93" s="15"/>
       <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
     </row>
     <row r="94" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
@@ -9534,12 +9558,10 @@
       <c r="H123" s="15"/>
       <c r="I123" s="15"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124" s="21"/>
-      <c r="C124" s="22"/>
       <c r="D124" s="15"/>
-      <c r="E124" s="22"/>
       <c r="F124" s="15"/>
       <c r="G124" s="15"/>
       <c r="H124" s="15"/>
@@ -9599,6 +9621,17 @@
       <c r="G129" s="15"/>
       <c r="H129" s="15"/>
       <c r="I129" s="15"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="15"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="22"/>
+      <c r="D130" s="15"/>
+      <c r="E130" s="22"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated to OS 1.12.5/E+ 8.6.
Added HVAC capacities to output results.

Latest measures.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="472">
   <si>
     <t>type</t>
   </si>
@@ -1431,13 +1431,25 @@
     <t>simulation_output_report.Hours Cooling Setpoint Not Met</t>
   </si>
   <si>
-    <t>1.19.1-rc5</t>
-  </si>
-  <si>
     <t>Occupants</t>
   </si>
   <si>
     <t>building_characteristics_report.Occupants</t>
+  </si>
+  <si>
+    <t>1.19.1-OS.1.12.5.de88f6a99d</t>
+  </si>
+  <si>
+    <t>HVAC Cooling Capacity W</t>
+  </si>
+  <si>
+    <t>simulation_output_report.HVAC Cooling Capacity W</t>
+  </si>
+  <si>
+    <t>HVAC Heating Capacity W</t>
+  </si>
+  <si>
+    <t>simulation_output_report.HVAC Heating Capacity W</t>
   </si>
 </sst>
 </file>
@@ -5572,7 +5584,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -7623,12 +7635,12 @@
     </row>
     <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -9204,16 +9216,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
       <c r="D90" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="E90" s="14"/>
       <c r="F90" s="14" t="s">
         <v>445</v>
       </c>
@@ -9226,21 +9235,18 @@
       <c r="I90" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J90" s="15"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="15"/>
-      <c r="M90" s="15"/>
-    </row>
-    <row r="91" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="49"/>
+      <c r="K90" s="49"/>
+      <c r="L90" s="49"/>
+      <c r="M90" s="49"/>
+    </row>
+    <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
       <c r="D91" s="14" t="s">
         <v>464</v>
       </c>
-      <c r="E91" s="14"/>
       <c r="F91" s="14" t="s">
         <v>445</v>
       </c>
@@ -9253,40 +9259,50 @@
       <c r="I91" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J91" s="15"/>
-      <c r="K91" s="15"/>
-      <c r="L91" s="15"/>
-      <c r="M91" s="15"/>
-    </row>
-    <row r="92" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15"/>
-      <c r="B92" s="15"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="15"/>
-      <c r="E92" s="15"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="15"/>
-      <c r="H92" s="15"/>
-      <c r="I92" s="15"/>
-      <c r="J92" s="15"/>
-      <c r="K92" s="15"/>
-      <c r="L92" s="15"/>
-      <c r="M92" s="15"/>
-    </row>
-    <row r="93" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
-      <c r="I93" s="15"/>
-      <c r="J93" s="15"/>
-      <c r="K93" s="15"/>
-      <c r="L93" s="15"/>
-      <c r="M93" s="15"/>
+      <c r="J91" s="49"/>
+      <c r="K91" s="49"/>
+      <c r="L91" s="49"/>
+      <c r="M91" s="49"/>
+    </row>
+    <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="49" t="s">
+        <v>468</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G92" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="49" t="s">
+        <v>470</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>

</xml_diff>

<commit_message>
Latest measures. Update to OS 1.13.1.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -1437,9 +1437,6 @@
     <t>building_characteristics_report.Occupants</t>
   </si>
   <si>
-    <t>1.19.1-OS.1.12.5.de88f6a99d</t>
-  </si>
-  <si>
     <t>HVAC Cooling Capacity W</t>
   </si>
   <si>
@@ -1450,6 +1447,9 @@
   </si>
   <si>
     <t>simulation_output_report.HVAC Heating Capacity W</t>
+  </si>
+  <si>
+    <t>1.20.0-rc2</t>
   </si>
 </sst>
 </file>
@@ -5525,7 +5525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5584,7 +5586,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -9266,10 +9268,10 @@
     </row>
     <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="49" t="s">
+        <v>467</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>468</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>469</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>445</v>
@@ -9286,10 +9288,10 @@
     </row>
     <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="49" t="s">
+        <v>469</v>
+      </c>
+      <c r="D93" s="14" t="s">
         <v>470</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>471</v>
       </c>
       <c r="F93" s="14" t="s">
         <v>445</v>

</xml_diff>

<commit_message>
Replaced Airflow EnergyPlus measure with OpenStudio measure.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="467">
   <si>
     <t>type</t>
   </si>
@@ -1150,21 +1150,6 @@
   </si>
   <si>
     <t>simulation_output_report.Other Fuel Water Systems MBtu</t>
-  </si>
-  <si>
-    <t>Build Existing Models EnergyPlus</t>
-  </si>
-  <si>
-    <t>BuildExistingModelEnergyPlus</t>
-  </si>
-  <si>
-    <t>Always Run</t>
-  </si>
-  <si>
-    <t>always_run</t>
-  </si>
-  <si>
-    <t>EnergyPlusMeasure</t>
   </si>
   <si>
     <t>Building Characteristics Report</t>
@@ -5525,9 +5510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5586,7 +5569,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5697,7 +5680,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5719,7 +5702,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5813,19 +5796,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5889,7 +5872,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6030,9 +6013,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6283,7 +6266,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6294,19 +6277,19 @@
     </row>
     <row r="6" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>372</v>
+        <v>271</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>373</v>
+        <v>268</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>373</v>
+        <v>268</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>376</v>
+        <v>40</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6328,29 +6311,25 @@
       <c r="W6" s="39"/>
       <c r="X6" s="39"/>
     </row>
-    <row r="7" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>264</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45" t="s">
-        <v>374</v>
+        <v>240</v>
+      </c>
+      <c r="D7" s="45" t="str">
+        <f>"Run " &amp; B6</f>
+        <v>Run R60 Attic Insulation Upgrade</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>375</v>
-      </c>
-      <c r="F7" s="45"/>
+        <v>265</v>
+      </c>
       <c r="G7" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="H7" s="45"/>
       <c r="I7" s="45">
         <v>1</v>
       </c>
-      <c r="J7" s="45"/>
       <c r="K7" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="45">
         <v>1</v>
@@ -6361,93 +6340,88 @@
       <c r="N7" s="45">
         <v>1</v>
       </c>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45" t="str">
-        <f>"[1]"</f>
-        <v>[1]</v>
-      </c>
-      <c r="Q7" s="45"/>
+      <c r="P7" s="45" t="s">
+        <v>267</v>
+      </c>
       <c r="R7" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-    </row>
-    <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-    </row>
-    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D9" s="45" t="str">
-        <f>"Run " &amp; B8</f>
-        <v>Run R60 Attic Insulation Upgrade</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="I9" s="45">
-        <v>1</v>
-      </c>
-      <c r="K9" s="45">
-        <v>0</v>
-      </c>
-      <c r="L9" s="45">
-        <v>1</v>
-      </c>
-      <c r="M9" s="45">
-        <v>1</v>
-      </c>
-      <c r="N9" s="45">
-        <v>1</v>
-      </c>
-      <c r="P9" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="R9" s="45" t="s">
-        <v>275</v>
-      </c>
+    </row>
+    <row r="8" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -6456,10 +6430,10 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>452</v>
+        <v>272</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>450</v>
+        <v>273</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
@@ -6467,7 +6441,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6487,153 +6461,153 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="39"/>
+    </row>
+    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="45" t="str">
+        <f>"Run " &amp; B11</f>
+        <v>Run Triple-Pane Windows Upgrade</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I12" s="45">
+        <v>1</v>
+      </c>
+      <c r="K12" s="45">
+        <v>0</v>
+      </c>
+      <c r="L12" s="45">
+        <v>1</v>
+      </c>
+      <c r="M12" s="45">
+        <v>1</v>
+      </c>
+      <c r="N12" s="45">
+        <v>1</v>
+      </c>
+      <c r="P12" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="R12" s="45" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+    </row>
+    <row r="14" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="39"/>
-    </row>
-    <row r="14" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D14" s="45" t="str">
-        <f>"Run " &amp; B13</f>
-        <v>Run Triple-Pane Windows Upgrade</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="G14" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="I14" s="45">
-        <v>1</v>
-      </c>
-      <c r="K14" s="45">
-        <v>0</v>
-      </c>
-      <c r="L14" s="45">
-        <v>1</v>
-      </c>
-      <c r="M14" s="45">
-        <v>1</v>
-      </c>
-      <c r="N14" s="45">
-        <v>1</v>
-      </c>
-      <c r="P14" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="R14" s="45" t="s">
-        <v>275</v>
-      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
     </row>
     <row r="15" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
@@ -6642,10 +6616,10 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>452</v>
+        <v>272</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>450</v>
+        <v>273</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
@@ -6653,7 +6627,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6673,153 +6647,153 @@
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10" t="s">
+    <row r="16" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+    </row>
+    <row r="17" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" s="45" t="str">
+        <f>"Run " &amp; B16</f>
+        <v>Run LED Lighting Upgrade</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I17" s="45">
+        <v>1</v>
+      </c>
+      <c r="K17" s="45">
+        <v>0</v>
+      </c>
+      <c r="L17" s="45">
+        <v>1</v>
+      </c>
+      <c r="M17" s="45">
+        <v>1</v>
+      </c>
+      <c r="N17" s="45">
+        <v>1</v>
+      </c>
+      <c r="P17" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="R17" s="45" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-    </row>
-    <row r="17" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10" t="s">
+      <c r="H18" s="10"/>
+      <c r="I18" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+    </row>
+    <row r="19" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-    </row>
-    <row r="18" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-      <c r="T18" s="39"/>
-      <c r="U18" s="39"/>
-      <c r="V18" s="39"/>
-      <c r="W18" s="39"/>
-      <c r="X18" s="39"/>
-    </row>
-    <row r="19" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D19" s="45" t="str">
-        <f>"Run " &amp; B18</f>
-        <v>Run LED Lighting Upgrade</v>
-      </c>
-      <c r="E19" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="I19" s="45">
-        <v>1</v>
-      </c>
-      <c r="K19" s="45">
-        <v>0</v>
-      </c>
-      <c r="L19" s="45">
-        <v>1</v>
-      </c>
-      <c r="M19" s="45">
-        <v>1</v>
-      </c>
-      <c r="N19" s="45">
-        <v>1</v>
-      </c>
-      <c r="P19" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="R19" s="45" t="s">
-        <v>275</v>
-      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
@@ -6828,10 +6802,10 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>452</v>
+        <v>272</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>450</v>
+        <v>273</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
@@ -6839,7 +6813,7 @@
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -6859,153 +6833,153 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10" t="s">
+    <row r="21" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+    </row>
+    <row r="22" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D22" s="45" t="str">
+        <f>"Run " &amp; B21</f>
+        <v>Run Attic+Windows+Lighting Package</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I22" s="45">
+        <v>1</v>
+      </c>
+      <c r="K22" s="45">
+        <v>0</v>
+      </c>
+      <c r="L22" s="45">
+        <v>1</v>
+      </c>
+      <c r="M22" s="45">
+        <v>1</v>
+      </c>
+      <c r="N22" s="45">
+        <v>1</v>
+      </c>
+      <c r="P22" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="R22" s="45" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="10"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-    </row>
-    <row r="22" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+    </row>
+    <row r="24" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-    </row>
-    <row r="23" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="39"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
-      <c r="X23" s="39"/>
-    </row>
-    <row r="24" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D24" s="45" t="str">
-        <f>"Run " &amp; B23</f>
-        <v>Run Attic+Windows+Lighting Package</v>
-      </c>
-      <c r="E24" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="I24" s="45">
-        <v>1</v>
-      </c>
-      <c r="K24" s="45">
-        <v>0</v>
-      </c>
-      <c r="L24" s="45">
-        <v>1</v>
-      </c>
-      <c r="M24" s="45">
-        <v>1</v>
-      </c>
-      <c r="N24" s="45">
-        <v>1</v>
-      </c>
-      <c r="P24" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="R24" s="45" t="s">
-        <v>275</v>
-      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
     </row>
     <row r="25" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
@@ -7014,10 +6988,10 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>452</v>
+        <v>272</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>450</v>
+        <v>273</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
@@ -7025,7 +6999,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>448</v>
+        <v>274</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7045,94 +7019,90 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
-    </row>
-    <row r="27" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
+    <row r="26" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>372</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="40"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="40"/>
+      <c r="X26" s="40"/>
+    </row>
+    <row r="27" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="40"/>
+      <c r="W27" s="40"/>
+      <c r="X27" s="40"/>
     </row>
     <row r="28" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="b">
         <v>1</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>377</v>
+        <v>238</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>378</v>
+        <v>237</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>378</v>
+        <v>237</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>236</v>
@@ -7157,83 +7127,11 @@
       <c r="W28" s="40"/>
       <c r="X28" s="40"/>
     </row>
-    <row r="29" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>352</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>353</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>353</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="40"/>
-      <c r="S29" s="40"/>
-      <c r="T29" s="40"/>
-      <c r="U29" s="40"/>
-      <c r="V29" s="40"/>
-      <c r="W29" s="40"/>
-      <c r="X29" s="40"/>
-    </row>
-    <row r="30" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="D30" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="40"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="40"/>
-      <c r="U30" s="40"/>
-      <c r="V30" s="40"/>
-      <c r="W30" s="40"/>
-      <c r="X30" s="40"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B31" s="50"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B32" s="50"/>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -7372,7 +7270,7 @@
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7399,7 +7297,7 @@
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7426,7 +7324,7 @@
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7453,7 +7351,7 @@
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7480,7 +7378,7 @@
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7507,7 +7405,7 @@
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7534,7 +7432,7 @@
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
       <c r="D10" s="48" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7561,7 +7459,7 @@
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7588,7 +7486,7 @@
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7615,7 +7513,7 @@
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7637,12 +7535,12 @@
     </row>
     <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7669,7 +7567,7 @@
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7696,7 +7594,7 @@
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7723,7 +7621,7 @@
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
       <c r="D17" s="48" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="48" t="s">
@@ -7748,7 +7646,7 @@
         <v>301</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7768,7 +7666,7 @@
         <v>302</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F19" s="48" t="s">
         <v>243</v>
@@ -7790,7 +7688,7 @@
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7817,7 +7715,7 @@
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -7844,7 +7742,7 @@
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -7871,7 +7769,7 @@
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -7898,7 +7796,7 @@
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="48" t="s">
@@ -7923,7 +7821,7 @@
         <v>307</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -7943,7 +7841,7 @@
         <v>308</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -7963,7 +7861,7 @@
         <v>309</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -7983,7 +7881,7 @@
         <v>310</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -8003,7 +7901,7 @@
         <v>311</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -8023,7 +7921,7 @@
         <v>312</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -8043,7 +7941,7 @@
         <v>313</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -8063,7 +7961,7 @@
         <v>314</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -8083,7 +7981,7 @@
         <v>315</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -8103,7 +8001,7 @@
         <v>316</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -8123,7 +8021,7 @@
         <v>317</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8143,7 +8041,7 @@
         <v>318</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8163,7 +8061,7 @@
         <v>319</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8183,7 +8081,7 @@
         <v>320</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8203,7 +8101,7 @@
         <v>321</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8223,7 +8121,7 @@
         <v>322</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8243,7 +8141,7 @@
         <v>323</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8263,7 +8161,7 @@
         <v>276</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8283,7 +8181,7 @@
         <v>324</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8303,7 +8201,7 @@
         <v>325</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8320,10 +8218,10 @@
     </row>
     <row r="45" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8343,7 +8241,7 @@
         <v>326</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8363,7 +8261,7 @@
         <v>327</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8383,7 +8281,7 @@
         <v>328</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8403,7 +8301,7 @@
         <v>329</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8423,7 +8321,7 @@
         <v>330</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8443,7 +8341,7 @@
         <v>331</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8463,7 +8361,7 @@
         <v>332</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8483,7 +8381,7 @@
         <v>333</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8503,7 +8401,7 @@
         <v>334</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8523,7 +8421,7 @@
         <v>335</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8543,7 +8441,7 @@
         <v>336</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8563,7 +8461,7 @@
         <v>278</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8583,7 +8481,7 @@
         <v>337</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8603,7 +8501,7 @@
         <v>338</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8623,7 +8521,7 @@
         <v>339</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8643,7 +8541,7 @@
         <v>340</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8663,7 +8561,7 @@
         <v>341</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8683,7 +8581,7 @@
         <v>342</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8703,7 +8601,7 @@
         <v>343</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8723,7 +8621,7 @@
         <v>344</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8743,7 +8641,7 @@
         <v>345</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8763,7 +8661,7 @@
         <v>346</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8783,7 +8681,7 @@
         <v>347</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8803,7 +8701,7 @@
         <v>348</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8823,7 +8721,7 @@
         <v>349</v>
       </c>
       <c r="D70" s="48" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>243</v>
@@ -8843,7 +8741,7 @@
         <v>350</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>243</v>
@@ -8866,7 +8764,7 @@
         <v>354</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G72" s="14" t="b">
         <v>0</v>
@@ -8886,7 +8784,7 @@
         <v>355</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G73" s="14" t="b">
         <v>0</v>
@@ -8906,7 +8804,7 @@
         <v>356</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -8926,7 +8824,7 @@
         <v>357</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -8946,7 +8844,7 @@
         <v>358</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -8966,7 +8864,7 @@
         <v>359</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -8986,7 +8884,7 @@
         <v>360</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -9006,7 +8904,7 @@
         <v>361</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -9026,7 +8924,7 @@
         <v>362</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -9046,7 +8944,7 @@
         <v>363</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -9066,7 +8964,7 @@
         <v>364</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -9086,7 +8984,7 @@
         <v>365</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -9106,7 +9004,7 @@
         <v>366</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G84" s="14" t="b">
         <v>0</v>
@@ -9126,7 +9024,7 @@
         <v>367</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9146,7 +9044,7 @@
         <v>368</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9166,7 +9064,7 @@
         <v>369</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>
@@ -9186,7 +9084,7 @@
         <v>370</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G88" s="14" t="b">
         <v>0</v>
@@ -9206,7 +9104,7 @@
         <v>371</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G89" s="14" t="b">
         <v>0</v>
@@ -9220,13 +9118,13 @@
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G90" s="14" t="b">
         <v>0</v>
@@ -9244,13 +9142,13 @@
     </row>
     <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G91" s="14" t="b">
         <v>0</v>
@@ -9268,13 +9166,13 @@
     </row>
     <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="49" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G92" s="14" t="b">
         <v>0</v>
@@ -9288,13 +9186,13 @@
     </row>
     <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="49" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G93" s="14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update to OpenStudio 1.13.2.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -1434,7 +1434,7 @@
     <t>simulation_output_report.HVAC Heating Capacity W</t>
   </si>
   <si>
-    <t>1.20.0-rc2</t>
+    <t>1.20.1</t>
   </si>
 </sst>
 </file>
@@ -5510,7 +5510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6015,7 +6017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Added ability to apply upgrades based on existing building options. Addresses #37.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Outputs" sheetId="12" r:id="rId3"/>
     <sheet name="Lookups" sheetId="11" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outputs!$A$2:$H$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$3</definedName>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="465">
   <si>
     <t>type</t>
   </si>
@@ -846,42 +849,18 @@
     <t>Insulation Unfinished Attic</t>
   </si>
   <si>
-    <t>Ceiling R-60, Vented</t>
-  </si>
-  <si>
-    <t>R60 Attic Insulation Upgrade</t>
-  </si>
-  <si>
-    <t>Apply Logic</t>
-  </si>
-  <si>
-    <t>apply_logic</t>
-  </si>
-  <si>
-    <t>FIXME</t>
-  </si>
-  <si>
     <t>discrete</t>
   </si>
   <si>
     <t>Windows</t>
   </si>
   <si>
-    <t>Low-E, Triple, Non-metal, Air, L-Gain</t>
-  </si>
-  <si>
     <t>Lighting</t>
   </si>
   <si>
-    <t>100% LED</t>
-  </si>
-  <si>
     <t>Attic+Windows+Lighting Package</t>
   </si>
   <si>
-    <t>Triple-Pane Windows Upgrade</t>
-  </si>
-  <si>
     <t>LED Lighting Upgrade</t>
   </si>
   <si>
@@ -1083,9 +1062,6 @@
     <t>Mechanical Ventilation</t>
   </si>
   <si>
-    <t>building_id</t>
-  </si>
-  <si>
     <t>Simulation Output Report</t>
   </si>
   <si>
@@ -1353,24 +1329,6 @@
     <t>0 or 1 (defines whether to run upgrade and existing building simulations, or only upgrade simulations)</t>
   </si>
   <si>
-    <t>Insulation Unfinished Attic|Windows|Lighting</t>
-  </si>
-  <si>
-    <t>Ceiling R-60, Vented|Low-E, Triple, Non-metal, Air, L-Gain|100% LED</t>
-  </si>
-  <si>
-    <t>parameter_names</t>
-  </si>
-  <si>
-    <t>option_names</t>
-  </si>
-  <si>
-    <t>Parameter Names</t>
-  </si>
-  <si>
-    <t>Option Names</t>
-  </si>
-  <si>
     <t>ResStock_National</t>
   </si>
   <si>
@@ -1423,6 +1381,57 @@
   </si>
   <si>
     <t>1.20.1</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Attic|Ceiling R-60, Vented</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Windows|Low-E, Triple, Non-metal, Air, L-Gain</t>
+  </si>
+  <si>
+    <t>Lighting|100% LED</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Option 3</t>
+  </si>
+  <si>
+    <t>Build Existing Models EnergyPlus</t>
+  </si>
+  <si>
+    <t>BuildExistingModelEnergyPlus</t>
+  </si>
+  <si>
+    <t>EnergyPlusMeasure</t>
+  </si>
+  <si>
+    <t>Always Run</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>R60 Attic Insulation Upgrade (If &lt;=R30)</t>
+  </si>
+  <si>
+    <t>Option 1 Apply Logic</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Attic|Uninsulated, Vented || Insulation Unfinished Attic|Ceiling R-7, Vented || Insulation Unfinished Attic|Ceiling R-13, Vented || Insulation Unfinished Attic|Ceiling R-19, Vented || Insulation Unfinished Attic|Ceiling R-30, Vented</t>
+  </si>
+  <si>
+    <t>Triple-Pane Windows Upgrade (If Single-Pane)</t>
+  </si>
+  <si>
+    <t>Windows|Clear, Single, Metal || Windows|Clear, Single, Non-metal</t>
+  </si>
+  <si>
+    <t>Option 2 Apply Logic</t>
   </si>
 </sst>
 </file>
@@ -5209,6 +5218,31 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Setup"/>
+      <sheetName val="Variables"/>
+      <sheetName val="Outputs"/>
+      <sheetName val="Lookups"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="24">
+          <cell r="B24">
+            <v>100</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5557,7 +5591,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5668,7 +5702,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5690,7 +5724,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5784,19 +5818,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5860,7 +5894,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5948,10 +5982,10 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C45" s="2" t="str">
         <f>"['national'," &amp; B24 &amp; "]"</f>
@@ -6008,7 +6042,7 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" bestFit="1" customWidth="1"/>
@@ -6185,13 +6219,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>40</v>
@@ -6223,10 +6257,11 @@
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45" t="s">
-        <v>287</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>349</v>
+        <v>279</v>
+      </c>
+      <c r="E5" s="45" t="str">
+        <f>LOWER(SUBSTITUTE(D5," ","_"))</f>
+        <v>building_id</v>
       </c>
       <c r="F5" s="45"/>
       <c r="G5" s="45" t="s">
@@ -6241,8 +6276,8 @@
         <v>1</v>
       </c>
       <c r="L5" s="45">
-        <f>Setup!B24</f>
-        <v>1000</v>
+        <f>[1]Setup!B24</f>
+        <v>100</v>
       </c>
       <c r="M5" s="45">
         <v>1</v>
@@ -6254,7 +6289,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6263,21 +6298,21 @@
       <c r="W5" s="45"/>
       <c r="X5" s="45"/>
     </row>
-    <row r="6" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>271</v>
+        <v>454</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>268</v>
+        <v>455</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>268</v>
+        <v>455</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>40</v>
+        <v>456</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6298,26 +6333,33 @@
       <c r="V6" s="39"/>
       <c r="W6" s="39"/>
       <c r="X6" s="39"/>
-    </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
+    </row>
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
       <c r="B7" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D7" s="45" t="str">
-        <f>"Run " &amp; B6</f>
-        <v>Run R60 Attic Insulation Upgrade</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>265</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45" t="s">
+        <v>457</v>
+      </c>
+      <c r="E7" s="45" t="str">
+        <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
+        <v>always_run</v>
+      </c>
+      <c r="F7" s="45"/>
       <c r="G7" s="45" t="s">
         <v>266</v>
       </c>
+      <c r="H7" s="45"/>
       <c r="I7" s="45">
         <v>1</v>
       </c>
+      <c r="J7" s="45"/>
       <c r="K7" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="45">
         <v>1</v>
@@ -6328,88 +6370,92 @@
       <c r="N7" s="45">
         <v>1</v>
       </c>
+      <c r="O7" s="45"/>
       <c r="P7" s="45" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+    </row>
+    <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+    </row>
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" s="45" t="str">
+        <f>"Run " &amp; B8</f>
+        <v>Run R60 Attic Insulation Upgrade (If &lt;=R30)</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I9" s="45">
+        <v>1</v>
+      </c>
+      <c r="K9" s="45">
+        <v>0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>1</v>
+      </c>
+      <c r="M9" s="45">
+        <v>1</v>
+      </c>
+      <c r="N9" s="45">
+        <v>1</v>
+      </c>
+      <c r="P9" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R7" s="45" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="R9" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -6418,10 +6464,11 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>273</v>
+        <v>449</v>
+      </c>
+      <c r="E10" s="10" t="str">
+        <f t="shared" ref="E10:E11" si="0">LOWER(SUBSTITUTE(D10," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
@@ -6429,7 +6476,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>274</v>
+        <v>448</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6449,115 +6496,116 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="39" t="s">
+    <row r="11" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>option_1_apply_logic</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>462</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D12" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E12" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="39"/>
-      <c r="X11" s="39"/>
-    </row>
-    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+    </row>
+    <row r="13" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="45" t="str">
-        <f>"Run " &amp; B11</f>
-        <v>Run Triple-Pane Windows Upgrade</v>
-      </c>
-      <c r="E12" s="45" t="s">
+      <c r="D13" s="45" t="str">
+        <f>"Run " &amp; B12</f>
+        <v>Run Triple-Pane Windows Upgrade (If Single-Pane)</v>
+      </c>
+      <c r="E13" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G13" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I12" s="45">
+      <c r="I13" s="45">
         <v>1</v>
       </c>
-      <c r="K12" s="45">
-        <v>0</v>
-      </c>
-      <c r="L12" s="45">
+      <c r="K13" s="45">
+        <v>0</v>
+      </c>
+      <c r="L13" s="45">
         <v>1</v>
       </c>
-      <c r="M12" s="45">
+      <c r="M13" s="45">
         <v>1</v>
       </c>
-      <c r="N12" s="45">
+      <c r="N13" s="45">
         <v>1</v>
       </c>
-      <c r="P12" s="45" t="s">
+      <c r="P13" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R12" s="45" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
+      <c r="R13" s="45" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="14" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -6566,10 +6614,11 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>442</v>
+        <v>449</v>
+      </c>
+      <c r="E14" s="10" t="str">
+        <f>LOWER(SUBSTITUTE(D14," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
@@ -6577,7 +6626,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>277</v>
+        <v>450</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -6604,10 +6653,11 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>273</v>
+        <v>460</v>
+      </c>
+      <c r="E15" s="10" t="str">
+        <f t="shared" ref="E15" si="1">LOWER(SUBSTITUTE(D15," ","_"))</f>
+        <v>option_1_apply_logic</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
@@ -6615,7 +6665,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>274</v>
+        <v>463</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6640,7 +6690,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C16" s="39" t="s">
         <v>268</v>
@@ -6704,7 +6754,7 @@
         <v>267</v>
       </c>
       <c r="R17" s="45" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6714,10 +6764,11 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>441</v>
+        <v>449</v>
+      </c>
+      <c r="E18" s="10" t="str">
+        <f>LOWER(SUBSTITUTE(D18," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
@@ -6725,7 +6776,7 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>278</v>
+        <v>451</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6745,153 +6796,155 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+    </row>
+    <row r="20" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="45" t="str">
+        <f>"Run " &amp; B19</f>
+        <v>Run Attic+Windows+Lighting Package</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I20" s="45">
+        <v>1</v>
+      </c>
+      <c r="K20" s="45">
+        <v>0</v>
+      </c>
+      <c r="L20" s="45">
+        <v>1</v>
+      </c>
+      <c r="M20" s="45">
+        <v>1</v>
+      </c>
+      <c r="N20" s="45">
+        <v>1</v>
+      </c>
+      <c r="P20" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="R20" s="45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="E21" s="10" t="str">
+        <f t="shared" ref="E21:E25" si="2">LOWER(SUBSTITUTE(D21," ","_"))</f>
+        <v>option_1</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-    </row>
-    <row r="20" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10" t="s">
+      <c r="H21" s="10"/>
+      <c r="I21" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+    </row>
+    <row r="22" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_1_apply_logic</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-    </row>
-    <row r="21" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-    </row>
-    <row r="22" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D22" s="45" t="str">
-        <f>"Run " &amp; B21</f>
-        <v>Run Attic+Windows+Lighting Package</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="I22" s="45">
-        <v>1</v>
-      </c>
-      <c r="K22" s="45">
-        <v>0</v>
-      </c>
-      <c r="L22" s="45">
-        <v>1</v>
-      </c>
-      <c r="M22" s="45">
-        <v>1</v>
-      </c>
-      <c r="N22" s="45">
-        <v>1</v>
-      </c>
-      <c r="P22" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="R22" s="45" t="s">
-        <v>275</v>
-      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
     </row>
     <row r="23" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
@@ -6900,10 +6953,11 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>441</v>
+        <v>452</v>
+      </c>
+      <c r="E23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_2</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10" t="s">
@@ -6911,7 +6965,7 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -6938,10 +6992,11 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>442</v>
+        <v>464</v>
+      </c>
+      <c r="E24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_2_apply_logic</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10" t="s">
@@ -6949,7 +7004,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -6976,10 +7031,11 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>273</v>
+        <v>453</v>
+      </c>
+      <c r="E25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_3</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
@@ -6987,7 +7043,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>274</v>
+        <v>451</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7012,13 +7068,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>236</v>
@@ -7048,13 +7104,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>236</v>
@@ -7253,12 +7309,12 @@
     </row>
     <row r="4" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7280,12 +7336,12 @@
     </row>
     <row r="5" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7307,12 +7363,12 @@
     </row>
     <row r="6" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7334,12 +7390,12 @@
     </row>
     <row r="7" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7361,12 +7417,12 @@
     </row>
     <row r="8" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7388,12 +7444,12 @@
     </row>
     <row r="9" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7415,12 +7471,12 @@
     </row>
     <row r="10" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
       <c r="D10" s="48" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7442,12 +7498,12 @@
     </row>
     <row r="11" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7469,12 +7525,12 @@
     </row>
     <row r="12" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7496,12 +7552,12 @@
     </row>
     <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7523,12 +7579,12 @@
     </row>
     <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7550,12 +7606,12 @@
     </row>
     <row r="15" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7577,12 +7633,12 @@
     </row>
     <row r="16" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7604,10 +7660,10 @@
     </row>
     <row r="17" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>243</v>
@@ -7624,10 +7680,10 @@
     </row>
     <row r="18" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7644,12 +7700,12 @@
     </row>
     <row r="19" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48" t="s">
@@ -7676,7 +7732,7 @@
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7698,12 +7754,12 @@
     </row>
     <row r="21" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -7725,12 +7781,12 @@
     </row>
     <row r="22" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -7752,12 +7808,12 @@
     </row>
     <row r="23" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -7779,10 +7835,10 @@
     </row>
     <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>243</v>
@@ -7799,10 +7855,10 @@
     </row>
     <row r="25" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -7819,10 +7875,10 @@
     </row>
     <row r="26" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -7839,10 +7895,10 @@
     </row>
     <row r="27" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -7859,10 +7915,10 @@
     </row>
     <row r="28" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -7879,10 +7935,10 @@
     </row>
     <row r="29" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -7899,10 +7955,10 @@
     </row>
     <row r="30" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -7919,10 +7975,10 @@
     </row>
     <row r="31" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -7939,10 +7995,10 @@
     </row>
     <row r="32" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -7959,10 +8015,10 @@
     </row>
     <row r="33" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -7979,10 +8035,10 @@
     </row>
     <row r="34" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -7999,10 +8055,10 @@
     </row>
     <row r="35" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8019,10 +8075,10 @@
     </row>
     <row r="36" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8039,10 +8095,10 @@
     </row>
     <row r="37" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8059,10 +8115,10 @@
     </row>
     <row r="38" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8079,10 +8135,10 @@
     </row>
     <row r="39" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8099,10 +8155,10 @@
     </row>
     <row r="40" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8119,10 +8175,10 @@
     </row>
     <row r="41" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8139,10 +8195,10 @@
     </row>
     <row r="42" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8159,10 +8215,10 @@
     </row>
     <row r="43" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8179,10 +8235,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8199,10 +8255,10 @@
     </row>
     <row r="45" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8219,10 +8275,10 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8239,10 +8295,10 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8259,10 +8315,10 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8279,10 +8335,10 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8299,10 +8355,10 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8319,10 +8375,10 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8339,10 +8395,10 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8359,10 +8415,10 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8379,10 +8435,10 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8399,10 +8455,10 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8419,10 +8475,10 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8439,10 +8495,10 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8459,10 +8515,10 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8479,10 +8535,10 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8499,10 +8555,10 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8519,10 +8575,10 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8539,10 +8595,10 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8559,10 +8615,10 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8579,10 +8635,10 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8599,10 +8655,10 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8619,10 +8675,10 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8639,10 +8695,10 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8659,10 +8715,10 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8679,10 +8735,10 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8702,10 +8758,10 @@
         <v>244</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G70" s="14" t="b">
         <v>0</v>
@@ -8722,10 +8778,10 @@
         <v>245</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G71" s="14" t="b">
         <v>0</v>
@@ -8742,10 +8798,10 @@
         <v>246</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G72" s="14" t="b">
         <v>0</v>
@@ -8762,10 +8818,10 @@
         <v>247</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G73" s="14" t="b">
         <v>0</v>
@@ -8782,10 +8838,10 @@
         <v>248</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -8802,10 +8858,10 @@
         <v>249</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -8822,10 +8878,10 @@
         <v>250</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -8842,10 +8898,10 @@
         <v>251</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -8862,10 +8918,10 @@
         <v>252</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -8882,10 +8938,10 @@
         <v>253</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -8902,10 +8958,10 @@
         <v>254</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -8922,10 +8978,10 @@
         <v>255</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -8942,10 +8998,10 @@
         <v>256</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -8962,10 +9018,10 @@
         <v>257</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -8982,10 +9038,10 @@
         <v>258</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G84" s="14" t="b">
         <v>0</v>
@@ -9002,10 +9058,10 @@
         <v>259</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9022,10 +9078,10 @@
         <v>260</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9042,10 +9098,10 @@
         <v>261</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>
@@ -9059,13 +9115,13 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G88" s="14" t="b">
         <v>0</v>
@@ -9083,13 +9139,13 @@
     </row>
     <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G89" s="14" t="b">
         <v>0</v>
@@ -9107,13 +9163,13 @@
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="49" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G90" s="14" t="b">
         <v>0</v>
@@ -9127,13 +9183,13 @@
     </row>
     <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="49" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G91" s="14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Allow "!" in apply logic for ApplyUpgrade measure, addresses #37. Some refactoring.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -1422,9 +1422,6 @@
     <t>Option 1 Apply Logic</t>
   </si>
   <si>
-    <t>Insulation Unfinished Attic|Uninsulated, Vented || Insulation Unfinished Attic|Ceiling R-7, Vented || Insulation Unfinished Attic|Ceiling R-13, Vented || Insulation Unfinished Attic|Ceiling R-19, Vented || Insulation Unfinished Attic|Ceiling R-30, Vented</t>
-  </si>
-  <si>
     <t>Triple-Pane Windows Upgrade (If Single-Pane)</t>
   </si>
   <si>
@@ -1432,6 +1429,9 @@
   </si>
   <si>
     <t>Option 2 Apply Logic</t>
+  </si>
+  <si>
+    <t>!Insulation Unfinished Attic|Ceiling R-38, Vented &amp;&amp; !Insulation Unfinished Attic|Ceiling R-49, Vented &amp;&amp; !Insulation Unfinished Attic|Ceiling R-60, Vented</t>
   </si>
 </sst>
 </file>
@@ -5231,7 +5231,7 @@
       <sheetData sheetId="0">
         <row r="24">
           <cell r="B24">
-            <v>100</v>
+            <v>1000</v>
           </cell>
         </row>
       </sheetData>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="L5" s="45">
         <f>[1]Setup!B24</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="M5" s="45">
         <v>1</v>
@@ -6515,7 +6515,7 @@
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -6540,7 +6540,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>268</v>
@@ -6665,7 +6665,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6926,7 +6926,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E24" s="10" t="str">
         <f t="shared" si="2"/>
@@ -7004,7 +7004,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>

</xml_diff>

<commit_message>
Connected new HVAC systems to measures. Fixed foundations for testing mode. Hooked up flue argument as appropriate.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Outputs" sheetId="12" r:id="rId3"/>
     <sheet name="Lookups" sheetId="11" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outputs!$A$2:$H$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$3</definedName>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="465">
   <si>
     <t>type</t>
   </si>
@@ -846,42 +849,15 @@
     <t>Insulation Unfinished Attic</t>
   </si>
   <si>
-    <t>Ceiling R-60, Vented</t>
-  </si>
-  <si>
-    <t>R60 Attic Insulation Upgrade</t>
-  </si>
-  <si>
-    <t>Apply Logic</t>
-  </si>
-  <si>
-    <t>apply_logic</t>
-  </si>
-  <si>
-    <t>FIXME</t>
-  </si>
-  <si>
     <t>discrete</t>
   </si>
   <si>
     <t>Windows</t>
   </si>
   <si>
-    <t>Low-E, Triple, Non-metal, Air, L-Gain</t>
-  </si>
-  <si>
     <t>Lighting</t>
   </si>
   <si>
-    <t>100% LED</t>
-  </si>
-  <si>
-    <t>Attic+Windows+Lighting Package</t>
-  </si>
-  <si>
-    <t>Triple-Pane Windows Upgrade</t>
-  </si>
-  <si>
     <t>LED Lighting Upgrade</t>
   </si>
   <si>
@@ -1083,9 +1059,6 @@
     <t>Mechanical Ventilation</t>
   </si>
   <si>
-    <t>building_id</t>
-  </si>
-  <si>
     <t>Simulation Output Report</t>
   </si>
   <si>
@@ -1353,24 +1326,6 @@
     <t>0 or 1 (defines whether to run upgrade and existing building simulations, or only upgrade simulations)</t>
   </si>
   <si>
-    <t>Insulation Unfinished Attic|Windows|Lighting</t>
-  </si>
-  <si>
-    <t>Ceiling R-60, Vented|Low-E, Triple, Non-metal, Air, L-Gain|100% LED</t>
-  </si>
-  <si>
-    <t>parameter_names</t>
-  </si>
-  <si>
-    <t>option_names</t>
-  </si>
-  <si>
-    <t>Parameter Names</t>
-  </si>
-  <si>
-    <t>Option Names</t>
-  </si>
-  <si>
     <t>ResStock_National</t>
   </si>
   <si>
@@ -1423,6 +1378,60 @@
   </si>
   <si>
     <t>1.20.1</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Windows|Low-E, Triple, Non-metal, Air, L-Gain</t>
+  </si>
+  <si>
+    <t>Lighting|100% LED</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Option 3</t>
+  </si>
+  <si>
+    <t>Build Existing Models EnergyPlus</t>
+  </si>
+  <si>
+    <t>BuildExistingModelEnergyPlus</t>
+  </si>
+  <si>
+    <t>EnergyPlusMeasure</t>
+  </si>
+  <si>
+    <t>Always Run</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>Option 1 Apply Logic</t>
+  </si>
+  <si>
+    <t>Triple-Pane Windows Upgrade (If Single-Pane)</t>
+  </si>
+  <si>
+    <t>Windows|Clear, Single, Metal || Windows|Clear, Single, Non-metal</t>
+  </si>
+  <si>
+    <t>Option 2 Apply Logic</t>
+  </si>
+  <si>
+    <t>R13 Wall Insulation Upgrade (If Uninsulated)</t>
+  </si>
+  <si>
+    <t>Insulation Wall|Wood Stud, R-13</t>
+  </si>
+  <si>
+    <t>Insulation Wall|Wood Stud, Uninsulated</t>
+  </si>
+  <si>
+    <t>Walls+Windows+Lighting Package</t>
   </si>
 </sst>
 </file>
@@ -5209,6 +5218,31 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Setup"/>
+      <sheetName val="Variables"/>
+      <sheetName val="Outputs"/>
+      <sheetName val="Lookups"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="24">
+          <cell r="B24">
+            <v>100</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5557,7 +5591,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5668,7 +5702,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5690,7 +5724,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5784,19 +5818,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5860,7 +5894,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5948,10 +5982,10 @@
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C45" s="2" t="str">
         <f>"['national'," &amp; B24 &amp; "]"</f>
@@ -6008,7 +6042,7 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" bestFit="1" customWidth="1"/>
@@ -6185,13 +6219,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>40</v>
@@ -6223,10 +6257,11 @@
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45" t="s">
-        <v>287</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>349</v>
+        <v>278</v>
+      </c>
+      <c r="E5" s="45" t="str">
+        <f>LOWER(SUBSTITUTE(D5," ","_"))</f>
+        <v>building_id</v>
       </c>
       <c r="F5" s="45"/>
       <c r="G5" s="45" t="s">
@@ -6241,8 +6276,8 @@
         <v>1</v>
       </c>
       <c r="L5" s="45">
-        <f>Setup!B24</f>
-        <v>1000</v>
+        <f>[1]Setup!B24</f>
+        <v>100</v>
       </c>
       <c r="M5" s="45">
         <v>1</v>
@@ -6254,7 +6289,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6263,21 +6298,21 @@
       <c r="W5" s="45"/>
       <c r="X5" s="45"/>
     </row>
-    <row r="6" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>271</v>
+        <v>452</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>268</v>
+        <v>453</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>268</v>
+        <v>453</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>40</v>
+        <v>454</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6298,26 +6333,33 @@
       <c r="V6" s="39"/>
       <c r="W6" s="39"/>
       <c r="X6" s="39"/>
-    </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
+    </row>
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
       <c r="B7" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D7" s="45" t="str">
-        <f>"Run " &amp; B6</f>
-        <v>Run R60 Attic Insulation Upgrade</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>265</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45" t="s">
+        <v>455</v>
+      </c>
+      <c r="E7" s="45" t="str">
+        <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
+        <v>always_run</v>
+      </c>
+      <c r="F7" s="45"/>
       <c r="G7" s="45" t="s">
         <v>266</v>
       </c>
+      <c r="H7" s="45"/>
       <c r="I7" s="45">
         <v>1</v>
       </c>
+      <c r="J7" s="45"/>
       <c r="K7" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="45">
         <v>1</v>
@@ -6328,88 +6370,92 @@
       <c r="N7" s="45">
         <v>1</v>
       </c>
+      <c r="O7" s="45"/>
       <c r="P7" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+    </row>
+    <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>461</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+    </row>
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" s="45" t="str">
+        <f>"Run " &amp; B8</f>
+        <v>Run R13 Wall Insulation Upgrade (If Uninsulated)</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I9" s="45">
+        <v>1</v>
+      </c>
+      <c r="K9" s="45">
+        <v>0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>1</v>
+      </c>
+      <c r="M9" s="45">
+        <v>1</v>
+      </c>
+      <c r="N9" s="45">
+        <v>1</v>
+      </c>
+      <c r="P9" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R7" s="45" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="R9" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -6418,10 +6464,11 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>273</v>
+        <v>447</v>
+      </c>
+      <c r="E10" s="10" t="str">
+        <f t="shared" ref="E10:E11" si="0">LOWER(SUBSTITUTE(D10," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
@@ -6429,7 +6476,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>274</v>
+        <v>462</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6449,115 +6496,116 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="39" t="s">
+    <row r="11" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="E11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>option_1_apply_logic</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>458</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D12" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E12" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="39"/>
-      <c r="X11" s="39"/>
-    </row>
-    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+    </row>
+    <row r="13" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="45" t="str">
-        <f>"Run " &amp; B11</f>
-        <v>Run Triple-Pane Windows Upgrade</v>
-      </c>
-      <c r="E12" s="45" t="s">
+      <c r="D13" s="45" t="str">
+        <f>"Run " &amp; B12</f>
+        <v>Run Triple-Pane Windows Upgrade (If Single-Pane)</v>
+      </c>
+      <c r="E13" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G13" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I12" s="45">
+      <c r="I13" s="45">
         <v>1</v>
       </c>
-      <c r="K12" s="45">
-        <v>0</v>
-      </c>
-      <c r="L12" s="45">
+      <c r="K13" s="45">
+        <v>0</v>
+      </c>
+      <c r="L13" s="45">
         <v>1</v>
       </c>
-      <c r="M12" s="45">
+      <c r="M13" s="45">
         <v>1</v>
       </c>
-      <c r="N12" s="45">
+      <c r="N13" s="45">
         <v>1</v>
       </c>
-      <c r="P12" s="45" t="s">
+      <c r="P13" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R12" s="45" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
+      <c r="R13" s="45" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="14" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -6566,10 +6614,11 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>442</v>
+        <v>447</v>
+      </c>
+      <c r="E14" s="10" t="str">
+        <f>LOWER(SUBSTITUTE(D14," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
@@ -6577,7 +6626,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>277</v>
+        <v>448</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -6604,10 +6653,11 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>273</v>
+        <v>457</v>
+      </c>
+      <c r="E15" s="10" t="str">
+        <f t="shared" ref="E15" si="1">LOWER(SUBSTITUTE(D15," ","_"))</f>
+        <v>option_1_apply_logic</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
@@ -6615,7 +6665,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>274</v>
+        <v>459</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6637,10 +6687,10 @@
     </row>
     <row r="16" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C16" s="39" t="s">
         <v>268</v>
@@ -6704,7 +6754,7 @@
         <v>267</v>
       </c>
       <c r="R17" s="45" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6714,10 +6764,11 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>441</v>
+        <v>447</v>
+      </c>
+      <c r="E18" s="10" t="str">
+        <f>LOWER(SUBSTITUTE(D18," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
@@ -6725,7 +6776,7 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>278</v>
+        <v>449</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6745,153 +6796,155 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+    </row>
+    <row r="20" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="45" t="str">
+        <f>"Run " &amp; B19</f>
+        <v>Run Walls+Windows+Lighting Package</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I20" s="45">
+        <v>1</v>
+      </c>
+      <c r="K20" s="45">
+        <v>0</v>
+      </c>
+      <c r="L20" s="45">
+        <v>1</v>
+      </c>
+      <c r="M20" s="45">
+        <v>1</v>
+      </c>
+      <c r="N20" s="45">
+        <v>1</v>
+      </c>
+      <c r="P20" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="R20" s="45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="E21" s="10" t="str">
+        <f t="shared" ref="E21:E25" si="2">LOWER(SUBSTITUTE(D21," ","_"))</f>
+        <v>option_1</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-    </row>
-    <row r="20" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10" t="s">
+      <c r="H21" s="10"/>
+      <c r="I21" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+    </row>
+    <row r="22" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="E22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_1_apply_logic</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-    </row>
-    <row r="21" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-    </row>
-    <row r="22" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="D22" s="45" t="str">
-        <f>"Run " &amp; B21</f>
-        <v>Run Attic+Windows+Lighting Package</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="I22" s="45">
-        <v>1</v>
-      </c>
-      <c r="K22" s="45">
-        <v>0</v>
-      </c>
-      <c r="L22" s="45">
-        <v>1</v>
-      </c>
-      <c r="M22" s="45">
-        <v>1</v>
-      </c>
-      <c r="N22" s="45">
-        <v>1</v>
-      </c>
-      <c r="P22" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="R22" s="45" t="s">
-        <v>275</v>
-      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
     </row>
     <row r="23" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
@@ -6900,10 +6953,11 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>441</v>
+        <v>450</v>
+      </c>
+      <c r="E23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_2</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10" t="s">
@@ -6911,7 +6965,7 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -6938,10 +6992,11 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>442</v>
+        <v>460</v>
+      </c>
+      <c r="E24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_2_apply_logic</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10" t="s">
@@ -6949,7 +7004,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>440</v>
+        <v>459</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -6976,10 +7031,11 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>273</v>
+        <v>451</v>
+      </c>
+      <c r="E25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_3</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
@@ -6987,7 +7043,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>274</v>
+        <v>449</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7012,13 +7068,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>236</v>
@@ -7048,13 +7104,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>236</v>
@@ -7253,12 +7309,12 @@
     </row>
     <row r="4" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7280,12 +7336,12 @@
     </row>
     <row r="5" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7307,12 +7363,12 @@
     </row>
     <row r="6" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7334,12 +7390,12 @@
     </row>
     <row r="7" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7361,12 +7417,12 @@
     </row>
     <row r="8" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7388,12 +7444,12 @@
     </row>
     <row r="9" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7415,12 +7471,12 @@
     </row>
     <row r="10" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
       <c r="D10" s="48" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7442,12 +7498,12 @@
     </row>
     <row r="11" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7469,12 +7525,12 @@
     </row>
     <row r="12" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7496,12 +7552,12 @@
     </row>
     <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7523,12 +7579,12 @@
     </row>
     <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7550,12 +7606,12 @@
     </row>
     <row r="15" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7577,12 +7633,12 @@
     </row>
     <row r="16" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7604,10 +7660,10 @@
     </row>
     <row r="17" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>243</v>
@@ -7624,10 +7680,10 @@
     </row>
     <row r="18" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7644,12 +7700,12 @@
     </row>
     <row r="19" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48" t="s">
@@ -7676,7 +7732,7 @@
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7698,12 +7754,12 @@
     </row>
     <row r="21" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -7725,12 +7781,12 @@
     </row>
     <row r="22" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -7752,12 +7808,12 @@
     </row>
     <row r="23" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -7779,10 +7835,10 @@
     </row>
     <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>243</v>
@@ -7799,10 +7855,10 @@
     </row>
     <row r="25" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -7819,10 +7875,10 @@
     </row>
     <row r="26" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -7839,10 +7895,10 @@
     </row>
     <row r="27" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -7859,10 +7915,10 @@
     </row>
     <row r="28" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -7879,10 +7935,10 @@
     </row>
     <row r="29" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -7899,10 +7955,10 @@
     </row>
     <row r="30" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -7919,10 +7975,10 @@
     </row>
     <row r="31" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -7939,10 +7995,10 @@
     </row>
     <row r="32" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -7959,10 +8015,10 @@
     </row>
     <row r="33" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -7979,10 +8035,10 @@
     </row>
     <row r="34" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -7999,10 +8055,10 @@
     </row>
     <row r="35" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8019,10 +8075,10 @@
     </row>
     <row r="36" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8039,10 +8095,10 @@
     </row>
     <row r="37" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8059,10 +8115,10 @@
     </row>
     <row r="38" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8079,10 +8135,10 @@
     </row>
     <row r="39" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8099,10 +8155,10 @@
     </row>
     <row r="40" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8119,10 +8175,10 @@
     </row>
     <row r="41" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8139,10 +8195,10 @@
     </row>
     <row r="42" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8159,10 +8215,10 @@
     </row>
     <row r="43" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8179,10 +8235,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8199,10 +8255,10 @@
     </row>
     <row r="45" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8219,10 +8275,10 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8239,10 +8295,10 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8259,10 +8315,10 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8279,10 +8335,10 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8299,10 +8355,10 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8319,10 +8375,10 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8339,10 +8395,10 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8359,10 +8415,10 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8379,10 +8435,10 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8399,10 +8455,10 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8419,10 +8475,10 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8439,10 +8495,10 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8459,10 +8515,10 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8479,10 +8535,10 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8499,10 +8555,10 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8519,10 +8575,10 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8539,10 +8595,10 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8559,10 +8615,10 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8579,10 +8635,10 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8599,10 +8655,10 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8619,10 +8675,10 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8639,10 +8695,10 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8659,10 +8715,10 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8679,10 +8735,10 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8702,10 +8758,10 @@
         <v>244</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G70" s="14" t="b">
         <v>0</v>
@@ -8722,10 +8778,10 @@
         <v>245</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G71" s="14" t="b">
         <v>0</v>
@@ -8742,10 +8798,10 @@
         <v>246</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G72" s="14" t="b">
         <v>0</v>
@@ -8762,10 +8818,10 @@
         <v>247</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G73" s="14" t="b">
         <v>0</v>
@@ -8782,10 +8838,10 @@
         <v>248</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -8802,10 +8858,10 @@
         <v>249</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -8822,10 +8878,10 @@
         <v>250</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -8842,10 +8898,10 @@
         <v>251</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -8862,10 +8918,10 @@
         <v>252</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -8882,10 +8938,10 @@
         <v>253</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -8902,10 +8958,10 @@
         <v>254</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -8922,10 +8978,10 @@
         <v>255</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -8942,10 +8998,10 @@
         <v>256</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -8962,10 +9018,10 @@
         <v>257</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -8982,10 +9038,10 @@
         <v>258</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G84" s="14" t="b">
         <v>0</v>
@@ -9002,10 +9058,10 @@
         <v>259</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9022,10 +9078,10 @@
         <v>260</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9042,10 +9098,10 @@
         <v>261</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>
@@ -9059,13 +9115,13 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G88" s="14" t="b">
         <v>0</v>
@@ -9083,13 +9139,13 @@
     </row>
     <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G89" s="14" t="b">
         <v>0</v>
@@ -9107,13 +9163,13 @@
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="49" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G90" s="14" t="b">
         <v>0</v>
@@ -9127,13 +9183,13 @@
     </row>
     <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="49" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="G91" s="14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added ability to specify upgrade package-level apply logic, addresses #37. Latest measures.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="468">
   <si>
     <t>type</t>
   </si>
@@ -1431,7 +1431,16 @@
     <t>Insulation Wall|Wood Stud, Uninsulated</t>
   </si>
   <si>
-    <t>Walls+Windows+Lighting Package</t>
+    <t>Upgrade Package (Allow Individual Options)</t>
+  </si>
+  <si>
+    <t>Upgrade Package (All or None)</t>
+  </si>
+  <si>
+    <t>Package Apply Logic</t>
+  </si>
+  <si>
+    <t>Insulation Wall|Wood Stud, Uninsulated &amp;&amp; (Windows|Clear, Single, Metal || Windows|Clear, Single, Non-metal)</t>
   </si>
 </sst>
 </file>
@@ -5231,7 +5240,7 @@
       <sheetData sheetId="0">
         <row r="24">
           <cell r="B24">
-            <v>100</v>
+            <v>1000</v>
           </cell>
         </row>
       </sheetData>
@@ -6035,7 +6044,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -6277,7 +6286,7 @@
       </c>
       <c r="L5" s="45">
         <f>[1]Setup!B24</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="M5" s="45">
         <v>1</v>
@@ -6838,7 +6847,7 @@
       </c>
       <c r="D20" s="45" t="str">
         <f>"Run " &amp; B19</f>
-        <v>Run Walls+Windows+Lighting Package</v>
+        <v>Run Upgrade Package (Allow Individual Options)</v>
       </c>
       <c r="E20" s="45" t="s">
         <v>265</v>
@@ -7063,119 +7072,347 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="b">
+    <row r="26" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="39" t="s">
+        <v>465</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+    </row>
+    <row r="27" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D27" s="45" t="str">
+        <f>"Run " &amp; B26</f>
+        <v>Run Upgrade Package (All or None)</v>
+      </c>
+      <c r="E27" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="I27" s="45">
+        <v>1</v>
+      </c>
+      <c r="K27" s="45">
+        <v>0</v>
+      </c>
+      <c r="L27" s="45">
+        <v>1</v>
+      </c>
+      <c r="M27" s="45">
+        <v>1</v>
+      </c>
+      <c r="N27" s="45">
+        <v>1</v>
+      </c>
+      <c r="P27" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="R27" s="45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="E28" s="10" t="str">
+        <f t="shared" ref="E28:E31" si="3">LOWER(SUBSTITUTE(D28," ","_"))</f>
+        <v>option_1</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+    </row>
+    <row r="29" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E29" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>option_2</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+    </row>
+    <row r="30" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="E30" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>option_3</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+    </row>
+    <row r="31" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="E31" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>package_apply_logic</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
+    </row>
+    <row r="32" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" s="40" t="s">
         <v>360</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C32" s="40" t="s">
         <v>361</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D32" s="40" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E32" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="40"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="40"/>
-      <c r="X26" s="40"/>
-    </row>
-    <row r="27" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="b">
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="40"/>
+      <c r="X32" s="40"/>
+    </row>
+    <row r="33" spans="1:24" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B33" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C33" s="40" t="s">
         <v>341</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D33" s="40" t="s">
         <v>341</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E33" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="40"/>
-      <c r="U27" s="40"/>
-      <c r="V27" s="40"/>
-      <c r="W27" s="40"/>
-      <c r="X27" s="40"/>
-    </row>
-    <row r="28" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="40" t="b">
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
+      <c r="X33" s="40"/>
+    </row>
+    <row r="34" spans="1:24" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B34" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C34" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D34" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E34" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40"/>
-      <c r="T28" s="40"/>
-      <c r="U28" s="40"/>
-      <c r="V28" s="40"/>
-      <c r="W28" s="40"/>
-      <c r="X28" s="40"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="40"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="40"/>
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B35" s="50"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B36" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>

</xml_diff>

<commit_message>
Synch everything else with heating fuel-specific HVAC tsv files.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="476">
   <si>
     <t>type</t>
   </si>
@@ -993,9 +993,6 @@
     <t>HVAC System Combined</t>
   </si>
   <si>
-    <t>HVAC System Heating</t>
-  </si>
-  <si>
     <t>HVAC System Cooling</t>
   </si>
   <si>
@@ -1248,9 +1245,6 @@
     <t>building_characteristics_report.HVAC System Combined</t>
   </si>
   <si>
-    <t>building_characteristics_report.HVAC System Heating</t>
-  </si>
-  <si>
     <t>building_characteristics_report.HVAC System Cooling</t>
   </si>
   <si>
@@ -1441,6 +1435,36 @@
   </si>
   <si>
     <t>Insulation Wall|Wood Stud, Uninsulated &amp;&amp; (Windows|Clear, Single, Metal || Windows|Clear, Single, Non-metal)</t>
+  </si>
+  <si>
+    <t>HVAC System Heating Electricity</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.HVAC System Heating Electricity</t>
+  </si>
+  <si>
+    <t>HVAC System Heating Fuel Oil</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.HVAC System Heating Fuel Oil</t>
+  </si>
+  <si>
+    <t>HVAC System Heating Natural Gas</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.HVAC System Heating Natural Gas</t>
+  </si>
+  <si>
+    <t>HVAC System Heating Other Fuel</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.HVAC System Heating Other Fuel</t>
+  </si>
+  <si>
+    <t>HVAC System Heating Propane</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.HVAC System Heating Propane</t>
   </si>
 </sst>
 </file>
@@ -5600,7 +5624,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5711,7 +5735,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5733,7 +5757,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5827,19 +5851,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5903,7 +5927,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6298,7 +6322,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6312,16 +6336,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="39" t="s">
+        <v>450</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>451</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>451</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>452</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>453</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>453</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>454</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6352,7 +6376,7 @@
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="45" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E7" s="45" t="str">
         <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
@@ -6381,7 +6405,7 @@
       </c>
       <c r="O7" s="45"/>
       <c r="P7" s="45" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q7" s="45"/>
       <c r="R7" s="45" t="s">
@@ -6399,7 +6423,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>268</v>
@@ -6473,7 +6497,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E10" s="10" t="str">
         <f t="shared" ref="E10:E11" si="0">LOWER(SUBSTITUTE(D10," ","_"))</f>
@@ -6485,7 +6509,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6512,7 +6536,7 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E11" s="10" t="str">
         <f t="shared" si="0"/>
@@ -6524,7 +6548,7 @@
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -6549,7 +6573,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>268</v>
@@ -6623,7 +6647,7 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E14" s="10" t="str">
         <f>LOWER(SUBSTITUTE(D14," ","_"))</f>
@@ -6635,7 +6659,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -6662,7 +6686,7 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E15" s="10" t="str">
         <f t="shared" ref="E15" si="1">LOWER(SUBSTITUTE(D15," ","_"))</f>
@@ -6674,7 +6698,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6773,7 +6797,7 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E18" s="10" t="str">
         <f>LOWER(SUBSTITUTE(D18," ","_"))</f>
@@ -6785,7 +6809,7 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6810,7 +6834,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>268</v>
@@ -6884,7 +6908,7 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E21" s="10" t="str">
         <f t="shared" ref="E21:E25" si="2">LOWER(SUBSTITUTE(D21," ","_"))</f>
@@ -6896,7 +6920,7 @@
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -6923,7 +6947,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E22" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6935,7 +6959,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6962,7 +6986,7 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E23" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6974,7 +6998,7 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -7001,7 +7025,7 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E24" s="10" t="str">
         <f t="shared" si="2"/>
@@ -7013,7 +7037,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -7040,7 +7064,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E25" s="10" t="str">
         <f t="shared" si="2"/>
@@ -7052,7 +7076,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7077,7 +7101,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>268</v>
@@ -7151,7 +7175,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E28" s="10" t="str">
         <f t="shared" ref="E28:E31" si="3">LOWER(SUBSTITUTE(D28," ","_"))</f>
@@ -7163,7 +7187,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -7190,7 +7214,7 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E29" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7202,7 +7226,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -7229,7 +7253,7 @@
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E30" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7241,7 +7265,7 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -7268,7 +7292,7 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E31" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7280,7 +7304,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7305,13 +7329,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="C32" s="40" t="s">
         <v>360</v>
       </c>
-      <c r="C32" s="40" t="s">
-        <v>361</v>
-      </c>
       <c r="D32" s="40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>236</v>
@@ -7341,13 +7365,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="40" t="s">
+        <v>339</v>
+      </c>
+      <c r="C33" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="C33" s="40" t="s">
-        <v>341</v>
-      </c>
       <c r="D33" s="40" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E33" s="40" t="s">
         <v>236</v>
@@ -7426,7 +7450,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M128"/>
+  <dimension ref="A1:M132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -7551,7 +7575,7 @@
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7578,7 +7602,7 @@
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7605,7 +7629,7 @@
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7632,7 +7656,7 @@
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7659,7 +7683,7 @@
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7686,7 +7710,7 @@
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7713,7 +7737,7 @@
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
       <c r="D10" s="48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7740,7 +7764,7 @@
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7767,7 +7791,7 @@
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7789,12 +7813,12 @@
     </row>
     <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7821,7 +7845,7 @@
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7848,7 +7872,7 @@
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7875,7 +7899,7 @@
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7900,7 +7924,7 @@
         <v>291</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>243</v>
@@ -7920,7 +7944,7 @@
         <v>292</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7942,7 +7966,7 @@
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48" t="s">
@@ -7969,7 +7993,7 @@
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7996,7 +8020,7 @@
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -8023,7 +8047,7 @@
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -8050,7 +8074,7 @@
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -8075,7 +8099,7 @@
         <v>297</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>243</v>
@@ -8095,7 +8119,7 @@
         <v>298</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -8115,7 +8139,7 @@
         <v>299</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -8135,7 +8159,7 @@
         <v>300</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -8155,7 +8179,7 @@
         <v>301</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -8175,7 +8199,7 @@
         <v>302</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -8195,7 +8219,7 @@
         <v>303</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -8215,7 +8239,7 @@
         <v>304</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -8235,7 +8259,7 @@
         <v>305</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -8255,7 +8279,7 @@
         <v>306</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -8275,7 +8299,7 @@
         <v>307</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -8295,7 +8319,7 @@
         <v>308</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8315,7 +8339,7 @@
         <v>309</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8335,7 +8359,7 @@
         <v>310</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8355,7 +8379,7 @@
         <v>311</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8375,7 +8399,7 @@
         <v>312</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8395,7 +8419,7 @@
         <v>313</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8415,7 +8439,7 @@
         <v>271</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8435,7 +8459,7 @@
         <v>314</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8455,7 +8479,7 @@
         <v>315</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8472,10 +8496,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8495,7 +8519,7 @@
         <v>316</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8515,7 +8539,7 @@
         <v>317</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8532,10 +8556,10 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>318</v>
+        <v>466</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>403</v>
+        <v>467</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8552,10 +8576,10 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>319</v>
+        <v>468</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>404</v>
+        <v>469</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8572,10 +8596,10 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>320</v>
+        <v>470</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>405</v>
+        <v>471</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8592,10 +8616,10 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>321</v>
+        <v>472</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>406</v>
+        <v>473</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8612,10 +8636,10 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>322</v>
+        <v>474</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>407</v>
+        <v>475</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8632,10 +8656,10 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8652,10 +8676,10 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8672,10 +8696,10 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8692,10 +8716,10 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8712,10 +8736,10 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>272</v>
+        <v>322</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8732,10 +8756,10 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8752,10 +8776,10 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8772,10 +8796,10 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8792,10 +8816,10 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>330</v>
+        <v>272</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8812,10 +8836,10 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8832,10 +8856,10 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8852,10 +8876,10 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8872,10 +8896,10 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8892,10 +8916,10 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8912,10 +8936,10 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8932,10 +8956,10 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8952,10 +8976,10 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8972,10 +8996,10 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8990,95 +9014,95 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
-        <v>244</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="F70" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G70" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I70" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
-        <v>245</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G71" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I71" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="F72" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G72" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H72" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I72" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G73" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H73" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I73" s="14" t="b">
+    <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="48" t="s">
+        <v>335</v>
+      </c>
+      <c r="D70" s="48" t="s">
+        <v>420</v>
+      </c>
+      <c r="F70" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G70" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="D71" s="48" t="s">
+        <v>421</v>
+      </c>
+      <c r="F71" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="48" t="s">
+        <v>337</v>
+      </c>
+      <c r="D72" s="48" t="s">
+        <v>422</v>
+      </c>
+      <c r="F72" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G72" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="48" t="s">
+        <v>338</v>
+      </c>
+      <c r="D73" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="F73" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -9092,13 +9116,13 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -9112,13 +9136,13 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -9132,13 +9156,13 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -9152,13 +9176,13 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -9172,13 +9196,13 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -9192,13 +9216,13 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -9212,93 +9236,93 @@
     </row>
     <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="F81" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G81" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="49" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G82" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G83" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G84" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="D81" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="F81" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G81" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H81" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I81" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G82" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H82" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I82" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="F83" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G83" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H83" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I83" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G84" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H84" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I84" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="s">
-        <v>259</v>
-      </c>
       <c r="D85" s="14" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9312,13 +9336,13 @@
     </row>
     <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9332,13 +9356,13 @@
     </row>
     <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>
@@ -9352,13 +9376,13 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>436</v>
+        <v>258</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>437</v>
+        <v>355</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G88" s="14" t="b">
         <v>0</v>
@@ -9369,20 +9393,16 @@
       <c r="I88" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J88" s="49"/>
-      <c r="K88" s="49"/>
-      <c r="L88" s="49"/>
-      <c r="M88" s="49"/>
     </row>
     <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>438</v>
+        <v>259</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>439</v>
+        <v>356</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G89" s="14" t="b">
         <v>0</v>
@@ -9393,86 +9413,134 @@
       <c r="I89" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J89" s="49"/>
-      <c r="K89" s="49"/>
-      <c r="L89" s="49"/>
-      <c r="M89" s="49"/>
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="49" t="s">
+      <c r="A90" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G91" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G92" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J92" s="49"/>
+      <c r="K92" s="49"/>
+      <c r="L92" s="49"/>
+      <c r="M92" s="49"/>
+    </row>
+    <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J93" s="49"/>
+      <c r="K93" s="49"/>
+      <c r="L93" s="49"/>
+      <c r="M93" s="49"/>
+    </row>
+    <row r="94" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="49" t="s">
+        <v>440</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G94" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="49" t="s">
         <v>442</v>
       </c>
-      <c r="D90" s="14" t="s">
+      <c r="D95" s="14" t="s">
         <v>443</v>
       </c>
-      <c r="F90" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G90" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H90" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I90" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
-        <v>444</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G91" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H91" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I91" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15"/>
-      <c r="B92" s="21"/>
-      <c r="D92" s="15"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="15"/>
-      <c r="H92" s="15"/>
-      <c r="I92" s="15"/>
-    </row>
-    <row r="93" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-      <c r="B93" s="21"/>
-      <c r="D93" s="15"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
-      <c r="I93" s="15"/>
-    </row>
-    <row r="94" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
-      <c r="B94" s="21"/>
-      <c r="D94" s="15"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
-      <c r="H94" s="15"/>
-      <c r="I94" s="15"/>
-    </row>
-    <row r="95" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
-      <c r="B95" s="21"/>
-      <c r="D95" s="15"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
-      <c r="I95" s="15"/>
+      <c r="F95" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G95" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
@@ -9717,45 +9785,37 @@
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123" s="21"/>
-      <c r="C123" s="22"/>
       <c r="D123" s="15"/>
-      <c r="E123" s="22"/>
       <c r="F123" s="15"/>
       <c r="G123" s="15"/>
       <c r="H123" s="15"/>
       <c r="I123" s="15"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124" s="21"/>
-      <c r="C124" s="22"/>
       <c r="D124" s="15"/>
-      <c r="E124" s="22"/>
       <c r="F124" s="15"/>
       <c r="G124" s="15"/>
       <c r="H124" s="15"/>
       <c r="I124" s="15"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15"/>
       <c r="B125" s="21"/>
-      <c r="C125" s="22"/>
       <c r="D125" s="15"/>
-      <c r="E125" s="22"/>
       <c r="F125" s="15"/>
       <c r="G125" s="15"/>
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
       <c r="B126" s="21"/>
-      <c r="C126" s="22"/>
       <c r="D126" s="15"/>
-      <c r="E126" s="22"/>
       <c r="F126" s="15"/>
       <c r="G126" s="15"/>
       <c r="H126" s="15"/>
@@ -9782,6 +9842,50 @@
       <c r="G128" s="15"/>
       <c r="H128" s="15"/>
       <c r="I128" s="15"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="15"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="22"/>
+      <c r="D129" s="15"/>
+      <c r="E129" s="22"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
+      <c r="I129" s="15"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="15"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="22"/>
+      <c r="D130" s="15"/>
+      <c r="E130" s="22"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="15"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="22"/>
+      <c r="D131" s="15"/>
+      <c r="E131" s="22"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="15"/>
+      <c r="I131" s="15"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="15"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="22"/>
+      <c r="D132" s="15"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="15"/>
+      <c r="G132" s="15"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Merged Insulation Interzonal Wall into Insulation Wall.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -12,9 +12,6 @@
     <sheet name="Outputs" sheetId="12" r:id="rId3"/>
     <sheet name="Lookups" sheetId="11" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outputs!$A$2:$H$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$3</definedName>
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="405">
   <si>
     <t>type</t>
   </si>
@@ -924,9 +921,6 @@
     <t>Insulation Wall</t>
   </si>
   <si>
-    <t>Insulation Interzonal Wall</t>
-  </si>
-  <si>
     <t>Insulation Slab</t>
   </si>
   <si>
@@ -1122,195 +1116,6 @@
     <t>BuildingCharacteristicsReport</t>
   </si>
   <si>
-    <t>building_characteristics_report.Location Region</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Location EPW</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Vintage</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Heating Fuel</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Usage Level</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Geometry Foundation Type</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Geometry House Size</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Geometry Stories</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Geometry Garage</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Orientation</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Eaves</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Overhangs</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Door Area</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Window Areas</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Neighbors</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Unfinished Attic</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Wall</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Interzonal Wall</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Slab</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Crawlspace</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Unfinished Basement</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Finished Basement</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Insulation Interzonal Floor</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Uninsulated Surfaces</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Roof Sheathing</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Wall Sheathing</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Floor Sheathing</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Exterior Finish</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Roof Material</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Floor Covering</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Thermal Mass Floor</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Thermal Mass Exterior Wall</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Thermal Mass Partition Wall</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Thermal Mass Ceiling</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Thermal Mass Furniture</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Doors</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Windows</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Water Heater</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Hot Water Fixtures</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.HVAC System Is Combined</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.HVAC System Combined</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.HVAC System Cooling</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Heating Setpoint</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Cooling Setpoint</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Refrigerator</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Cooking Range</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Dishwasher</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Clothes Washer</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Clothes Dryer</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Lighting</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Plug Loads</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Extra Refrigerator</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Freezer</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Gas Fireplace</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Gas Grill</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Gas Lighting</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Hot Tub Spa</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Pool</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Misc Well Pump</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Ducts</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Infiltration</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Natural Ventilation</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Mechanical Ventilation</t>
-  </si>
-  <si>
     <t>Double</t>
   </si>
   <si>
@@ -1335,9 +1140,6 @@
     <t>Hot Water Distribution</t>
   </si>
   <si>
-    <t>building_characteristics_report.Hot Water Distribution</t>
-  </si>
-  <si>
     <t>../analysis_results</t>
   </si>
   <si>
@@ -1356,9 +1158,6 @@
     <t>Occupants</t>
   </si>
   <si>
-    <t>building_characteristics_report.Occupants</t>
-  </si>
-  <si>
     <t>HVAC Cooling Capacity W</t>
   </si>
   <si>
@@ -1440,31 +1239,16 @@
     <t>HVAC System Heating Electricity</t>
   </si>
   <si>
-    <t>building_characteristics_report.HVAC System Heating Electricity</t>
-  </si>
-  <si>
     <t>HVAC System Heating Fuel Oil</t>
   </si>
   <si>
-    <t>building_characteristics_report.HVAC System Heating Fuel Oil</t>
-  </si>
-  <si>
     <t>HVAC System Heating Natural Gas</t>
   </si>
   <si>
-    <t>building_characteristics_report.HVAC System Heating Natural Gas</t>
-  </si>
-  <si>
     <t>HVAC System Heating Other Fuel</t>
   </si>
   <si>
-    <t>building_characteristics_report.HVAC System Heating Other Fuel</t>
-  </si>
-  <si>
     <t>HVAC System Heating Propane</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.HVAC System Heating Propane</t>
   </si>
 </sst>
 </file>
@@ -5251,31 +5035,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Setup"/>
-      <sheetName val="Variables"/>
-      <sheetName val="Outputs"/>
-      <sheetName val="Lookups"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="24">
-          <cell r="B24">
-            <v>1000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5624,7 +5383,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>444</v>
+        <v>378</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5735,7 +5494,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>427</v>
+        <v>363</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5757,7 +5516,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>433</v>
+        <v>368</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5851,19 +5610,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>425</v>
+        <v>361</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>430</v>
+        <v>366</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>426</v>
+        <v>362</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5927,7 +5686,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>428</v>
+        <v>364</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6309,7 +6068,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="45">
-        <f>[1]Setup!B24</f>
+        <f>Setup!B24</f>
         <v>1000</v>
       </c>
       <c r="M5" s="45">
@@ -6322,7 +6081,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>429</v>
+        <v>365</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6336,16 +6095,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>451</v>
+        <v>385</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>451</v>
+        <v>385</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6376,7 +6135,7 @@
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="45" t="s">
-        <v>453</v>
+        <v>387</v>
       </c>
       <c r="E7" s="45" t="str">
         <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
@@ -6405,7 +6164,7 @@
       </c>
       <c r="O7" s="45"/>
       <c r="P7" s="45" t="s">
-        <v>454</v>
+        <v>388</v>
       </c>
       <c r="Q7" s="45"/>
       <c r="R7" s="45" t="s">
@@ -6423,7 +6182,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>459</v>
+        <v>393</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>268</v>
@@ -6497,7 +6256,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="E10" s="10" t="str">
         <f t="shared" ref="E10:E11" si="0">LOWER(SUBSTITUTE(D10," ","_"))</f>
@@ -6509,7 +6268,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>460</v>
+        <v>394</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6536,7 +6295,7 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>455</v>
+        <v>389</v>
       </c>
       <c r="E11" s="10" t="str">
         <f t="shared" si="0"/>
@@ -6548,7 +6307,7 @@
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>461</v>
+        <v>395</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -6573,7 +6332,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>456</v>
+        <v>390</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>268</v>
@@ -6647,7 +6406,7 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="E14" s="10" t="str">
         <f>LOWER(SUBSTITUTE(D14," ","_"))</f>
@@ -6659,7 +6418,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -6686,7 +6445,7 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>455</v>
+        <v>389</v>
       </c>
       <c r="E15" s="10" t="str">
         <f t="shared" ref="E15" si="1">LOWER(SUBSTITUTE(D15," ","_"))</f>
@@ -6698,7 +6457,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>457</v>
+        <v>391</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6797,7 +6556,7 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="E18" s="10" t="str">
         <f>LOWER(SUBSTITUTE(D18," ","_"))</f>
@@ -6809,7 +6568,7 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6834,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>462</v>
+        <v>396</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>268</v>
@@ -6908,7 +6667,7 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="E21" s="10" t="str">
         <f t="shared" ref="E21:E25" si="2">LOWER(SUBSTITUTE(D21," ","_"))</f>
@@ -6920,7 +6679,7 @@
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10" t="s">
-        <v>460</v>
+        <v>394</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -6947,7 +6706,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>455</v>
+        <v>389</v>
       </c>
       <c r="E22" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6959,7 +6718,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>461</v>
+        <v>395</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6986,7 +6745,7 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>448</v>
+        <v>382</v>
       </c>
       <c r="E23" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6998,7 +6757,7 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -7025,7 +6784,7 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>458</v>
+        <v>392</v>
       </c>
       <c r="E24" s="10" t="str">
         <f t="shared" si="2"/>
@@ -7037,7 +6796,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>457</v>
+        <v>391</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -7064,7 +6823,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>449</v>
+        <v>383</v>
       </c>
       <c r="E25" s="10" t="str">
         <f t="shared" si="2"/>
@@ -7076,7 +6835,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7101,7 +6860,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>463</v>
+        <v>397</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>268</v>
@@ -7175,7 +6934,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="E28" s="10" t="str">
         <f t="shared" ref="E28:E31" si="3">LOWER(SUBSTITUTE(D28," ","_"))</f>
@@ -7187,7 +6946,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>460</v>
+        <v>394</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -7214,7 +6973,7 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>448</v>
+        <v>382</v>
       </c>
       <c r="E29" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7226,7 +6985,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -7253,7 +7012,7 @@
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>449</v>
+        <v>383</v>
       </c>
       <c r="E30" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7265,7 +7024,7 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -7292,7 +7051,7 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>464</v>
+        <v>398</v>
       </c>
       <c r="E31" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7304,7 +7063,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>465</v>
+        <v>399</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7329,13 +7088,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="C32" s="40" t="s">
         <v>359</v>
       </c>
-      <c r="C32" s="40" t="s">
-        <v>360</v>
-      </c>
       <c r="D32" s="40" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>236</v>
@@ -7365,13 +7124,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="C33" s="40" t="s">
         <v>339</v>
       </c>
-      <c r="C33" s="40" t="s">
-        <v>340</v>
-      </c>
       <c r="D33" s="40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E33" s="40" t="s">
         <v>236</v>
@@ -7450,7 +7209,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M132"/>
+  <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -7574,8 +7333,9 @@
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
-      <c r="D4" s="48" t="s">
-        <v>361</v>
+      <c r="D4" s="48" t="str">
+        <f>"building_characteristics_report."&amp;A4</f>
+        <v>building_characteristics_report.Location Region</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7601,8 +7361,9 @@
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
-      <c r="D5" s="48" t="s">
-        <v>362</v>
+      <c r="D5" s="48" t="str">
+        <f t="shared" ref="D5:D67" si="0">"building_characteristics_report."&amp;A5</f>
+        <v>building_characteristics_report.Location EPW</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7628,8 +7389,9 @@
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
-      <c r="D6" s="48" t="s">
-        <v>363</v>
+      <c r="D6" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Vintage</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7655,8 +7417,9 @@
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
-      <c r="D7" s="48" t="s">
-        <v>364</v>
+      <c r="D7" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Heating Fuel</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7682,8 +7445,9 @@
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
-      <c r="D8" s="48" t="s">
-        <v>365</v>
+      <c r="D8" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Usage Level</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7709,8 +7473,9 @@
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
-      <c r="D9" s="48" t="s">
-        <v>366</v>
+      <c r="D9" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Geometry Foundation Type</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7736,8 +7501,9 @@
       </c>
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
-      <c r="D10" s="48" t="s">
-        <v>367</v>
+      <c r="D10" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Geometry House Size</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7763,8 +7529,9 @@
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
-      <c r="D11" s="48" t="s">
-        <v>368</v>
+      <c r="D11" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Geometry Stories</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7790,8 +7557,9 @@
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
-      <c r="D12" s="48" t="s">
-        <v>369</v>
+      <c r="D12" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Geometry Garage</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7813,12 +7581,13 @@
     </row>
     <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>438</v>
+        <v>373</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
-      <c r="D13" s="48" t="s">
-        <v>439</v>
+      <c r="D13" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Occupants</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7844,8 +7613,9 @@
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
-      <c r="D14" s="48" t="s">
-        <v>370</v>
+      <c r="D14" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Orientation</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7871,8 +7641,9 @@
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
-      <c r="D15" s="48" t="s">
-        <v>371</v>
+      <c r="D15" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Eaves</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7898,8 +7669,9 @@
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
-      <c r="D16" s="48" t="s">
-        <v>372</v>
+      <c r="D16" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Overhangs</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7923,8 +7695,9 @@
       <c r="A17" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="D17" s="48" t="s">
-        <v>373</v>
+      <c r="D17" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Door Area</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>243</v>
@@ -7943,8 +7716,9 @@
       <c r="A18" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="D18" s="48" t="s">
-        <v>374</v>
+      <c r="D18" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Window Areas</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7965,8 +7739,9 @@
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
-      <c r="D19" s="48" t="s">
-        <v>375</v>
+      <c r="D19" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Neighbors</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48" t="s">
@@ -7992,8 +7767,9 @@
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
-      <c r="D20" s="48" t="s">
-        <v>376</v>
+      <c r="D20" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Unfinished Attic</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -8019,8 +7795,9 @@
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
-      <c r="D21" s="48" t="s">
-        <v>377</v>
+      <c r="D21" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Wall</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -8046,8 +7823,9 @@
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
-      <c r="D22" s="48" t="s">
-        <v>378</v>
+      <c r="D22" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Slab</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -8071,12 +7849,10 @@
       <c r="A23" s="48" t="s">
         <v>296</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48" t="s">
-        <v>379</v>
-      </c>
-      <c r="E23" s="48"/>
+      <c r="D23" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Crawlspace</v>
+      </c>
       <c r="F23" s="48" t="s">
         <v>243</v>
       </c>
@@ -8089,17 +7865,14 @@
       <c r="I23" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
     </row>
     <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="D24" s="48" t="s">
-        <v>380</v>
+      <c r="D24" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Unfinished Basement</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>243</v>
@@ -8118,8 +7891,9 @@
       <c r="A25" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="D25" s="48" t="s">
-        <v>381</v>
+      <c r="D25" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Finished Basement</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -8138,8 +7912,9 @@
       <c r="A26" s="48" t="s">
         <v>299</v>
       </c>
-      <c r="D26" s="48" t="s">
-        <v>382</v>
+      <c r="D26" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Insulation Interzonal Floor</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -8158,8 +7933,9 @@
       <c r="A27" s="48" t="s">
         <v>300</v>
       </c>
-      <c r="D27" s="48" t="s">
-        <v>383</v>
+      <c r="D27" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Uninsulated Surfaces</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -8178,8 +7954,9 @@
       <c r="A28" s="48" t="s">
         <v>301</v>
       </c>
-      <c r="D28" s="48" t="s">
-        <v>384</v>
+      <c r="D28" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Roof Sheathing</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -8198,8 +7975,9 @@
       <c r="A29" s="48" t="s">
         <v>302</v>
       </c>
-      <c r="D29" s="48" t="s">
-        <v>385</v>
+      <c r="D29" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Wall Sheathing</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -8218,8 +7996,9 @@
       <c r="A30" s="48" t="s">
         <v>303</v>
       </c>
-      <c r="D30" s="48" t="s">
-        <v>386</v>
+      <c r="D30" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Floor Sheathing</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -8238,8 +8017,9 @@
       <c r="A31" s="48" t="s">
         <v>304</v>
       </c>
-      <c r="D31" s="48" t="s">
-        <v>387</v>
+      <c r="D31" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Exterior Finish</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -8258,8 +8038,9 @@
       <c r="A32" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="D32" s="48" t="s">
-        <v>388</v>
+      <c r="D32" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Roof Material</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -8278,8 +8059,9 @@
       <c r="A33" s="48" t="s">
         <v>306</v>
       </c>
-      <c r="D33" s="48" t="s">
-        <v>389</v>
+      <c r="D33" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Floor Covering</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -8298,8 +8080,9 @@
       <c r="A34" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="D34" s="48" t="s">
-        <v>390</v>
+      <c r="D34" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Thermal Mass Floor</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -8318,8 +8101,9 @@
       <c r="A35" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="D35" s="48" t="s">
-        <v>391</v>
+      <c r="D35" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Thermal Mass Exterior Wall</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8338,8 +8122,9 @@
       <c r="A36" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="48" t="s">
-        <v>392</v>
+      <c r="D36" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Thermal Mass Partition Wall</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8358,8 +8143,9 @@
       <c r="A37" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="D37" s="48" t="s">
-        <v>393</v>
+      <c r="D37" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Thermal Mass Ceiling</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8378,8 +8164,9 @@
       <c r="A38" s="48" t="s">
         <v>311</v>
       </c>
-      <c r="D38" s="48" t="s">
-        <v>394</v>
+      <c r="D38" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Thermal Mass Furniture</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8398,8 +8185,9 @@
       <c r="A39" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="D39" s="48" t="s">
-        <v>395</v>
+      <c r="D39" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Doors</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8416,10 +8204,11 @@
     </row>
     <row r="40" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>313</v>
-      </c>
-      <c r="D40" s="48" t="s">
-        <v>396</v>
+        <v>271</v>
+      </c>
+      <c r="D40" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Windows</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8436,10 +8225,11 @@
     </row>
     <row r="41" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>271</v>
-      </c>
-      <c r="D41" s="48" t="s">
-        <v>397</v>
+        <v>313</v>
+      </c>
+      <c r="D41" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Water Heater</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8458,8 +8248,9 @@
       <c r="A42" s="48" t="s">
         <v>314</v>
       </c>
-      <c r="D42" s="48" t="s">
-        <v>398</v>
+      <c r="D42" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Hot Water Fixtures</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8476,10 +8267,11 @@
     </row>
     <row r="43" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>315</v>
-      </c>
-      <c r="D43" s="48" t="s">
-        <v>399</v>
+        <v>367</v>
+      </c>
+      <c r="D43" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Hot Water Distribution</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8496,10 +8288,11 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>431</v>
-      </c>
-      <c r="D44" s="48" t="s">
-        <v>432</v>
+        <v>315</v>
+      </c>
+      <c r="D44" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Is Combined</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8518,8 +8311,9 @@
       <c r="A45" s="48" t="s">
         <v>316</v>
       </c>
-      <c r="D45" s="48" t="s">
-        <v>400</v>
+      <c r="D45" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Combined</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8536,10 +8330,11 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>317</v>
-      </c>
-      <c r="D46" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
+      </c>
+      <c r="D46" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Heating Electricity</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8556,10 +8351,11 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>466</v>
-      </c>
-      <c r="D47" s="48" t="s">
-        <v>467</v>
+        <v>401</v>
+      </c>
+      <c r="D47" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Heating Fuel Oil</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8576,10 +8372,11 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>468</v>
-      </c>
-      <c r="D48" s="48" t="s">
-        <v>469</v>
+        <v>402</v>
+      </c>
+      <c r="D48" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Heating Natural Gas</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8596,10 +8393,11 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>470</v>
-      </c>
-      <c r="D49" s="48" t="s">
-        <v>471</v>
+        <v>403</v>
+      </c>
+      <c r="D49" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Heating Other Fuel</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8616,10 +8414,11 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>472</v>
-      </c>
-      <c r="D50" s="48" t="s">
-        <v>473</v>
+        <v>404</v>
+      </c>
+      <c r="D50" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Heating Propane</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8636,10 +8435,11 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>474</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>475</v>
+        <v>317</v>
+      </c>
+      <c r="D51" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.HVAC System Cooling</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8658,8 +8458,9 @@
       <c r="A52" s="48" t="s">
         <v>318</v>
       </c>
-      <c r="D52" s="48" t="s">
-        <v>402</v>
+      <c r="D52" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Heating Setpoint</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8678,8 +8479,9 @@
       <c r="A53" s="48" t="s">
         <v>319</v>
       </c>
-      <c r="D53" s="48" t="s">
-        <v>403</v>
+      <c r="D53" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Cooling Setpoint</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8698,8 +8500,9 @@
       <c r="A54" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="D54" s="48" t="s">
-        <v>404</v>
+      <c r="D54" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Refrigerator</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8718,8 +8521,9 @@
       <c r="A55" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="D55" s="48" t="s">
-        <v>405</v>
+      <c r="D55" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Cooking Range</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8738,8 +8542,9 @@
       <c r="A56" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="D56" s="48" t="s">
-        <v>406</v>
+      <c r="D56" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Dishwasher</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8758,8 +8563,9 @@
       <c r="A57" s="48" t="s">
         <v>323</v>
       </c>
-      <c r="D57" s="48" t="s">
-        <v>407</v>
+      <c r="D57" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Clothes Washer</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8778,8 +8584,9 @@
       <c r="A58" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="D58" s="48" t="s">
-        <v>408</v>
+      <c r="D58" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Clothes Dryer</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8796,10 +8603,11 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>325</v>
-      </c>
-      <c r="D59" s="48" t="s">
-        <v>409</v>
+        <v>272</v>
+      </c>
+      <c r="D59" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Lighting</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8816,10 +8624,11 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>272</v>
-      </c>
-      <c r="D60" s="48" t="s">
-        <v>410</v>
+        <v>325</v>
+      </c>
+      <c r="D60" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Plug Loads</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8838,8 +8647,9 @@
       <c r="A61" s="48" t="s">
         <v>326</v>
       </c>
-      <c r="D61" s="48" t="s">
-        <v>411</v>
+      <c r="D61" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Extra Refrigerator</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8858,8 +8668,9 @@
       <c r="A62" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="D62" s="48" t="s">
-        <v>412</v>
+      <c r="D62" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Freezer</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8878,8 +8689,9 @@
       <c r="A63" s="48" t="s">
         <v>328</v>
       </c>
-      <c r="D63" s="48" t="s">
-        <v>413</v>
+      <c r="D63" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Gas Fireplace</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8898,8 +8710,9 @@
       <c r="A64" s="48" t="s">
         <v>329</v>
       </c>
-      <c r="D64" s="48" t="s">
-        <v>414</v>
+      <c r="D64" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Gas Grill</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8918,8 +8731,9 @@
       <c r="A65" s="48" t="s">
         <v>330</v>
       </c>
-      <c r="D65" s="48" t="s">
-        <v>415</v>
+      <c r="D65" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Gas Lighting</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8938,8 +8752,9 @@
       <c r="A66" s="48" t="s">
         <v>331</v>
       </c>
-      <c r="D66" s="48" t="s">
-        <v>416</v>
+      <c r="D66" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Hot Tub Spa</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8958,8 +8773,9 @@
       <c r="A67" s="48" t="s">
         <v>332</v>
       </c>
-      <c r="D67" s="48" t="s">
-        <v>417</v>
+      <c r="D67" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.Misc Pool</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8978,8 +8794,9 @@
       <c r="A68" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="D68" s="48" t="s">
-        <v>418</v>
+      <c r="D68" s="48" t="str">
+        <f t="shared" ref="D68:D72" si="1">"building_characteristics_report."&amp;A68</f>
+        <v>building_characteristics_report.Misc Well Pump</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8998,8 +8815,9 @@
       <c r="A69" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="D69" s="48" t="s">
-        <v>419</v>
+      <c r="D69" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.Ducts</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -9018,8 +8836,9 @@
       <c r="A70" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="D70" s="48" t="s">
-        <v>420</v>
+      <c r="D70" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.Infiltration</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>243</v>
@@ -9038,8 +8857,9 @@
       <c r="A71" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="D71" s="48" t="s">
-        <v>421</v>
+      <c r="D71" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.Natural Ventilation</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>243</v>
@@ -9058,8 +8878,9 @@
       <c r="A72" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="D72" s="48" t="s">
-        <v>422</v>
+      <c r="D72" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.Mechanical Ventilation</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>243</v>
@@ -9074,35 +8895,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="48" t="s">
-        <v>338</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>423</v>
-      </c>
-      <c r="F73" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="G73" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H73" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I73" s="48" t="b">
+    <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G73" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D74" s="14" t="s">
         <v>341</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -9116,13 +8937,13 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D75" s="14" t="s">
         <v>342</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -9136,13 +8957,13 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D76" s="14" t="s">
         <v>343</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -9156,13 +8977,13 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D77" s="14" t="s">
         <v>344</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -9176,13 +8997,13 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D78" s="14" t="s">
         <v>345</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -9196,13 +9017,13 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D79" s="14" t="s">
         <v>346</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -9216,13 +9037,13 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D80" s="14" t="s">
         <v>347</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -9236,13 +9057,13 @@
     </row>
     <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D81" s="14" t="s">
         <v>348</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -9256,13 +9077,13 @@
     </row>
     <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D82" s="14" t="s">
         <v>349</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -9276,13 +9097,13 @@
     </row>
     <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="49" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D83" s="14" t="s">
         <v>350</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -9296,13 +9117,13 @@
     </row>
     <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="49" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D84" s="14" t="s">
         <v>351</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G84" s="14" t="b">
         <v>0</v>
@@ -9315,14 +9136,14 @@
       </c>
     </row>
     <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="49" t="s">
-        <v>255</v>
+      <c r="A85" s="14" t="s">
+        <v>256</v>
       </c>
       <c r="D85" s="14" t="s">
         <v>352</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9336,13 +9157,13 @@
     </row>
     <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D86" s="14" t="s">
         <v>353</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9356,13 +9177,13 @@
     </row>
     <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D87" s="14" t="s">
         <v>354</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>
@@ -9376,13 +9197,13 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D88" s="14" t="s">
         <v>355</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G88" s="14" t="b">
         <v>0</v>
@@ -9396,13 +9217,13 @@
     </row>
     <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D89" s="14" t="s">
         <v>356</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G89" s="14" t="b">
         <v>0</v>
@@ -9416,13 +9237,13 @@
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D90" s="14" t="s">
         <v>357</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G90" s="14" t="b">
         <v>0</v>
@@ -9436,13 +9257,13 @@
     </row>
     <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>261</v>
+        <v>369</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G91" s="14" t="b">
         <v>0</v>
@@ -9453,16 +9274,20 @@
       <c r="I91" s="14" t="b">
         <v>0</v>
       </c>
+      <c r="J91" s="49"/>
+      <c r="K91" s="49"/>
+      <c r="L91" s="49"/>
+      <c r="M91" s="49"/>
     </row>
     <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>434</v>
+        <v>371</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>435</v>
+        <v>372</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G92" s="14" t="b">
         <v>0</v>
@@ -9479,14 +9304,14 @@
       <c r="M92" s="49"/>
     </row>
     <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="s">
-        <v>436</v>
+      <c r="A93" s="49" t="s">
+        <v>374</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>437</v>
+        <v>375</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G93" s="14" t="b">
         <v>0</v>
@@ -9497,20 +9322,16 @@
       <c r="I93" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J93" s="49"/>
-      <c r="K93" s="49"/>
-      <c r="L93" s="49"/>
-      <c r="M93" s="49"/>
     </row>
     <row r="94" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="49" t="s">
-        <v>440</v>
+        <v>376</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>441</v>
+        <v>377</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>424</v>
+        <v>360</v>
       </c>
       <c r="G94" s="14" t="b">
         <v>0</v>
@@ -9522,25 +9343,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="s">
-        <v>442</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="F95" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="G95" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H95" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I95" s="14" t="b">
-        <v>0</v>
-      </c>
+    <row r="95" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="15"/>
+      <c r="B95" s="21"/>
+      <c r="D95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
     </row>
     <row r="96" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
@@ -9812,10 +9622,12 @@
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
     </row>
-    <row r="126" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
       <c r="B126" s="21"/>
+      <c r="C126" s="22"/>
       <c r="D126" s="15"/>
+      <c r="E126" s="22"/>
       <c r="F126" s="15"/>
       <c r="G126" s="15"/>
       <c r="H126" s="15"/>
@@ -9875,17 +9687,6 @@
       <c r="G131" s="15"/>
       <c r="H131" s="15"/>
       <c r="I131" s="15"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="15"/>
-      <c r="B132" s="21"/>
-      <c r="C132" s="22"/>
-      <c r="D132" s="15"/>
-      <c r="E132" s="22"/>
-      <c r="F132" s="15"/>
-      <c r="G132" s="15"/>
-      <c r="H132" s="15"/>
-      <c r="I132" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Latest measures. Update to 1.14 AMI. Various changes to reporting measures and output variables to handle a 1.14 change where registerValue now stores the name in snake case.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="384">
   <si>
     <t>type</t>
   </si>
@@ -1056,60 +1056,6 @@
     <t>SimulationOutputReport</t>
   </si>
   <si>
-    <t>simulation_output_report.Total Site Energy MBtu</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Total Site Electricity kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Total Site Natural Gas therm</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Total Site Other Fuel MBtu</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Heating kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Cooling kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Interior Lighting kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Exterior Lighting kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Interior Equipment kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Fans kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Pumps kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Electricity Water Systems kWh</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Natural Gas Heating therm</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Natural Gas Interior Equipment therm</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Natural Gas Water Systems therm</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Other Fuel Heating MBtu</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Other Fuel Interior Equipment MBtu</t>
-  </si>
-  <si>
-    <t>simulation_output_report.Other Fuel Water Systems MBtu</t>
-  </si>
-  <si>
     <t>Building Characteristics Report</t>
   </si>
   <si>
@@ -1146,33 +1092,18 @@
     <t>Hours Heating Setpoint Not Met</t>
   </si>
   <si>
-    <t>simulation_output_report.Hours Heating Setpoint Not Met</t>
-  </si>
-  <si>
     <t>Hours Cooling Setpoint Not Met</t>
   </si>
   <si>
-    <t>simulation_output_report.Hours Cooling Setpoint Not Met</t>
-  </si>
-  <si>
     <t>Occupants</t>
   </si>
   <si>
     <t>HVAC Cooling Capacity W</t>
   </si>
   <si>
-    <t>simulation_output_report.HVAC Cooling Capacity W</t>
-  </si>
-  <si>
     <t>HVAC Heating Capacity W</t>
   </si>
   <si>
-    <t>simulation_output_report.HVAC Heating Capacity W</t>
-  </si>
-  <si>
-    <t>1.20.1</t>
-  </si>
-  <si>
     <t>Option 1</t>
   </si>
   <si>
@@ -1249,6 +1180,12 @@
   </si>
   <si>
     <t>HVAC System Heating Propane</t>
+  </si>
+  <si>
+    <t>1.21.14</t>
+  </si>
+  <si>
+    <t>Ceiling Fan</t>
   </si>
 </sst>
 </file>
@@ -5383,7 +5320,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>154</v>
@@ -5494,7 +5431,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>76</v>
@@ -5516,7 +5453,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>155</v>
@@ -5610,19 +5547,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="22"/>
@@ -5686,7 +5623,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5829,7 +5766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6081,7 +6020,7 @@
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="45" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
@@ -6095,16 +6034,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6135,7 +6074,7 @@
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="45" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="E7" s="45" t="str">
         <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
@@ -6164,7 +6103,7 @@
       </c>
       <c r="O7" s="45"/>
       <c r="P7" s="45" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="Q7" s="45"/>
       <c r="R7" s="45" t="s">
@@ -6179,10 +6118,10 @@
     </row>
     <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>268</v>
@@ -6256,7 +6195,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="E10" s="10" t="str">
         <f t="shared" ref="E10:E11" si="0">LOWER(SUBSTITUTE(D10," ","_"))</f>
@@ -6268,7 +6207,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6295,7 +6234,7 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="E11" s="10" t="str">
         <f t="shared" si="0"/>
@@ -6307,7 +6246,7 @@
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -6329,10 +6268,10 @@
     </row>
     <row r="12" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>268</v>
@@ -6406,7 +6345,7 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="E14" s="10" t="str">
         <f>LOWER(SUBSTITUTE(D14," ","_"))</f>
@@ -6418,7 +6357,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -6445,7 +6384,7 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="E15" s="10" t="str">
         <f t="shared" ref="E15" si="1">LOWER(SUBSTITUTE(D15," ","_"))</f>
@@ -6457,7 +6396,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6479,7 +6418,7 @@
     </row>
     <row r="16" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="39" t="s">
         <v>273</v>
@@ -6556,7 +6495,7 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="E18" s="10" t="str">
         <f>LOWER(SUBSTITUTE(D18," ","_"))</f>
@@ -6568,7 +6507,7 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6590,10 +6529,10 @@
     </row>
     <row r="19" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>268</v>
@@ -6667,7 +6606,7 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="E21" s="10" t="str">
         <f t="shared" ref="E21:E25" si="2">LOWER(SUBSTITUTE(D21," ","_"))</f>
@@ -6679,7 +6618,7 @@
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -6706,7 +6645,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="E22" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6718,7 +6657,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6745,7 +6684,7 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="E23" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6757,7 +6696,7 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -6784,7 +6723,7 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="E24" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6796,7 +6735,7 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -6823,7 +6762,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="E25" s="10" t="str">
         <f t="shared" si="2"/>
@@ -6835,7 +6774,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -6857,10 +6796,10 @@
     </row>
     <row r="26" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>268</v>
@@ -6934,7 +6873,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="E28" s="10" t="str">
         <f t="shared" ref="E28:E31" si="3">LOWER(SUBSTITUTE(D28," ","_"))</f>
@@ -6946,7 +6885,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -6973,7 +6912,7 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="E29" s="10" t="str">
         <f t="shared" si="3"/>
@@ -6985,7 +6924,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -7012,7 +6951,7 @@
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="E30" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7024,7 +6963,7 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -7051,7 +6990,7 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="E31" s="10" t="str">
         <f t="shared" si="3"/>
@@ -7063,7 +7002,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7088,13 +7027,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="40" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>236</v>
@@ -7209,11 +7148,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M131"/>
+  <dimension ref="A1:M132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7334,8 +7273,8 @@
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48" t="str">
-        <f>"building_characteristics_report."&amp;A4</f>
-        <v>building_characteristics_report.Location Region</v>
+        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A4," ","_"))</f>
+        <v>building_characteristics_report.location_region</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48" t="s">
@@ -7362,8 +7301,8 @@
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48" t="str">
-        <f t="shared" ref="D5:D67" si="0">"building_characteristics_report."&amp;A5</f>
-        <v>building_characteristics_report.Location EPW</v>
+        <f t="shared" ref="D5:D68" si="0">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A5," ","_"))</f>
+        <v>building_characteristics_report.location_epw</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48" t="s">
@@ -7391,7 +7330,7 @@
       <c r="C6" s="48"/>
       <c r="D6" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Vintage</v>
+        <v>building_characteristics_report.vintage</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="48" t="s">
@@ -7419,7 +7358,7 @@
       <c r="C7" s="48"/>
       <c r="D7" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Heating Fuel</v>
+        <v>building_characteristics_report.heating_fuel</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48" t="s">
@@ -7447,7 +7386,7 @@
       <c r="C8" s="48"/>
       <c r="D8" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Usage Level</v>
+        <v>building_characteristics_report.usage_level</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="48" t="s">
@@ -7475,7 +7414,7 @@
       <c r="C9" s="48"/>
       <c r="D9" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Geometry Foundation Type</v>
+        <v>building_characteristics_report.geometry_foundation_type</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="48" t="s">
@@ -7503,7 +7442,7 @@
       <c r="C10" s="48"/>
       <c r="D10" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Geometry House Size</v>
+        <v>building_characteristics_report.geometry_house_size</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48" t="s">
@@ -7531,7 +7470,7 @@
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Geometry Stories</v>
+        <v>building_characteristics_report.geometry_stories</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7559,7 +7498,7 @@
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Geometry Garage</v>
+        <v>building_characteristics_report.geometry_garage</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7581,13 +7520,13 @@
     </row>
     <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Occupants</v>
+        <v>building_characteristics_report.occupants</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7615,7 +7554,7 @@
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Orientation</v>
+        <v>building_characteristics_report.orientation</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7643,7 +7582,7 @@
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Eaves</v>
+        <v>building_characteristics_report.eaves</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7671,7 +7610,7 @@
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Overhangs</v>
+        <v>building_characteristics_report.overhangs</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7697,7 +7636,7 @@
       </c>
       <c r="D17" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Door Area</v>
+        <v>building_characteristics_report.door_area</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>243</v>
@@ -7718,7 +7657,7 @@
       </c>
       <c r="D18" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Window Areas</v>
+        <v>building_characteristics_report.window_areas</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>243</v>
@@ -7741,7 +7680,7 @@
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Neighbors</v>
+        <v>building_characteristics_report.neighbors</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48" t="s">
@@ -7769,7 +7708,7 @@
       <c r="C20" s="48"/>
       <c r="D20" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Unfinished Attic</v>
+        <v>building_characteristics_report.insulation_unfinished_attic</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48" t="s">
@@ -7797,7 +7736,7 @@
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Wall</v>
+        <v>building_characteristics_report.insulation_wall</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -7825,7 +7764,7 @@
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Slab</v>
+        <v>building_characteristics_report.insulation_slab</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -7851,7 +7790,7 @@
       </c>
       <c r="D23" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Crawlspace</v>
+        <v>building_characteristics_report.insulation_crawlspace</v>
       </c>
       <c r="F23" s="48" t="s">
         <v>243</v>
@@ -7872,7 +7811,7 @@
       </c>
       <c r="D24" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Unfinished Basement</v>
+        <v>building_characteristics_report.insulation_unfinished_basement</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>243</v>
@@ -7893,7 +7832,7 @@
       </c>
       <c r="D25" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Finished Basement</v>
+        <v>building_characteristics_report.insulation_finished_basement</v>
       </c>
       <c r="F25" s="48" t="s">
         <v>243</v>
@@ -7914,7 +7853,7 @@
       </c>
       <c r="D26" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Insulation Interzonal Floor</v>
+        <v>building_characteristics_report.insulation_interzonal_floor</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>243</v>
@@ -7935,7 +7874,7 @@
       </c>
       <c r="D27" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Uninsulated Surfaces</v>
+        <v>building_characteristics_report.uninsulated_surfaces</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>243</v>
@@ -7956,7 +7895,7 @@
       </c>
       <c r="D28" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Roof Sheathing</v>
+        <v>building_characteristics_report.roof_sheathing</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>243</v>
@@ -7977,7 +7916,7 @@
       </c>
       <c r="D29" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Wall Sheathing</v>
+        <v>building_characteristics_report.wall_sheathing</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>243</v>
@@ -7998,7 +7937,7 @@
       </c>
       <c r="D30" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Floor Sheathing</v>
+        <v>building_characteristics_report.floor_sheathing</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>243</v>
@@ -8019,7 +7958,7 @@
       </c>
       <c r="D31" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Exterior Finish</v>
+        <v>building_characteristics_report.exterior_finish</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>243</v>
@@ -8040,7 +7979,7 @@
       </c>
       <c r="D32" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Roof Material</v>
+        <v>building_characteristics_report.roof_material</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>243</v>
@@ -8061,7 +8000,7 @@
       </c>
       <c r="D33" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Floor Covering</v>
+        <v>building_characteristics_report.floor_covering</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>243</v>
@@ -8082,7 +8021,7 @@
       </c>
       <c r="D34" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Thermal Mass Floor</v>
+        <v>building_characteristics_report.thermal_mass_floor</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>243</v>
@@ -8103,7 +8042,7 @@
       </c>
       <c r="D35" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Thermal Mass Exterior Wall</v>
+        <v>building_characteristics_report.thermal_mass_exterior_wall</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>243</v>
@@ -8124,7 +8063,7 @@
       </c>
       <c r="D36" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Thermal Mass Partition Wall</v>
+        <v>building_characteristics_report.thermal_mass_partition_wall</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>243</v>
@@ -8145,7 +8084,7 @@
       </c>
       <c r="D37" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Thermal Mass Ceiling</v>
+        <v>building_characteristics_report.thermal_mass_ceiling</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>243</v>
@@ -8166,7 +8105,7 @@
       </c>
       <c r="D38" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Thermal Mass Furniture</v>
+        <v>building_characteristics_report.thermal_mass_furniture</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>243</v>
@@ -8187,7 +8126,7 @@
       </c>
       <c r="D39" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Doors</v>
+        <v>building_characteristics_report.doors</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>243</v>
@@ -8208,7 +8147,7 @@
       </c>
       <c r="D40" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Windows</v>
+        <v>building_characteristics_report.windows</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>243</v>
@@ -8229,7 +8168,7 @@
       </c>
       <c r="D41" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Water Heater</v>
+        <v>building_characteristics_report.water_heater</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8250,7 +8189,7 @@
       </c>
       <c r="D42" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Hot Water Fixtures</v>
+        <v>building_characteristics_report.hot_water_fixtures</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
@@ -8267,11 +8206,11 @@
     </row>
     <row r="43" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
       <c r="D43" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Hot Water Distribution</v>
+        <v>building_characteristics_report.hot_water_distribution</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>243</v>
@@ -8292,7 +8231,7 @@
       </c>
       <c r="D44" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Is Combined</v>
+        <v>building_characteristics_report.hvac_system_is_combined</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>243</v>
@@ -8313,7 +8252,7 @@
       </c>
       <c r="D45" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Combined</v>
+        <v>building_characteristics_report.hvac_system_combined</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
@@ -8330,11 +8269,11 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="D46" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Heating Electricity</v>
+        <v>building_characteristics_report.hvac_system_heating_electricity</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
@@ -8351,11 +8290,11 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="D47" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Heating Fuel Oil</v>
+        <v>building_characteristics_report.hvac_system_heating_fuel_oil</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -8372,11 +8311,11 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="D48" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Heating Natural Gas</v>
+        <v>building_characteristics_report.hvac_system_heating_natural_gas</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -8393,11 +8332,11 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="D49" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Heating Other Fuel</v>
+        <v>building_characteristics_report.hvac_system_heating_other_fuel</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -8414,11 +8353,11 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="D50" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Heating Propane</v>
+        <v>building_characteristics_report.hvac_system_heating_propane</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -8439,7 +8378,7 @@
       </c>
       <c r="D51" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.HVAC System Cooling</v>
+        <v>building_characteristics_report.hvac_system_cooling</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -8460,7 +8399,7 @@
       </c>
       <c r="D52" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Heating Setpoint</v>
+        <v>building_characteristics_report.heating_setpoint</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -8481,7 +8420,7 @@
       </c>
       <c r="D53" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Cooling Setpoint</v>
+        <v>building_characteristics_report.cooling_setpoint</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -8498,11 +8437,11 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>320</v>
+        <v>383</v>
       </c>
       <c r="D54" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Refrigerator</v>
+        <v>building_characteristics_report.ceiling_fan</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -8519,11 +8458,11 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D55" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Cooking Range</v>
+        <v>building_characteristics_report.refrigerator</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -8540,11 +8479,11 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D56" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Dishwasher</v>
+        <v>building_characteristics_report.cooking_range</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -8561,11 +8500,11 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D57" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Clothes Washer</v>
+        <v>building_characteristics_report.dishwasher</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -8582,11 +8521,11 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D58" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Clothes Dryer</v>
+        <v>building_characteristics_report.clothes_washer</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -8603,11 +8542,11 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>272</v>
+        <v>324</v>
       </c>
       <c r="D59" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Lighting</v>
+        <v>building_characteristics_report.clothes_dryer</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -8624,11 +8563,11 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>325</v>
+        <v>272</v>
       </c>
       <c r="D60" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Plug Loads</v>
+        <v>building_characteristics_report.lighting</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -8645,11 +8584,11 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D61" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Extra Refrigerator</v>
+        <v>building_characteristics_report.plug_loads</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -8666,11 +8605,11 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D62" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Freezer</v>
+        <v>building_characteristics_report.misc_extra_refrigerator</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -8687,11 +8626,11 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D63" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Gas Fireplace</v>
+        <v>building_characteristics_report.misc_freezer</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -8708,11 +8647,11 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D64" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Gas Grill</v>
+        <v>building_characteristics_report.misc_gas_fireplace</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -8729,11 +8668,11 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D65" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Gas Lighting</v>
+        <v>building_characteristics_report.misc_gas_grill</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -8750,11 +8689,11 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D66" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Hot Tub Spa</v>
+        <v>building_characteristics_report.misc_gas_lighting</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -8771,11 +8710,11 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D67" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>building_characteristics_report.Misc Pool</v>
+        <v>building_characteristics_report.misc_hot_tub_spa</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -8792,11 +8731,11 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D68" s="48" t="str">
-        <f t="shared" ref="D68:D72" si="1">"building_characteristics_report."&amp;A68</f>
-        <v>building_characteristics_report.Misc Well Pump</v>
+        <f t="shared" si="0"/>
+        <v>building_characteristics_report.misc_pool</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -8813,11 +8752,11 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D69" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>building_characteristics_report.Ducts</v>
+        <f t="shared" ref="D69:D73" si="1">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A69," ","_"))</f>
+        <v>building_characteristics_report.misc_well_pump</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -8834,11 +8773,11 @@
     </row>
     <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D70" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.Infiltration</v>
+        <v>building_characteristics_report.ducts</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>243</v>
@@ -8855,11 +8794,11 @@
     </row>
     <row r="71" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D71" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.Natural Ventilation</v>
+        <v>building_characteristics_report.infiltration</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>243</v>
@@ -8876,11 +8815,11 @@
     </row>
     <row r="72" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D72" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.Mechanical Ventilation</v>
+        <v>building_characteristics_report.natural_ventilation</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>243</v>
@@ -8895,35 +8834,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
-        <v>244</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="G73" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H73" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I73" s="14" t="b">
+    <row r="73" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="48" t="s">
+        <v>337</v>
+      </c>
+      <c r="D73" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.mechanical_ventilation</v>
+      </c>
+      <c r="F73" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
-        <v>245</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>341</v>
+        <v>244</v>
+      </c>
+      <c r="D74" s="14" t="str">
+        <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A74," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
+        <v>simulation_output_report.total_site_energy_m_btu</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -8937,13 +8878,14 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="D75" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D75" s="14" t="str">
+        <f t="shared" ref="D75:D95" si="2">"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A75," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
+        <v>simulation_output_report.total_site_electricity_k_wh</v>
+      </c>
+      <c r="F75" s="14" t="s">
         <v>342</v>
-      </c>
-      <c r="F75" s="14" t="s">
-        <v>360</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -8957,13 +8899,14 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="D76" s="14" t="s">
-        <v>343</v>
+        <v>246</v>
+      </c>
+      <c r="D76" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.total_site_natural_gas_therm</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -8977,13 +8920,14 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
-        <v>248</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>344</v>
+        <v>247</v>
+      </c>
+      <c r="D77" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.total_site_other_fuel_m_btu</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -8997,13 +8941,14 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
-        <v>249</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>345</v>
+        <v>248</v>
+      </c>
+      <c r="D78" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_heating_k_wh</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -9017,13 +8962,14 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
-        <v>250</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>346</v>
+        <v>249</v>
+      </c>
+      <c r="D79" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_cooling_k_wh</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -9037,13 +8983,14 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
-        <v>251</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>347</v>
+        <v>250</v>
+      </c>
+      <c r="D80" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_interior_lighting_k_wh</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -9057,13 +9004,14 @@
     </row>
     <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
-        <v>252</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>348</v>
+        <v>251</v>
+      </c>
+      <c r="D81" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_exterior_lighting_k_wh</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -9077,13 +9025,14 @@
     </row>
     <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>349</v>
+        <v>252</v>
+      </c>
+      <c r="D82" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_interior_equipment_k_wh</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -9097,13 +9046,14 @@
     </row>
     <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="49" t="s">
-        <v>254</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>350</v>
+        <v>253</v>
+      </c>
+      <c r="D83" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_fans_k_wh</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -9117,33 +9067,35 @@
     </row>
     <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="D84" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_pumps_k_wh</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="G84" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="D84" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="G84" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H84" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I84" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>352</v>
+      <c r="D85" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.electricity_water_systems_k_wh</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -9157,13 +9109,14 @@
     </row>
     <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>353</v>
+        <v>256</v>
+      </c>
+      <c r="D86" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.natural_gas_heating_therm</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -9177,13 +9130,14 @@
     </row>
     <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>354</v>
+        <v>257</v>
+      </c>
+      <c r="D87" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.natural_gas_interior_equipment_therm</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>
@@ -9197,13 +9151,14 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>355</v>
+        <v>258</v>
+      </c>
+      <c r="D88" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.natural_gas_water_systems_therm</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G88" s="14" t="b">
         <v>0</v>
@@ -9217,13 +9172,14 @@
     </row>
     <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>356</v>
+        <v>259</v>
+      </c>
+      <c r="D89" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.other_fuel_heating_m_btu</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G89" s="14" t="b">
         <v>0</v>
@@ -9237,13 +9193,14 @@
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>357</v>
+        <v>260</v>
+      </c>
+      <c r="D90" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.other_fuel_interior_equipment_m_btu</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G90" s="14" t="b">
         <v>0</v>
@@ -9257,13 +9214,14 @@
     </row>
     <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>370</v>
+        <v>261</v>
+      </c>
+      <c r="D91" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.other_fuel_water_systems_m_btu</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G91" s="14" t="b">
         <v>0</v>
@@ -9274,20 +9232,17 @@
       <c r="I91" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J91" s="49"/>
-      <c r="K91" s="49"/>
-      <c r="L91" s="49"/>
-      <c r="M91" s="49"/>
     </row>
     <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>372</v>
+        <v>351</v>
+      </c>
+      <c r="D92" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.hours_heating_setpoint_not_met</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G92" s="14" t="b">
         <v>0</v>
@@ -9304,14 +9259,15 @@
       <c r="M92" s="49"/>
     </row>
     <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="49" t="s">
-        <v>374</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>375</v>
+      <c r="A93" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="D93" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.hours_cooling_setpoint_not_met</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G93" s="14" t="b">
         <v>0</v>
@@ -9322,16 +9278,21 @@
       <c r="I93" s="14" t="b">
         <v>0</v>
       </c>
+      <c r="J93" s="49"/>
+      <c r="K93" s="49"/>
+      <c r="L93" s="49"/>
+      <c r="M93" s="49"/>
     </row>
     <row r="94" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="49" t="s">
-        <v>376</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>377</v>
+        <v>354</v>
+      </c>
+      <c r="D94" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.hvac_cooling_capacity_w</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G94" s="14" t="b">
         <v>0</v>
@@ -9343,14 +9304,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
-      <c r="B95" s="21"/>
-      <c r="D95" s="15"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
-      <c r="I95" s="15"/>
+    <row r="95" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="49" t="s">
+        <v>355</v>
+      </c>
+      <c r="D95" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>simulation_output_report.hvac_heating_capacity_w</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="G95" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
@@ -9622,12 +9595,10 @@
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
       <c r="B126" s="21"/>
-      <c r="C126" s="22"/>
       <c r="D126" s="15"/>
-      <c r="E126" s="22"/>
       <c r="F126" s="15"/>
       <c r="G126" s="15"/>
       <c r="H126" s="15"/>
@@ -9687,6 +9658,17 @@
       <c r="G131" s="15"/>
       <c r="H131" s="15"/>
       <c r="I131" s="15"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="15"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="22"/>
+      <c r="D132" s="15"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="15"/>
+      <c r="G132" s="15"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added weight (house count) column to results csv. Blank out upgrade costs for the existing building and any upgrades that weren't applied.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="396">
   <si>
     <t>type</t>
   </si>
@@ -1216,6 +1216,12 @@
   </si>
   <si>
     <t>Upgrade Cost</t>
+  </si>
+  <si>
+    <t>Number of Buildings Represented</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -5421,7 +5427,7 @@
         <v>66</v>
       </c>
       <c r="B9" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5429,7 +5435,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$8.4/hour</v>
+        <v>$1.68/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>201</v>
@@ -5797,7 +5803,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z54"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -6060,203 +6066,203 @@
       <c r="W5" s="45"/>
       <c r="X5" s="45"/>
     </row>
-    <row r="6" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="b">
+    <row r="6" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E6" s="10" t="str">
+        <f t="shared" ref="E6" si="0">LOWER(SUBSTITUTE(D6," ","_"))</f>
+        <v>number_of_buildings_represented</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="51">
+        <v>80000000</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+    </row>
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B7" s="39" t="s">
         <v>361</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C7" s="39" t="s">
         <v>362</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D7" s="39" t="s">
         <v>362</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E7" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="36"/>
-      <c r="Z6" s="36"/>
-    </row>
-    <row r="7" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45" t="s">
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="36"/>
+      <c r="Z7" s="36"/>
+    </row>
+    <row r="8" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45" t="s">
+      <c r="C8" s="45"/>
+      <c r="D8" s="45" t="s">
         <v>364</v>
       </c>
-      <c r="E7" s="45" t="str">
-        <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
+      <c r="E8" s="45" t="str">
+        <f>LOWER(SUBSTITUTE(D8," ","_"))</f>
         <v>always_run</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45" t="s">
+      <c r="F8" s="45"/>
+      <c r="G8" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45">
+      <c r="H8" s="45"/>
+      <c r="I8" s="45">
         <v>1</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45">
+      <c r="J8" s="45"/>
+      <c r="K8" s="45">
         <v>1</v>
       </c>
-      <c r="L7" s="45">
+      <c r="L8" s="45">
         <v>1</v>
       </c>
-      <c r="M7" s="45">
+      <c r="M8" s="45">
         <v>1</v>
       </c>
-      <c r="N7" s="45">
+      <c r="N8" s="45">
         <v>1</v>
       </c>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45" t="s">
+      <c r="O8" s="45"/>
+      <c r="P8" s="45" t="s">
         <v>365</v>
       </c>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45" t="s">
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-    </row>
-    <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="b">
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
+    </row>
+    <row r="9" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B9" s="39" t="s">
         <v>370</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C9" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D9" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-    </row>
-    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+    </row>
+    <row r="10" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D9" s="45" t="str">
-        <f>"Run " &amp; B8</f>
+      <c r="D10" s="45" t="str">
+        <f>"Run " &amp; B9</f>
         <v>Run R13 Wall Insulation Upgrade (If Uninsulated)</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E10" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G10" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I9" s="45">
+      <c r="I10" s="45">
         <v>1</v>
       </c>
-      <c r="K9" s="45">
-        <v>0</v>
-      </c>
-      <c r="L9" s="45">
+      <c r="K10" s="45">
+        <v>0</v>
+      </c>
+      <c r="L10" s="45">
         <v>1</v>
       </c>
-      <c r="M9" s="45">
+      <c r="M10" s="45">
         <v>1</v>
       </c>
-      <c r="N9" s="45">
+      <c r="N10" s="45">
         <v>1</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P10" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R9" s="45" t="s">
+      <c r="R10" s="45" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E10" s="10" t="str">
-        <f t="shared" ref="E10:E13" si="0">LOWER(SUBSTITUTE(D10," ","_"))</f>
-        <v>option_1</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -6265,11 +6271,11 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="E11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>option_1_apply_logic</v>
+        <f t="shared" ref="E11:E14" si="1">LOWER(SUBSTITUTE(D11," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
@@ -6277,7 +6283,7 @@
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -6304,19 +6310,19 @@
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="E12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>option_1_cost_1_value</v>
+        <f t="shared" si="1"/>
+        <v>option_1_apply_logic</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H12" s="10"/>
-      <c r="I12" s="51">
-        <v>2.21</v>
+      <c r="I12" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -6343,19 +6349,19 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>option_1_cost_1_multiplier</v>
+        <f t="shared" si="1"/>
+        <v>option_1_cost_1_value</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>386</v>
+      <c r="I13" s="51">
+        <v>2.21</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -6375,116 +6381,116 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="b">
+    <row r="14" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="E14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>option_1_cost_1_multiplier</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+    </row>
+    <row r="15" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B15" s="39" t="s">
         <v>367</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C15" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D15" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E15" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
-      <c r="X14" s="39"/>
-    </row>
-    <row r="15" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="45" t="s">
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="39"/>
+    </row>
+    <row r="16" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D15" s="45" t="str">
-        <f>"Run " &amp; B14</f>
+      <c r="D16" s="45" t="str">
+        <f>"Run " &amp; B15</f>
         <v>Run Triple-Pane Windows Upgrade (If Single-Pane)</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E16" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G16" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I15" s="45">
+      <c r="I16" s="45">
         <v>1</v>
       </c>
-      <c r="K15" s="45">
-        <v>0</v>
-      </c>
-      <c r="L15" s="45">
+      <c r="K16" s="45">
+        <v>0</v>
+      </c>
+      <c r="L16" s="45">
         <v>1</v>
       </c>
-      <c r="M15" s="45">
+      <c r="M16" s="45">
         <v>1</v>
       </c>
-      <c r="N15" s="45">
+      <c r="N16" s="45">
         <v>1</v>
       </c>
-      <c r="P15" s="45" t="s">
+      <c r="P16" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R15" s="45" t="s">
+      <c r="R16" s="45" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E16" s="10" t="str">
-        <f>LOWER(SUBSTITUTE(D16," ","_"))</f>
-        <v>option_1</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
     </row>
     <row r="17" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
@@ -6493,11 +6499,11 @@
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="E17" s="10" t="str">
-        <f t="shared" ref="E17:E19" si="1">LOWER(SUBSTITUTE(D17," ","_"))</f>
-        <v>option_1_apply_logic</v>
+        <f>LOWER(SUBSTITUTE(D17," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
@@ -6505,7 +6511,7 @@
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -6532,19 +6538,19 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="E18" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>option_1_cost_1_value</v>
+        <f t="shared" ref="E18:E20" si="2">LOWER(SUBSTITUTE(D18," ","_"))</f>
+        <v>option_1_apply_logic</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="51">
-        <v>39.54</v>
+      <c r="I18" s="10" t="s">
+        <v>368</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6571,19 +6577,19 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E19" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>option_1_cost_1_multiplier</v>
+        <f t="shared" si="2"/>
+        <v>option_1_cost_1_value</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
-        <v>387</v>
+      <c r="I19" s="51">
+        <v>39.54</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6603,116 +6609,116 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="b">
+    <row r="20" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>option_1_cost_1_multiplier</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+    </row>
+    <row r="21" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B21" s="39" t="s">
         <v>273</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C21" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D21" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E21" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39"/>
-      <c r="W20" s="39"/>
-      <c r="X20" s="39"/>
-    </row>
-    <row r="21" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="s">
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+    </row>
+    <row r="22" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D21" s="45" t="str">
-        <f>"Run " &amp; B20</f>
+      <c r="D22" s="45" t="str">
+        <f>"Run " &amp; B21</f>
         <v>Run LED Lighting Upgrade</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E22" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G22" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I21" s="45">
+      <c r="I22" s="45">
         <v>1</v>
       </c>
-      <c r="K21" s="45">
-        <v>0</v>
-      </c>
-      <c r="L21" s="45">
+      <c r="K22" s="45">
+        <v>0</v>
+      </c>
+      <c r="L22" s="45">
         <v>1</v>
       </c>
-      <c r="M21" s="45">
+      <c r="M22" s="45">
         <v>1</v>
       </c>
-      <c r="N21" s="45">
+      <c r="N22" s="45">
         <v>1</v>
       </c>
-      <c r="P21" s="45" t="s">
+      <c r="P22" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R21" s="45" t="s">
+      <c r="R22" s="45" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E22" s="10" t="str">
-        <f>LOWER(SUBSTITUTE(D22," ","_"))</f>
-        <v>option_1</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
     </row>
     <row r="23" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
@@ -6721,19 +6727,19 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>384</v>
+        <v>356</v>
       </c>
       <c r="E23" s="10" t="str">
-        <f t="shared" ref="E23:E24" si="2">LOWER(SUBSTITUTE(D23," ","_"))</f>
-        <v>option_1_cost_1_value</v>
+        <f>LOWER(SUBSTITUTE(D23," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H23" s="10"/>
-      <c r="I23" s="51">
-        <v>0.09</v>
+      <c r="I23" s="10" t="s">
+        <v>358</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -6760,19 +6766,19 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E24" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>option_1_cost_1_multiplier</v>
+        <f t="shared" ref="E24:E25" si="3">LOWER(SUBSTITUTE(D24," ","_"))</f>
+        <v>option_1_cost_1_value</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
-        <v>388</v>
+      <c r="I24" s="51">
+        <v>0.09</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -6792,116 +6798,116 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="b">
+    <row r="25" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="E25" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>option_1_cost_1_multiplier</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+    </row>
+    <row r="26" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B26" s="39" t="s">
         <v>373</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C26" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D26" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E26" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="39"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
-      <c r="V25" s="39"/>
-      <c r="W25" s="39"/>
-      <c r="X25" s="39"/>
-    </row>
-    <row r="26" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+    </row>
+    <row r="27" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D26" s="45" t="str">
-        <f>"Run " &amp; B25</f>
+      <c r="D27" s="45" t="str">
+        <f>"Run " &amp; B26</f>
         <v>Run Upgrade Package (Allow Individual Options)</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="E27" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G27" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I26" s="45">
+      <c r="I27" s="45">
         <v>1</v>
       </c>
-      <c r="K26" s="45">
-        <v>0</v>
-      </c>
-      <c r="L26" s="45">
+      <c r="K27" s="45">
+        <v>0</v>
+      </c>
+      <c r="L27" s="45">
         <v>1</v>
       </c>
-      <c r="M26" s="45">
+      <c r="M27" s="45">
         <v>1</v>
       </c>
-      <c r="N26" s="45">
+      <c r="N27" s="45">
         <v>1</v>
       </c>
-      <c r="P26" s="45" t="s">
+      <c r="P27" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R26" s="45" t="s">
+      <c r="R27" s="45" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E27" s="10" t="str">
-        <f t="shared" ref="E27:E37" si="3">LOWER(SUBSTITUTE(D27," ","_"))</f>
-        <v>option_1</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
     </row>
     <row r="28" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
@@ -6910,11 +6916,11 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="E28" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_1_apply_logic</v>
+        <f t="shared" ref="E28:E38" si="4">LOWER(SUBSTITUTE(D28," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
@@ -6922,7 +6928,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -6949,19 +6955,19 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="E29" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_1_cost_1_value</v>
+        <f t="shared" si="4"/>
+        <v>option_1_apply_logic</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H29" s="10"/>
-      <c r="I29" s="51">
-        <v>2.21</v>
+      <c r="I29" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -6988,19 +6994,19 @@
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E30" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_1_cost_1_multiplier</v>
+        <f t="shared" si="4"/>
+        <v>option_1_cost_1_value</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H30" s="10"/>
-      <c r="I30" s="10" t="s">
-        <v>386</v>
+      <c r="I30" s="51">
+        <v>2.21</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -7027,11 +7033,11 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>359</v>
+        <v>385</v>
       </c>
       <c r="E31" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_2</v>
+        <f t="shared" si="4"/>
+        <v>option_1_cost_1_multiplier</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="s">
@@ -7039,7 +7045,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>357</v>
+        <v>386</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7066,11 +7072,11 @@
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E32" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_2_apply_logic</v>
+        <f t="shared" si="4"/>
+        <v>option_2</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10" t="s">
@@ -7078,7 +7084,7 @@
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
@@ -7105,19 +7111,19 @@
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="E33" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_2_cost_1_value</v>
+        <f t="shared" si="4"/>
+        <v>option_2_apply_logic</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H33" s="10"/>
-      <c r="I33" s="51">
-        <v>39.54</v>
+      <c r="I33" s="10" t="s">
+        <v>368</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
@@ -7144,19 +7150,19 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E34" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_2_cost_1_multiplier</v>
+        <f t="shared" si="4"/>
+        <v>option_2_cost_1_value</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H34" s="10"/>
-      <c r="I34" s="10" t="s">
-        <v>387</v>
+      <c r="I34" s="51">
+        <v>39.54</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7183,11 +7189,11 @@
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>360</v>
+        <v>390</v>
       </c>
       <c r="E35" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_3</v>
+        <f t="shared" si="4"/>
+        <v>option_2_cost_1_multiplier</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
@@ -7195,7 +7201,7 @@
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10" t="s">
-        <v>358</v>
+        <v>387</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
@@ -7215,26 +7221,26 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
     </row>
-    <row r="36" spans="1:26" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="E36" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_3_cost_1_value</v>
+        <f t="shared" si="4"/>
+        <v>option_3</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H36" s="10"/>
-      <c r="I36" s="51">
-        <v>0.09</v>
+      <c r="I36" s="10" t="s">
+        <v>358</v>
       </c>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -7261,19 +7267,19 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E37" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>option_3_cost_1_multiplier</v>
+        <f t="shared" si="4"/>
+        <v>option_3_cost_1_value</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H37" s="10"/>
-      <c r="I37" s="10" t="s">
-        <v>388</v>
+      <c r="I37" s="51">
+        <v>0.09</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7293,116 +7299,116 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="b">
+    <row r="38" spans="1:26" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E38" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>option_3_cost_1_multiplier</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+    </row>
+    <row r="39" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B39" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C39" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D39" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E39" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="39"/>
-      <c r="R38" s="39"/>
-      <c r="S38" s="39"/>
-      <c r="T38" s="39"/>
-      <c r="U38" s="39"/>
-      <c r="V38" s="39"/>
-      <c r="W38" s="39"/>
-      <c r="X38" s="39"/>
-    </row>
-    <row r="39" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="45" t="s">
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="39"/>
+      <c r="Q39" s="39"/>
+      <c r="R39" s="39"/>
+      <c r="S39" s="39"/>
+      <c r="T39" s="39"/>
+      <c r="U39" s="39"/>
+      <c r="V39" s="39"/>
+      <c r="W39" s="39"/>
+      <c r="X39" s="39"/>
+    </row>
+    <row r="40" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D39" s="45" t="str">
-        <f>"Run " &amp; B38</f>
+      <c r="D40" s="45" t="str">
+        <f>"Run " &amp; B39</f>
         <v>Run Upgrade Package (All or None)</v>
       </c>
-      <c r="E39" s="45" t="s">
+      <c r="E40" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G39" s="45" t="s">
+      <c r="G40" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="I39" s="45">
+      <c r="I40" s="45">
         <v>1</v>
       </c>
-      <c r="K39" s="45">
-        <v>0</v>
-      </c>
-      <c r="L39" s="45">
+      <c r="K40" s="45">
+        <v>0</v>
+      </c>
+      <c r="L40" s="45">
         <v>1</v>
       </c>
-      <c r="M39" s="45">
+      <c r="M40" s="45">
         <v>1</v>
       </c>
-      <c r="N39" s="45">
+      <c r="N40" s="45">
         <v>1</v>
       </c>
-      <c r="P39" s="45" t="s">
+      <c r="P40" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="R39" s="45" t="s">
+      <c r="R40" s="45" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E40" s="10" t="str">
-        <f t="shared" ref="E40:E49" si="4">LOWER(SUBSTITUTE(D40," ","_"))</f>
-        <v>option_1</v>
-      </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
-      <c r="W40" s="10"/>
-      <c r="X40" s="10"/>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="15"/>
     </row>
     <row r="41" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
@@ -7411,19 +7417,19 @@
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
-        <v>384</v>
+        <v>356</v>
       </c>
       <c r="E41" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_1_cost_1_value</v>
+        <f t="shared" ref="E41:E50" si="5">LOWER(SUBSTITUTE(D41," ","_"))</f>
+        <v>option_1</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H41" s="10"/>
-      <c r="I41" s="51">
-        <v>2.21</v>
+      <c r="I41" s="10" t="s">
+        <v>371</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
@@ -7450,19 +7456,19 @@
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E42" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_1_cost_1_multiplier</v>
+        <f t="shared" si="5"/>
+        <v>option_1_cost_1_value</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H42" s="10"/>
-      <c r="I42" s="10" t="s">
-        <v>386</v>
+      <c r="I42" s="51">
+        <v>2.21</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -7489,11 +7495,11 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>359</v>
+        <v>385</v>
       </c>
       <c r="E43" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_2</v>
+        <f t="shared" si="5"/>
+        <v>option_1_cost_1_multiplier</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10" t="s">
@@ -7501,7 +7507,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>357</v>
+        <v>386</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7528,19 +7534,19 @@
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>389</v>
+        <v>359</v>
       </c>
       <c r="E44" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_2_cost_1_value</v>
+        <f t="shared" si="5"/>
+        <v>option_2</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H44" s="10"/>
-      <c r="I44" s="51">
-        <v>39.54</v>
+      <c r="I44" s="10" t="s">
+        <v>357</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -7567,19 +7573,19 @@
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E45" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_2_cost_1_multiplier</v>
+        <f t="shared" si="5"/>
+        <v>option_2_cost_1_value</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H45" s="10"/>
-      <c r="I45" s="10" t="s">
-        <v>387</v>
+      <c r="I45" s="51">
+        <v>39.54</v>
       </c>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
@@ -7606,11 +7612,11 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>360</v>
+        <v>390</v>
       </c>
       <c r="E46" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_3</v>
+        <f t="shared" si="5"/>
+        <v>option_2_cost_1_multiplier</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
@@ -7618,7 +7624,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>358</v>
+        <v>387</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7645,19 +7651,19 @@
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="E47" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_3_cost_1_value</v>
+        <f t="shared" si="5"/>
+        <v>option_3</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="H47" s="10"/>
-      <c r="I47" s="51">
-        <v>0.09</v>
+      <c r="I47" s="10" t="s">
+        <v>358</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
@@ -7684,19 +7690,19 @@
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E48" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>option_3_cost_1_multiplier</v>
+        <f t="shared" si="5"/>
+        <v>option_3_cost_1_value</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="H48" s="10"/>
-      <c r="I48" s="10" t="s">
-        <v>388</v>
+      <c r="I48" s="51">
+        <v>0.09</v>
       </c>
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
@@ -7723,11 +7729,11 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="E49" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>package_apply_logic</v>
+        <f t="shared" si="5"/>
+        <v>option_3_cost_1_multiplier</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
@@ -7735,7 +7741,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -7755,54 +7761,57 @@
       <c r="Y49" s="15"/>
       <c r="Z49" s="15"/>
     </row>
-    <row r="50" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="B50" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="D50" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="E50" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40"/>
-      <c r="N50" s="40"/>
-      <c r="O50" s="40"/>
-      <c r="P50" s="40"/>
-      <c r="Q50" s="40"/>
-      <c r="R50" s="40"/>
-      <c r="S50" s="40"/>
-      <c r="T50" s="40"/>
-      <c r="U50" s="40"/>
-      <c r="V50" s="40"/>
-      <c r="W50" s="40"/>
-      <c r="X50" s="40"/>
+    <row r="50" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="E50" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>package_apply_logic</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="10"/>
+      <c r="V50" s="10"/>
+      <c r="W50" s="10"/>
+      <c r="X50" s="10"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="15"/>
     </row>
     <row r="51" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="b">
         <v>1</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>236</v>
@@ -7832,13 +7841,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>238</v>
+        <v>340</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>237</v>
+        <v>341</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>237</v>
+        <v>341</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>236</v>
@@ -7863,11 +7872,47 @@
       <c r="W52" s="40"/>
       <c r="X52" s="40"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B53" s="50"/>
+    <row r="53" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B53" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="40"/>
+      <c r="K53" s="40"/>
+      <c r="L53" s="40"/>
+      <c r="M53" s="40"/>
+      <c r="N53" s="40"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
+      <c r="Q53" s="40"/>
+      <c r="R53" s="40"/>
+      <c r="S53" s="40"/>
+      <c r="T53" s="40"/>
+      <c r="U53" s="40"/>
+      <c r="V53" s="40"/>
+      <c r="W53" s="40"/>
+      <c r="X53" s="40"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B54" s="50"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B55" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -7881,7 +7926,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M133"/>
+  <dimension ref="A1:M134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8000,15 +8045,15 @@
       <c r="M3" s="32"/>
     </row>
     <row r="4" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>393</v>
+      <c r="A4" s="49" t="s">
+        <v>244</v>
       </c>
       <c r="D4" s="14" t="str">
         <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A4," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
-        <v>simulation_output_report.upgrade_cost</v>
+        <v>simulation_output_report.total_site_energy_m_btu</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>243</v>
+        <v>342</v>
       </c>
       <c r="G4" s="14" t="b">
         <v>0</v>
@@ -8022,11 +8067,11 @@
     </row>
     <row r="5" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D5" s="14" t="str">
-        <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A5," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
-        <v>simulation_output_report.total_site_energy_m_btu</v>
+        <f t="shared" ref="D5:D25" si="0">"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A5," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
+        <v>simulation_output_report.total_site_electricity_k_wh</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>342</v>
@@ -8043,11 +8088,11 @@
     </row>
     <row r="6" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D6" s="14" t="str">
-        <f t="shared" ref="D6:D26" si="0">"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A6," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
-        <v>simulation_output_report.total_site_electricity_k_wh</v>
+        <f t="shared" si="0"/>
+        <v>simulation_output_report.total_site_natural_gas_therm</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>342</v>
@@ -8064,11 +8109,11 @@
     </row>
     <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D7" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.total_site_natural_gas_therm</v>
+        <v>simulation_output_report.total_site_other_fuel_m_btu</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>342</v>
@@ -8085,11 +8130,11 @@
     </row>
     <row r="8" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D8" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.total_site_other_fuel_m_btu</v>
+        <v>simulation_output_report.electricity_heating_k_wh</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>342</v>
@@ -8106,11 +8151,11 @@
     </row>
     <row r="9" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D9" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_heating_k_wh</v>
+        <v>simulation_output_report.electricity_cooling_k_wh</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>342</v>
@@ -8127,11 +8172,11 @@
     </row>
     <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D10" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_cooling_k_wh</v>
+        <v>simulation_output_report.electricity_interior_lighting_k_wh</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>342</v>
@@ -8148,11 +8193,11 @@
     </row>
     <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D11" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_interior_lighting_k_wh</v>
+        <v>simulation_output_report.electricity_exterior_lighting_k_wh</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>342</v>
@@ -8169,11 +8214,11 @@
     </row>
     <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D12" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_exterior_lighting_k_wh</v>
+        <v>simulation_output_report.electricity_interior_equipment_k_wh</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>342</v>
@@ -8190,11 +8235,11 @@
     </row>
     <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D13" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_interior_equipment_k_wh</v>
+        <v>simulation_output_report.electricity_fans_k_wh</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>342</v>
@@ -8211,11 +8256,11 @@
     </row>
     <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_fans_k_wh</v>
+        <v>simulation_output_report.electricity_pumps_k_wh</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>342</v>
@@ -8232,11 +8277,11 @@
     </row>
     <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D15" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_pumps_k_wh</v>
+        <v>simulation_output_report.electricity_water_systems_k_wh</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>342</v>
@@ -8252,12 +8297,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
-        <v>255</v>
+      <c r="A16" s="14" t="s">
+        <v>256</v>
       </c>
       <c r="D16" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.electricity_water_systems_k_wh</v>
+        <v>simulation_output_report.natural_gas_heating_therm</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>342</v>
@@ -8274,11 +8319,11 @@
     </row>
     <row r="17" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.natural_gas_heating_therm</v>
+        <v>simulation_output_report.natural_gas_interior_equipment_therm</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>342</v>
@@ -8295,11 +8340,11 @@
     </row>
     <row r="18" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D18" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.natural_gas_interior_equipment_therm</v>
+        <v>simulation_output_report.natural_gas_water_systems_therm</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>342</v>
@@ -8316,11 +8361,11 @@
     </row>
     <row r="19" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D19" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.natural_gas_water_systems_therm</v>
+        <v>simulation_output_report.other_fuel_heating_m_btu</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>342</v>
@@ -8337,11 +8382,11 @@
     </row>
     <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D20" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.other_fuel_heating_m_btu</v>
+        <v>simulation_output_report.other_fuel_interior_equipment_m_btu</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>342</v>
@@ -8358,11 +8403,11 @@
     </row>
     <row r="21" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D21" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.other_fuel_interior_equipment_m_btu</v>
+        <v>simulation_output_report.other_fuel_water_systems_m_btu</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>342</v>
@@ -8379,11 +8424,11 @@
     </row>
     <row r="22" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>261</v>
+        <v>351</v>
       </c>
       <c r="D22" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.other_fuel_water_systems_m_btu</v>
+        <v>simulation_output_report.hours_heating_setpoint_not_met</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>342</v>
@@ -8397,14 +8442,18 @@
       <c r="I22" s="14" t="b">
         <v>0</v>
       </c>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
     </row>
     <row r="23" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D23" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.hours_heating_setpoint_not_met</v>
+        <v>simulation_output_report.hours_cooling_setpoint_not_met</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>342</v>
@@ -8424,12 +8473,12 @@
       <c r="M23" s="49"/>
     </row>
     <row r="24" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>352</v>
+      <c r="A24" s="49" t="s">
+        <v>354</v>
       </c>
       <c r="D24" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.hours_cooling_setpoint_not_met</v>
+        <v>simulation_output_report.hvac_cooling_capacity_w</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>342</v>
@@ -8443,18 +8492,14 @@
       <c r="I24" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
     </row>
     <row r="25" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D25" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>simulation_output_report.hvac_cooling_capacity_w</v>
+        <v>simulation_output_report.hvac_heating_capacity_w</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>342</v>
@@ -8470,63 +8515,56 @@
       </c>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
-        <v>355</v>
+      <c r="A26" s="14" t="s">
+        <v>393</v>
       </c>
       <c r="D26" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>simulation_output_report.hvac_heating_capacity_w</v>
+        <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A26," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
+        <v>simulation_output_report.upgrade_cost</v>
       </c>
       <c r="F26" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="G26" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="D27" s="14" t="str">
+        <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A27," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
+        <v>simulation_output_report.weight</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="G26" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
-        <v>279</v>
-      </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48" t="str">
-        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A27," ","_"))</f>
-        <v>building_characteristics_report.location_region</v>
-      </c>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="G27" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
+      <c r="G27" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
       <c r="D28" s="48" t="str">
-        <f t="shared" ref="D28:D91" si="1">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A28," ","_"))</f>
-        <v>building_characteristics_report.location_epw</v>
+        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A28," ","_"))</f>
+        <v>building_characteristics_report.location_region</v>
       </c>
       <c r="E28" s="48"/>
       <c r="F28" s="48" t="s">
@@ -8548,13 +8586,13 @@
     </row>
     <row r="29" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>building_characteristics_report.vintage</v>
+        <f t="shared" ref="D29:D92" si="1">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A29," ","_"))</f>
+        <v>building_characteristics_report.location_epw</v>
       </c>
       <c r="E29" s="48"/>
       <c r="F29" s="48" t="s">
@@ -8576,13 +8614,13 @@
     </row>
     <row r="30" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
       <c r="D30" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.heating_fuel</v>
+        <v>building_characteristics_report.vintage</v>
       </c>
       <c r="E30" s="48"/>
       <c r="F30" s="48" t="s">
@@ -8604,13 +8642,13 @@
     </row>
     <row r="31" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.usage_level</v>
+        <v>building_characteristics_report.heating_fuel</v>
       </c>
       <c r="E31" s="48"/>
       <c r="F31" s="48" t="s">
@@ -8632,13 +8670,13 @@
     </row>
     <row r="32" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_foundation_type</v>
+        <v>building_characteristics_report.usage_level</v>
       </c>
       <c r="E32" s="48"/>
       <c r="F32" s="48" t="s">
@@ -8660,13 +8698,13 @@
     </row>
     <row r="33" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
       <c r="D33" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_house_size</v>
+        <v>building_characteristics_report.geometry_foundation_type</v>
       </c>
       <c r="E33" s="48"/>
       <c r="F33" s="48" t="s">
@@ -8688,13 +8726,13 @@
     </row>
     <row r="34" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
       <c r="D34" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_stories</v>
+        <v>building_characteristics_report.geometry_house_size</v>
       </c>
       <c r="E34" s="48"/>
       <c r="F34" s="48" t="s">
@@ -8716,13 +8754,13 @@
     </row>
     <row r="35" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
       <c r="D35" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_garage</v>
+        <v>building_characteristics_report.geometry_stories</v>
       </c>
       <c r="E35" s="48"/>
       <c r="F35" s="48" t="s">
@@ -8744,13 +8782,13 @@
     </row>
     <row r="36" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
       <c r="D36" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.occupants</v>
+        <v>building_characteristics_report.geometry_garage</v>
       </c>
       <c r="E36" s="48"/>
       <c r="F36" s="48" t="s">
@@ -8772,13 +8810,13 @@
     </row>
     <row r="37" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>288</v>
+        <v>353</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
       <c r="D37" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.orientation</v>
+        <v>building_characteristics_report.occupants</v>
       </c>
       <c r="E37" s="48"/>
       <c r="F37" s="48" t="s">
@@ -8800,13 +8838,13 @@
     </row>
     <row r="38" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
       <c r="D38" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.eaves</v>
+        <v>building_characteristics_report.orientation</v>
       </c>
       <c r="E38" s="48"/>
       <c r="F38" s="48" t="s">
@@ -8828,13 +8866,13 @@
     </row>
     <row r="39" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
       <c r="D39" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.overhangs</v>
+        <v>building_characteristics_report.eaves</v>
       </c>
       <c r="E39" s="48"/>
       <c r="F39" s="48" t="s">
@@ -8856,12 +8894,15 @@
     </row>
     <row r="40" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>291</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
       <c r="D40" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.door_area</v>
-      </c>
+        <v>building_characteristics_report.overhangs</v>
+      </c>
+      <c r="E40" s="48"/>
       <c r="F40" s="48" t="s">
         <v>243</v>
       </c>
@@ -8874,14 +8915,18 @@
       <c r="I40" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
     </row>
     <row r="41" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D41" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.window_areas</v>
+        <v>building_characteristics_report.door_area</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>243</v>
@@ -8898,15 +8943,12 @@
     </row>
     <row r="42" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>293</v>
-      </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
+        <v>292</v>
+      </c>
       <c r="D42" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.neighbors</v>
-      </c>
-      <c r="E42" s="48"/>
+        <v>building_characteristics_report.window_areas</v>
+      </c>
       <c r="F42" s="48" t="s">
         <v>243</v>
       </c>
@@ -8919,20 +8961,16 @@
       <c r="I42" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
     </row>
     <row r="43" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="B43" s="48"/>
       <c r="C43" s="48"/>
       <c r="D43" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_unfinished_attic</v>
+        <v>building_characteristics_report.neighbors</v>
       </c>
       <c r="E43" s="48"/>
       <c r="F43" s="48" t="s">
@@ -8954,13 +8992,13 @@
     </row>
     <row r="44" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="B44" s="48"/>
       <c r="C44" s="48"/>
       <c r="D44" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_wall</v>
+        <v>building_characteristics_report.insulation_unfinished_attic</v>
       </c>
       <c r="E44" s="48"/>
       <c r="F44" s="48" t="s">
@@ -8982,13 +9020,13 @@
     </row>
     <row r="45" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>
       <c r="D45" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_slab</v>
+        <v>building_characteristics_report.insulation_wall</v>
       </c>
       <c r="E45" s="48"/>
       <c r="F45" s="48" t="s">
@@ -9010,12 +9048,15 @@
     </row>
     <row r="46" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>296</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
       <c r="D46" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_crawlspace</v>
-      </c>
+        <v>building_characteristics_report.insulation_slab</v>
+      </c>
+      <c r="E46" s="48"/>
       <c r="F46" s="48" t="s">
         <v>243</v>
       </c>
@@ -9028,14 +9069,18 @@
       <c r="I46" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
     </row>
     <row r="47" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D47" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_unfinished_basement</v>
+        <v>building_characteristics_report.insulation_crawlspace</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>243</v>
@@ -9052,11 +9097,11 @@
     </row>
     <row r="48" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D48" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_finished_basement</v>
+        <v>building_characteristics_report.insulation_unfinished_basement</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>243</v>
@@ -9073,11 +9118,11 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D49" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_interzonal_floor</v>
+        <v>building_characteristics_report.insulation_finished_basement</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>243</v>
@@ -9094,11 +9139,11 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D50" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.uninsulated_surfaces</v>
+        <v>building_characteristics_report.insulation_interzonal_floor</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>243</v>
@@ -9115,11 +9160,11 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D51" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.roof_sheathing</v>
+        <v>building_characteristics_report.uninsulated_surfaces</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -9136,11 +9181,11 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D52" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.wall_sheathing</v>
+        <v>building_characteristics_report.roof_sheathing</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -9157,11 +9202,11 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D53" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.floor_sheathing</v>
+        <v>building_characteristics_report.wall_sheathing</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -9178,11 +9223,11 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D54" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.exterior_finish</v>
+        <v>building_characteristics_report.floor_sheathing</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -9199,11 +9244,11 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D55" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.roof_material</v>
+        <v>building_characteristics_report.exterior_finish</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -9220,11 +9265,11 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D56" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.floor_covering</v>
+        <v>building_characteristics_report.roof_material</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -9241,11 +9286,11 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D57" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_floor</v>
+        <v>building_characteristics_report.floor_covering</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -9262,11 +9307,11 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D58" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_exterior_wall</v>
+        <v>building_characteristics_report.thermal_mass_floor</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -9283,11 +9328,11 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D59" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_partition_wall</v>
+        <v>building_characteristics_report.thermal_mass_exterior_wall</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -9304,11 +9349,11 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D60" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_ceiling</v>
+        <v>building_characteristics_report.thermal_mass_partition_wall</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -9325,11 +9370,11 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D61" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_furniture</v>
+        <v>building_characteristics_report.thermal_mass_ceiling</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -9346,11 +9391,11 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D62" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.doors</v>
+        <v>building_characteristics_report.thermal_mass_furniture</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -9367,11 +9412,11 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="D63" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.windows</v>
+        <v>building_characteristics_report.doors</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -9388,11 +9433,11 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>313</v>
+        <v>271</v>
       </c>
       <c r="D64" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.water_heater</v>
+        <v>building_characteristics_report.windows</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -9409,11 +9454,11 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D65" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hot_water_fixtures</v>
+        <v>building_characteristics_report.water_heater</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -9430,11 +9475,11 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="D66" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hot_water_distribution</v>
+        <v>building_characteristics_report.hot_water_fixtures</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -9451,11 +9496,11 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>315</v>
+        <v>349</v>
       </c>
       <c r="D67" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_is_combined</v>
+        <v>building_characteristics_report.hot_water_distribution</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -9472,11 +9517,11 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D68" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_combined</v>
+        <v>building_characteristics_report.hvac_system_is_combined</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -9493,11 +9538,11 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>377</v>
+        <v>316</v>
       </c>
       <c r="D69" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_electricity</v>
+        <v>building_characteristics_report.hvac_system_combined</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -9514,11 +9559,11 @@
     </row>
     <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D70" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_fuel_oil</v>
+        <v>building_characteristics_report.hvac_system_heating_electricity</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>243</v>
@@ -9535,11 +9580,11 @@
     </row>
     <row r="71" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D71" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_natural_gas</v>
+        <v>building_characteristics_report.hvac_system_heating_fuel_oil</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>243</v>
@@ -9556,11 +9601,11 @@
     </row>
     <row r="72" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D72" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_other_fuel</v>
+        <v>building_characteristics_report.hvac_system_heating_natural_gas</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>243</v>
@@ -9577,11 +9622,11 @@
     </row>
     <row r="73" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D73" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_propane</v>
+        <v>building_characteristics_report.hvac_system_heating_other_fuel</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>243</v>
@@ -9598,11 +9643,11 @@
     </row>
     <row r="74" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
-        <v>317</v>
+        <v>381</v>
       </c>
       <c r="D74" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_cooling</v>
+        <v>building_characteristics_report.hvac_system_heating_propane</v>
       </c>
       <c r="F74" s="48" t="s">
         <v>243</v>
@@ -9619,11 +9664,11 @@
     </row>
     <row r="75" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D75" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.heating_setpoint</v>
+        <v>building_characteristics_report.hvac_system_cooling</v>
       </c>
       <c r="F75" s="48" t="s">
         <v>243</v>
@@ -9640,11 +9685,11 @@
     </row>
     <row r="76" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D76" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.cooling_setpoint</v>
+        <v>building_characteristics_report.heating_setpoint</v>
       </c>
       <c r="F76" s="48" t="s">
         <v>243</v>
@@ -9661,11 +9706,11 @@
     </row>
     <row r="77" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
-        <v>383</v>
+        <v>319</v>
       </c>
       <c r="D77" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.ceiling_fan</v>
+        <v>building_characteristics_report.cooling_setpoint</v>
       </c>
       <c r="F77" s="48" t="s">
         <v>243</v>
@@ -9682,11 +9727,11 @@
     </row>
     <row r="78" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="48" t="s">
-        <v>320</v>
+        <v>383</v>
       </c>
       <c r="D78" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.refrigerator</v>
+        <v>building_characteristics_report.ceiling_fan</v>
       </c>
       <c r="F78" s="48" t="s">
         <v>243</v>
@@ -9703,11 +9748,11 @@
     </row>
     <row r="79" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D79" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.cooking_range</v>
+        <v>building_characteristics_report.refrigerator</v>
       </c>
       <c r="F79" s="48" t="s">
         <v>243</v>
@@ -9724,11 +9769,11 @@
     </row>
     <row r="80" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D80" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.dishwasher</v>
+        <v>building_characteristics_report.cooking_range</v>
       </c>
       <c r="F80" s="48" t="s">
         <v>243</v>
@@ -9745,11 +9790,11 @@
     </row>
     <row r="81" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D81" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.clothes_washer</v>
+        <v>building_characteristics_report.dishwasher</v>
       </c>
       <c r="F81" s="48" t="s">
         <v>243</v>
@@ -9766,11 +9811,11 @@
     </row>
     <row r="82" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D82" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.clothes_dryer</v>
+        <v>building_characteristics_report.clothes_washer</v>
       </c>
       <c r="F82" s="48" t="s">
         <v>243</v>
@@ -9787,11 +9832,11 @@
     </row>
     <row r="83" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="48" t="s">
-        <v>272</v>
+        <v>324</v>
       </c>
       <c r="D83" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.lighting</v>
+        <v>building_characteristics_report.clothes_dryer</v>
       </c>
       <c r="F83" s="48" t="s">
         <v>243</v>
@@ -9808,11 +9853,11 @@
     </row>
     <row r="84" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="48" t="s">
-        <v>325</v>
+        <v>272</v>
       </c>
       <c r="D84" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.plug_loads</v>
+        <v>building_characteristics_report.lighting</v>
       </c>
       <c r="F84" s="48" t="s">
         <v>243</v>
@@ -9829,11 +9874,11 @@
     </row>
     <row r="85" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D85" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_extra_refrigerator</v>
+        <v>building_characteristics_report.plug_loads</v>
       </c>
       <c r="F85" s="48" t="s">
         <v>243</v>
@@ -9850,11 +9895,11 @@
     </row>
     <row r="86" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D86" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_freezer</v>
+        <v>building_characteristics_report.misc_extra_refrigerator</v>
       </c>
       <c r="F86" s="48" t="s">
         <v>243</v>
@@ -9871,11 +9916,11 @@
     </row>
     <row r="87" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D87" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_gas_fireplace</v>
+        <v>building_characteristics_report.misc_freezer</v>
       </c>
       <c r="F87" s="48" t="s">
         <v>243</v>
@@ -9892,11 +9937,11 @@
     </row>
     <row r="88" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D88" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_gas_grill</v>
+        <v>building_characteristics_report.misc_gas_fireplace</v>
       </c>
       <c r="F88" s="48" t="s">
         <v>243</v>
@@ -9913,11 +9958,11 @@
     </row>
     <row r="89" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D89" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_gas_lighting</v>
+        <v>building_characteristics_report.misc_gas_grill</v>
       </c>
       <c r="F89" s="48" t="s">
         <v>243</v>
@@ -9934,11 +9979,11 @@
     </row>
     <row r="90" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D90" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_hot_tub_spa</v>
+        <v>building_characteristics_report.misc_gas_lighting</v>
       </c>
       <c r="F90" s="48" t="s">
         <v>243</v>
@@ -9955,11 +10000,11 @@
     </row>
     <row r="91" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D91" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_pool</v>
+        <v>building_characteristics_report.misc_hot_tub_spa</v>
       </c>
       <c r="F91" s="48" t="s">
         <v>243</v>
@@ -9976,11 +10021,11 @@
     </row>
     <row r="92" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D92" s="48" t="str">
-        <f t="shared" ref="D92:D96" si="2">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A92," ","_"))</f>
-        <v>building_characteristics_report.misc_well_pump</v>
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.misc_pool</v>
       </c>
       <c r="F92" s="48" t="s">
         <v>243</v>
@@ -9997,96 +10042,108 @@
     </row>
     <row r="93" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="D93" s="48" t="str">
+        <f t="shared" ref="D93:D97" si="2">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A93," ","_"))</f>
+        <v>building_characteristics_report.misc_well_pump</v>
+      </c>
+      <c r="F93" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G93" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="D93" s="48" t="str">
+      <c r="D94" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.ducts</v>
       </c>
-      <c r="F93" s="48" t="s">
+      <c r="F94" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G93" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H93" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I93" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="48" t="s">
+      <c r="G94" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="D94" s="48" t="str">
+      <c r="D95" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.infiltration</v>
       </c>
-      <c r="F94" s="48" t="s">
+      <c r="F95" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G94" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H94" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I94" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="48" t="s">
+      <c r="G95" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="D95" s="48" t="str">
+      <c r="D96" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.natural_ventilation</v>
       </c>
-      <c r="F95" s="48" t="s">
+      <c r="F96" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G95" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H95" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I95" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="48" t="s">
+      <c r="G96" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="D96" s="48" t="str">
+      <c r="D97" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.mechanical_ventilation</v>
       </c>
-      <c r="F96" s="48" t="s">
+      <c r="F97" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G96" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H96" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I96" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-      <c r="B97" s="21"/>
-      <c r="D97" s="15"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="15"/>
-      <c r="H97" s="15"/>
-      <c r="I97" s="15"/>
+      <c r="G97" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" s="48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
@@ -10358,12 +10415,10 @@
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="15"/>
       <c r="B128" s="21"/>
-      <c r="C128" s="22"/>
       <c r="D128" s="15"/>
-      <c r="E128" s="22"/>
       <c r="F128" s="15"/>
       <c r="G128" s="15"/>
       <c r="H128" s="15"/>
@@ -10423,6 +10478,17 @@
       <c r="G133" s="15"/>
       <c r="H133" s="15"/>
       <c r="I133" s="15"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="15"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="22"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="15"/>
+      <c r="H134" s="15"/>
+      <c r="I134" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add city, state, lat, and long to CSV. Removed "$" from upgrade cost value.
</commit_message>
<xml_diff>
--- a/projects/resstock_national.xlsx
+++ b/projects/resstock_national.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="400">
   <si>
     <t>type</t>
   </si>
@@ -1215,13 +1215,25 @@
     <t>Option 3 Cost 1 Multiplier</t>
   </si>
   <si>
-    <t>Upgrade Cost</t>
-  </si>
-  <si>
     <t>Number of Buildings Represented</t>
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Upgrade Cost USD</t>
+  </si>
+  <si>
+    <t>Location City</t>
+  </si>
+  <si>
+    <t>Location State</t>
+  </si>
+  <si>
+    <t>Location Latitude</t>
+  </si>
+  <si>
+    <t>Location Longitude</t>
   </si>
 </sst>
 </file>
@@ -6073,7 +6085,7 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E6" s="10" t="str">
         <f t="shared" ref="E6" si="0">LOWER(SUBSTITUTE(D6," ","_"))</f>
@@ -7926,7 +7938,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M134"/>
+  <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8516,14 +8528,14 @@
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D26" s="14" t="str">
         <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A26," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
-        <v>simulation_output_report.upgrade_cost</v>
+        <v>simulation_output_report.upgrade_cost_usd</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>243</v>
+        <v>342</v>
       </c>
       <c r="G26" s="14" t="b">
         <v>0</v>
@@ -8537,7 +8549,7 @@
     </row>
     <row r="27" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D27" s="14" t="str">
         <f>"simulation_output_report."&amp;SUBSTITUTE(SUBSTITUTE(LOWER(SUBSTITUTE(A27," ","_")), "kwh", "k_wh"), "mbtu", "m_btu")</f>
@@ -8591,7 +8603,7 @@
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="48" t="str">
-        <f t="shared" ref="D29:D92" si="1">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A29," ","_"))</f>
+        <f t="shared" ref="D29:D96" si="1">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A29," ","_"))</f>
         <v>building_characteristics_report.location_epw</v>
       </c>
       <c r="E29" s="48"/>
@@ -8614,13 +8626,13 @@
     </row>
     <row r="30" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>281</v>
+        <v>396</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
       <c r="D30" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>building_characteristics_report.vintage</v>
+        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A30," ","_"))</f>
+        <v>building_characteristics_report.location_city</v>
       </c>
       <c r="E30" s="48"/>
       <c r="F30" s="48" t="s">
@@ -8642,13 +8654,13 @@
     </row>
     <row r="31" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>282</v>
+        <v>397</v>
       </c>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>building_characteristics_report.heating_fuel</v>
+        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A31," ","_"))</f>
+        <v>building_characteristics_report.location_state</v>
       </c>
       <c r="E31" s="48"/>
       <c r="F31" s="48" t="s">
@@ -8670,17 +8682,17 @@
     </row>
     <row r="32" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>283</v>
+        <v>398</v>
       </c>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>building_characteristics_report.usage_level</v>
+        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A32," ","_"))</f>
+        <v>building_characteristics_report.location_latitude</v>
       </c>
       <c r="E32" s="48"/>
       <c r="F32" s="48" t="s">
-        <v>243</v>
+        <v>342</v>
       </c>
       <c r="G32" s="48" t="b">
         <v>0</v>
@@ -8698,17 +8710,17 @@
     </row>
     <row r="33" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>284</v>
+        <v>399</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
       <c r="D33" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_foundation_type</v>
+        <f>"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A33," ","_"))</f>
+        <v>building_characteristics_report.location_longitude</v>
       </c>
       <c r="E33" s="48"/>
       <c r="F33" s="48" t="s">
-        <v>243</v>
+        <v>342</v>
       </c>
       <c r="G33" s="48" t="b">
         <v>0</v>
@@ -8726,13 +8738,13 @@
     </row>
     <row r="34" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
       <c r="D34" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_house_size</v>
+        <v>building_characteristics_report.vintage</v>
       </c>
       <c r="E34" s="48"/>
       <c r="F34" s="48" t="s">
@@ -8754,13 +8766,13 @@
     </row>
     <row r="35" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
       <c r="D35" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_stories</v>
+        <v>building_characteristics_report.heating_fuel</v>
       </c>
       <c r="E35" s="48"/>
       <c r="F35" s="48" t="s">
@@ -8782,13 +8794,13 @@
     </row>
     <row r="36" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
       <c r="D36" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.geometry_garage</v>
+        <v>building_characteristics_report.usage_level</v>
       </c>
       <c r="E36" s="48"/>
       <c r="F36" s="48" t="s">
@@ -8810,13 +8822,13 @@
     </row>
     <row r="37" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>353</v>
+        <v>284</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
       <c r="D37" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.occupants</v>
+        <v>building_characteristics_report.geometry_foundation_type</v>
       </c>
       <c r="E37" s="48"/>
       <c r="F37" s="48" t="s">
@@ -8838,13 +8850,13 @@
     </row>
     <row r="38" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
       <c r="D38" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.orientation</v>
+        <v>building_characteristics_report.geometry_house_size</v>
       </c>
       <c r="E38" s="48"/>
       <c r="F38" s="48" t="s">
@@ -8866,13 +8878,13 @@
     </row>
     <row r="39" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
       <c r="D39" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.eaves</v>
+        <v>building_characteristics_report.geometry_stories</v>
       </c>
       <c r="E39" s="48"/>
       <c r="F39" s="48" t="s">
@@ -8894,13 +8906,13 @@
     </row>
     <row r="40" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="48"/>
       <c r="D40" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.overhangs</v>
+        <v>building_characteristics_report.geometry_garage</v>
       </c>
       <c r="E40" s="48"/>
       <c r="F40" s="48" t="s">
@@ -8922,12 +8934,15 @@
     </row>
     <row r="41" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>291</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.door_area</v>
-      </c>
+        <v>building_characteristics_report.occupants</v>
+      </c>
+      <c r="E41" s="48"/>
       <c r="F41" s="48" t="s">
         <v>243</v>
       </c>
@@ -8940,15 +8955,22 @@
       <c r="I41" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
     </row>
     <row r="42" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>292</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
       <c r="D42" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.window_areas</v>
-      </c>
+        <v>building_characteristics_report.orientation</v>
+      </c>
+      <c r="E42" s="48"/>
       <c r="F42" s="48" t="s">
         <v>243</v>
       </c>
@@ -8961,16 +8983,20 @@
       <c r="I42" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J42" s="48"/>
+      <c r="K42" s="48"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
     </row>
     <row r="43" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B43" s="48"/>
       <c r="C43" s="48"/>
       <c r="D43" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.neighbors</v>
+        <v>building_characteristics_report.eaves</v>
       </c>
       <c r="E43" s="48"/>
       <c r="F43" s="48" t="s">
@@ -8992,13 +9018,13 @@
     </row>
     <row r="44" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="B44" s="48"/>
       <c r="C44" s="48"/>
       <c r="D44" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_unfinished_attic</v>
+        <v>building_characteristics_report.overhangs</v>
       </c>
       <c r="E44" s="48"/>
       <c r="F44" s="48" t="s">
@@ -9020,15 +9046,12 @@
     </row>
     <row r="45" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>294</v>
-      </c>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
+        <v>291</v>
+      </c>
       <c r="D45" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_wall</v>
-      </c>
-      <c r="E45" s="48"/>
+        <v>building_characteristics_report.door_area</v>
+      </c>
       <c r="F45" s="48" t="s">
         <v>243</v>
       </c>
@@ -9041,22 +9064,15 @@
       <c r="I45" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
     </row>
     <row r="46" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>295</v>
-      </c>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
+        <v>292</v>
+      </c>
       <c r="D46" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_slab</v>
-      </c>
-      <c r="E46" s="48"/>
+        <v>building_characteristics_report.window_areas</v>
+      </c>
       <c r="F46" s="48" t="s">
         <v>243</v>
       </c>
@@ -9069,19 +9085,18 @@
       <c r="I46" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
     </row>
     <row r="47" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>296</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
       <c r="D47" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_crawlspace</v>
-      </c>
+        <v>building_characteristics_report.neighbors</v>
+      </c>
+      <c r="E47" s="48"/>
       <c r="F47" s="48" t="s">
         <v>243</v>
       </c>
@@ -9094,15 +9109,22 @@
       <c r="I47" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
     </row>
     <row r="48" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>297</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
       <c r="D48" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_unfinished_basement</v>
-      </c>
+        <v>building_characteristics_report.insulation_unfinished_attic</v>
+      </c>
+      <c r="E48" s="48"/>
       <c r="F48" s="48" t="s">
         <v>243</v>
       </c>
@@ -9115,15 +9137,22 @@
       <c r="I48" s="48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+    </row>
+    <row r="49" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>298</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
       <c r="D49" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_finished_basement</v>
-      </c>
+        <v>building_characteristics_report.insulation_wall</v>
+      </c>
+      <c r="E49" s="48"/>
       <c r="F49" s="48" t="s">
         <v>243</v>
       </c>
@@ -9136,15 +9165,22 @@
       <c r="I49" s="48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+    </row>
+    <row r="50" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>299</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="B50" s="48"/>
+      <c r="C50" s="48"/>
       <c r="D50" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.insulation_interzonal_floor</v>
-      </c>
+        <v>building_characteristics_report.insulation_slab</v>
+      </c>
+      <c r="E50" s="48"/>
       <c r="F50" s="48" t="s">
         <v>243</v>
       </c>
@@ -9157,14 +9193,18 @@
       <c r="I50" s="48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+    </row>
+    <row r="51" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D51" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.uninsulated_surfaces</v>
+        <v>building_characteristics_report.insulation_crawlspace</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>243</v>
@@ -9179,13 +9219,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D52" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.roof_sheathing</v>
+        <v>building_characteristics_report.insulation_unfinished_basement</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>243</v>
@@ -9200,13 +9240,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D53" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.wall_sheathing</v>
+        <v>building_characteristics_report.insulation_finished_basement</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>243</v>
@@ -9221,13 +9261,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D54" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.floor_sheathing</v>
+        <v>building_characteristics_report.insulation_interzonal_floor</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>243</v>
@@ -9242,13 +9282,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D55" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.exterior_finish</v>
+        <v>building_characteristics_report.uninsulated_surfaces</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>243</v>
@@ -9263,13 +9303,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D56" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.roof_material</v>
+        <v>building_characteristics_report.roof_sheathing</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>243</v>
@@ -9284,13 +9324,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D57" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.floor_covering</v>
+        <v>building_characteristics_report.wall_sheathing</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>243</v>
@@ -9305,13 +9345,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D58" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_floor</v>
+        <v>building_characteristics_report.floor_sheathing</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>243</v>
@@ -9326,13 +9366,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D59" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_exterior_wall</v>
+        <v>building_characteristics_report.exterior_finish</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>243</v>
@@ -9347,13 +9387,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D60" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_partition_wall</v>
+        <v>building_characteristics_report.roof_material</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>243</v>
@@ -9368,13 +9408,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D61" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_ceiling</v>
+        <v>building_characteristics_report.floor_covering</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>243</v>
@@ -9389,13 +9429,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D62" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.thermal_mass_furniture</v>
+        <v>building_characteristics_report.thermal_mass_floor</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>243</v>
@@ -9410,13 +9450,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D63" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.doors</v>
+        <v>building_characteristics_report.thermal_mass_exterior_wall</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>243</v>
@@ -9431,13 +9471,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="D64" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.windows</v>
+        <v>building_characteristics_report.thermal_mass_partition_wall</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>243</v>
@@ -9454,11 +9494,11 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D65" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.water_heater</v>
+        <v>building_characteristics_report.thermal_mass_ceiling</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>243</v>
@@ -9475,11 +9515,11 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D66" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hot_water_fixtures</v>
+        <v>building_characteristics_report.thermal_mass_furniture</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>243</v>
@@ -9496,11 +9536,11 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>349</v>
+        <v>312</v>
       </c>
       <c r="D67" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hot_water_distribution</v>
+        <v>building_characteristics_report.doors</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>243</v>
@@ -9517,11 +9557,11 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>315</v>
+        <v>271</v>
       </c>
       <c r="D68" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_is_combined</v>
+        <v>building_characteristics_report.windows</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>243</v>
@@ -9538,11 +9578,11 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D69" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_combined</v>
+        <v>building_characteristics_report.water_heater</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>243</v>
@@ -9559,11 +9599,11 @@
     </row>
     <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>377</v>
+        <v>314</v>
       </c>
       <c r="D70" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_electricity</v>
+        <v>building_characteristics_report.hot_water_fixtures</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>243</v>
@@ -9580,11 +9620,11 @@
     </row>
     <row r="71" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="D71" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_fuel_oil</v>
+        <v>building_characteristics_report.hot_water_distribution</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>243</v>
@@ -9601,11 +9641,11 @@
     </row>
     <row r="72" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>379</v>
+        <v>315</v>
       </c>
       <c r="D72" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_natural_gas</v>
+        <v>building_characteristics_report.hvac_system_is_combined</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>243</v>
@@ -9622,11 +9662,11 @@
     </row>
     <row r="73" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
-        <v>380</v>
+        <v>316</v>
       </c>
       <c r="D73" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_other_fuel</v>
+        <v>building_characteristics_report.hvac_system_combined</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>243</v>
@@ -9643,11 +9683,11 @@
     </row>
     <row r="74" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D74" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_heating_propane</v>
+        <v>building_characteristics_report.hvac_system_heating_electricity</v>
       </c>
       <c r="F74" s="48" t="s">
         <v>243</v>
@@ -9664,11 +9704,11 @@
     </row>
     <row r="75" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
-        <v>317</v>
+        <v>378</v>
       </c>
       <c r="D75" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.hvac_system_cooling</v>
+        <v>building_characteristics_report.hvac_system_heating_fuel_oil</v>
       </c>
       <c r="F75" s="48" t="s">
         <v>243</v>
@@ -9685,11 +9725,11 @@
     </row>
     <row r="76" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
-        <v>318</v>
+        <v>379</v>
       </c>
       <c r="D76" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.heating_setpoint</v>
+        <v>building_characteristics_report.hvac_system_heating_natural_gas</v>
       </c>
       <c r="F76" s="48" t="s">
         <v>243</v>
@@ -9706,11 +9746,11 @@
     </row>
     <row r="77" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
-        <v>319</v>
+        <v>380</v>
       </c>
       <c r="D77" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.cooling_setpoint</v>
+        <v>building_characteristics_report.hvac_system_heating_other_fuel</v>
       </c>
       <c r="F77" s="48" t="s">
         <v>243</v>
@@ -9727,11 +9767,11 @@
     </row>
     <row r="78" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="48" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D78" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.ceiling_fan</v>
+        <v>building_characteristics_report.hvac_system_heating_propane</v>
       </c>
       <c r="F78" s="48" t="s">
         <v>243</v>
@@ -9748,11 +9788,11 @@
     </row>
     <row r="79" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D79" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.refrigerator</v>
+        <v>building_characteristics_report.hvac_system_cooling</v>
       </c>
       <c r="F79" s="48" t="s">
         <v>243</v>
@@ -9769,11 +9809,11 @@
     </row>
     <row r="80" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D80" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.cooking_range</v>
+        <v>building_characteristics_report.heating_setpoint</v>
       </c>
       <c r="F80" s="48" t="s">
         <v>243</v>
@@ -9790,11 +9830,11 @@
     </row>
     <row r="81" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D81" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.dishwasher</v>
+        <v>building_characteristics_report.cooling_setpoint</v>
       </c>
       <c r="F81" s="48" t="s">
         <v>243</v>
@@ -9811,11 +9851,11 @@
     </row>
     <row r="82" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="48" t="s">
-        <v>323</v>
+        <v>383</v>
       </c>
       <c r="D82" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.clothes_washer</v>
+        <v>building_characteristics_report.ceiling_fan</v>
       </c>
       <c r="F82" s="48" t="s">
         <v>243</v>
@@ -9832,11 +9872,11 @@
     </row>
     <row r="83" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="48" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D83" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.clothes_dryer</v>
+        <v>building_characteristics_report.refrigerator</v>
       </c>
       <c r="F83" s="48" t="s">
         <v>243</v>
@@ -9853,11 +9893,11 @@
     </row>
     <row r="84" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="48" t="s">
-        <v>272</v>
+        <v>321</v>
       </c>
       <c r="D84" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.lighting</v>
+        <v>building_characteristics_report.cooking_range</v>
       </c>
       <c r="F84" s="48" t="s">
         <v>243</v>
@@ -9874,11 +9914,11 @@
     </row>
     <row r="85" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D85" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.plug_loads</v>
+        <v>building_characteristics_report.dishwasher</v>
       </c>
       <c r="F85" s="48" t="s">
         <v>243</v>
@@ -9895,11 +9935,11 @@
     </row>
     <row r="86" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="48" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D86" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_extra_refrigerator</v>
+        <v>building_characteristics_report.clothes_washer</v>
       </c>
       <c r="F86" s="48" t="s">
         <v>243</v>
@@ -9916,11 +9956,11 @@
     </row>
     <row r="87" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="48" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D87" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_freezer</v>
+        <v>building_characteristics_report.clothes_dryer</v>
       </c>
       <c r="F87" s="48" t="s">
         <v>243</v>
@@ -9937,11 +9977,11 @@
     </row>
     <row r="88" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="48" t="s">
-        <v>328</v>
+        <v>272</v>
       </c>
       <c r="D88" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_gas_fireplace</v>
+        <v>building_characteristics_report.lighting</v>
       </c>
       <c r="F88" s="48" t="s">
         <v>243</v>
@@ -9958,11 +9998,11 @@
     </row>
     <row r="89" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="48" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D89" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_gas_grill</v>
+        <v>building_characteristics_report.plug_loads</v>
       </c>
       <c r="F89" s="48" t="s">
         <v>243</v>
@@ -9979,11 +10019,11 @@
     </row>
     <row r="90" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="48" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D90" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_gas_lighting</v>
+        <v>building_characteristics_report.misc_extra_refrigerator</v>
       </c>
       <c r="F90" s="48" t="s">
         <v>243</v>
@@ -10000,11 +10040,11 @@
     </row>
     <row r="91" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="48" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D91" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_hot_tub_spa</v>
+        <v>building_characteristics_report.misc_freezer</v>
       </c>
       <c r="F91" s="48" t="s">
         <v>243</v>
@@ -10021,11 +10061,11 @@
     </row>
     <row r="92" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="48" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D92" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>building_characteristics_report.misc_pool</v>
+        <v>building_characteristics_report.misc_gas_fireplace</v>
       </c>
       <c r="F92" s="48" t="s">
         <v>243</v>
@@ -10042,11 +10082,11 @@
     </row>
     <row r="93" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="48" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D93" s="48" t="str">
-        <f t="shared" ref="D93:D97" si="2">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A93," ","_"))</f>
-        <v>building_characteristics_report.misc_well_pump</v>
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.misc_gas_grill</v>
       </c>
       <c r="F93" s="48" t="s">
         <v>243</v>
@@ -10063,123 +10103,171 @@
     </row>
     <row r="94" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="48" t="s">
+        <v>330</v>
+      </c>
+      <c r="D94" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.misc_gas_lighting</v>
+      </c>
+      <c r="F94" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G94" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="D95" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.misc_hot_tub_spa</v>
+      </c>
+      <c r="F95" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G95" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="48" t="s">
+        <v>332</v>
+      </c>
+      <c r="D96" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>building_characteristics_report.misc_pool</v>
+      </c>
+      <c r="F96" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G96" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="D97" s="48" t="str">
+        <f t="shared" ref="D97:D101" si="2">"building_characteristics_report."&amp;LOWER(SUBSTITUTE(A97," ","_"))</f>
+        <v>building_characteristics_report.misc_well_pump</v>
+      </c>
+      <c r="F97" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G97" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="D94" s="48" t="str">
+      <c r="D98" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.ducts</v>
       </c>
-      <c r="F94" s="48" t="s">
+      <c r="F98" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G94" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H94" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I94" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="48" t="s">
+      <c r="G98" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="D95" s="48" t="str">
+      <c r="D99" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.infiltration</v>
       </c>
-      <c r="F95" s="48" t="s">
+      <c r="F99" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G95" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H95" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I95" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="48" t="s">
+      <c r="G99" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="D96" s="48" t="str">
+      <c r="D100" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.natural_ventilation</v>
       </c>
-      <c r="F96" s="48" t="s">
+      <c r="F100" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G96" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H96" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I96" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="48" t="s">
+      <c r="G100" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" s="48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="D97" s="48" t="str">
+      <c r="D101" s="48" t="str">
         <f t="shared" si="2"/>
         <v>building_characteristics_report.mechanical_ventilation</v>
       </c>
-      <c r="F97" s="48" t="s">
+      <c r="F101" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="G97" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H97" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I97" s="48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-      <c r="B98" s="21"/>
-      <c r="D98" s="15"/>
-      <c r="F98" s="15"/>
-      <c r="G98" s="15"/>
-      <c r="H98" s="15"/>
-      <c r="I98" s="15"/>
-    </row>
-    <row r="99" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="15"/>
-      <c r="B99" s="21"/>
-      <c r="D99" s="15"/>
-      <c r="F99" s="15"/>
-      <c r="G99" s="15"/>
-      <c r="H99" s="15"/>
-      <c r="I99" s="15"/>
-    </row>
-    <row r="100" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="15"/>
-      <c r="B100" s="21"/>
-      <c r="D100" s="15"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="15"/>
-      <c r="H100" s="15"/>
-      <c r="I100" s="15"/>
-    </row>
-    <row r="101" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="15"/>
-      <c r="B101" s="21"/>
-      <c r="D101" s="15"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="15"/>
-      <c r="H101" s="15"/>
-      <c r="I101" s="15"/>
+      <c r="G101" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" s="48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
@@ -10424,45 +10512,37 @@
       <c r="H128" s="15"/>
       <c r="I128" s="15"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="15"/>
       <c r="B129" s="21"/>
-      <c r="C129" s="22"/>
       <c r="D129" s="15"/>
-      <c r="E129" s="22"/>
       <c r="F129" s="15"/>
       <c r="G129" s="15"/>
       <c r="H129" s="15"/>
       <c r="I129" s="15"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="15"/>
       <c r="B130" s="21"/>
-      <c r="C130" s="22"/>
       <c r="D130" s="15"/>
-      <c r="E130" s="22"/>
       <c r="F130" s="15"/>
       <c r="G130" s="15"/>
       <c r="H130" s="15"/>
       <c r="I130" s="15"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="15"/>
       <c r="B131" s="21"/>
-      <c r="C131" s="22"/>
       <c r="D131" s="15"/>
-      <c r="E131" s="22"/>
       <c r="F131" s="15"/>
       <c r="G131" s="15"/>
       <c r="H131" s="15"/>
       <c r="I131" s="15"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="15"/>
       <c r="B132" s="21"/>
-      <c r="C132" s="22"/>
       <c r="D132" s="15"/>
-      <c r="E132" s="22"/>
       <c r="F132" s="15"/>
       <c r="G132" s="15"/>
       <c r="H132" s="15"/>
@@ -10489,6 +10569,50 @@
       <c r="G134" s="15"/>
       <c r="H134" s="15"/>
       <c r="I134" s="15"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="15"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="22"/>
+      <c r="D135" s="15"/>
+      <c r="E135" s="22"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="15"/>
+      <c r="H135" s="15"/>
+      <c r="I135" s="15"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="15"/>
+      <c r="B136" s="21"/>
+      <c r="C136" s="22"/>
+      <c r="D136" s="15"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="15"/>
+      <c r="H136" s="15"/>
+      <c r="I136" s="15"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="15"/>
+      <c r="B137" s="21"/>
+      <c r="C137" s="22"/>
+      <c r="D137" s="15"/>
+      <c r="E137" s="22"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="15"/>
+      <c r="H137" s="15"/>
+      <c r="I137" s="15"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="15"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="22"/>
+      <c r="D138" s="15"/>
+      <c r="E138" s="22"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="15"/>
+      <c r="H138" s="15"/>
+      <c r="I138" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>